<commit_message>
Update Excel data - 2024-11-22 04:11:09
</commit_message>
<xml_diff>
--- a/crypto_live_data.xlsx
+++ b/crypto_live_data.xlsx
@@ -479,16 +479,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>98206</v>
+        <v>98936</v>
       </c>
       <c r="D2" t="n">
-        <v>1937942266754</v>
+        <v>1957410186256</v>
       </c>
       <c r="E2" t="n">
-        <v>111173545973</v>
+        <v>115913150141</v>
       </c>
       <c r="F2" t="n">
-        <v>5.04191</v>
+        <v>2.57984</v>
       </c>
     </row>
     <row r="3">
@@ -503,16 +503,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3172.09</v>
+        <v>3371.17</v>
       </c>
       <c r="D3" t="n">
-        <v>379068348709</v>
+        <v>406015687428</v>
       </c>
       <c r="E3" t="n">
-        <v>38975748260</v>
+        <v>57864085710</v>
       </c>
       <c r="F3" t="n">
-        <v>2.42196</v>
+        <v>8.711589999999999</v>
       </c>
     </row>
     <row r="4">
@@ -527,16 +527,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.001</v>
+        <v>1.002</v>
       </c>
       <c r="D4" t="n">
-        <v>130187884714</v>
+        <v>130920758489</v>
       </c>
       <c r="E4" t="n">
-        <v>134169107107</v>
+        <v>180658001561</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.00333</v>
+        <v>-0.33176</v>
       </c>
     </row>
     <row r="5">
@@ -551,16 +551,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>241.63</v>
+        <v>262.94</v>
       </c>
       <c r="D5" t="n">
-        <v>114196457382</v>
+        <v>124821488522</v>
       </c>
       <c r="E5" t="n">
-        <v>10131983343</v>
+        <v>15497913447</v>
       </c>
       <c r="F5" t="n">
-        <v>1.86215</v>
+        <v>10.74741</v>
       </c>
     </row>
     <row r="6">
@@ -575,16 +575,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>611.37</v>
+        <v>636.66</v>
       </c>
       <c r="D6" t="n">
-        <v>88935613146</v>
+        <v>92924369009</v>
       </c>
       <c r="E6" t="n">
-        <v>1890020749</v>
+        <v>2560789290</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.28023</v>
+        <v>5.02412</v>
       </c>
     </row>
     <row r="7">
@@ -599,16 +599,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.12</v>
+        <v>1.38</v>
       </c>
       <c r="D7" t="n">
-        <v>63260205482</v>
+        <v>78666166648</v>
       </c>
       <c r="E7" t="n">
-        <v>7225031390</v>
+        <v>17004059380</v>
       </c>
       <c r="F7" t="n">
-        <v>-1.09162</v>
+        <v>25.01952</v>
       </c>
     </row>
     <row r="8">
@@ -623,16 +623,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.384384</v>
+        <v>0.393894</v>
       </c>
       <c r="D8" t="n">
-        <v>56230024031</v>
+        <v>57853509205</v>
       </c>
       <c r="E8" t="n">
-        <v>10067224828</v>
+        <v>10366188434</v>
       </c>
       <c r="F8" t="n">
-        <v>-1.1252</v>
+        <v>3.63818</v>
       </c>
     </row>
     <row r="9">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1.001</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>37680036688</v>
+        <v>38253314257</v>
       </c>
       <c r="E9" t="n">
-        <v>9235189037</v>
+        <v>17378138495</v>
       </c>
       <c r="F9" t="n">
-        <v>0.05294</v>
+        <v>-0.29745</v>
       </c>
     </row>
     <row r="10">
@@ -671,16 +671,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3177.87</v>
+        <v>3367.64</v>
       </c>
       <c r="D10" t="n">
-        <v>30878384496</v>
+        <v>32985342102</v>
       </c>
       <c r="E10" t="n">
-        <v>135551179</v>
+        <v>149669851</v>
       </c>
       <c r="F10" t="n">
-        <v>2.53049</v>
+        <v>8.403560000000001</v>
       </c>
     </row>
     <row r="11">
@@ -695,16 +695,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.790636</v>
+        <v>0.869827</v>
       </c>
       <c r="D11" t="n">
-        <v>28151756772</v>
+        <v>31086812023</v>
       </c>
       <c r="E11" t="n">
-        <v>2877763516</v>
+        <v>3350520127</v>
       </c>
       <c r="F11" t="n">
-        <v>-4.51973</v>
+        <v>11.21959</v>
       </c>
     </row>
     <row r="12">
@@ -719,40 +719,40 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.199577</v>
+        <v>0.200809</v>
       </c>
       <c r="D12" t="n">
-        <v>17171133491</v>
+        <v>17337544762</v>
       </c>
       <c r="E12" t="n">
-        <v>1038286070</v>
+        <v>1063110796</v>
       </c>
       <c r="F12" t="n">
-        <v>0.8565199999999999</v>
+        <v>2.15375</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Avalanche</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>wbtc</t>
+          <t>avax</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>97717</v>
+        <v>36.29</v>
       </c>
       <c r="D13" t="n">
-        <v>14307557368</v>
+        <v>14842978811</v>
       </c>
       <c r="E13" t="n">
-        <v>705951753</v>
+        <v>1056089658</v>
       </c>
       <c r="F13" t="n">
-        <v>4.76264</v>
+        <v>8.61652</v>
       </c>
     </row>
     <row r="14">
@@ -767,136 +767,136 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.409e-05</v>
+        <v>2.499e-05</v>
       </c>
       <c r="D14" t="n">
-        <v>14147040507</v>
+        <v>14710554787</v>
       </c>
       <c r="E14" t="n">
-        <v>1291546638</v>
+        <v>1616603700</v>
       </c>
       <c r="F14" t="n">
-        <v>-1.07413</v>
+        <v>5.48248</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Avalanche</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>avax</t>
+          <t>wbtc</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>34.32</v>
+        <v>98586</v>
       </c>
       <c r="D15" t="n">
-        <v>13940439777</v>
+        <v>14398896989</v>
       </c>
       <c r="E15" t="n">
-        <v>819099732</v>
+        <v>921826657</v>
       </c>
       <c r="F15" t="n">
-        <v>-1.54943</v>
+        <v>2.38183</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Toncoin</t>
+          <t>Wrapped stETH</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ton</t>
+          <t>wsteth</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5.47</v>
+        <v>3988.96</v>
       </c>
       <c r="D16" t="n">
-        <v>13844221595</v>
+        <v>14386360829</v>
       </c>
       <c r="E16" t="n">
-        <v>627042423</v>
+        <v>167163549</v>
       </c>
       <c r="F16" t="n">
-        <v>0.98315</v>
+        <v>8.905950000000001</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Wrapped stETH</t>
+          <t>Toncoin</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>wsteth</t>
+          <t>ton</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>3732.67</v>
+        <v>5.55</v>
       </c>
       <c r="D17" t="n">
-        <v>13494574676</v>
+        <v>14144705757</v>
       </c>
       <c r="E17" t="n">
-        <v>101564641</v>
+        <v>621432219</v>
       </c>
       <c r="F17" t="n">
-        <v>1.56171</v>
+        <v>4.44313</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>Sui</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>bch</t>
+          <t>sui</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>524.13</v>
+        <v>3.6</v>
       </c>
       <c r="D18" t="n">
-        <v>10306140945</v>
+        <v>10231629493</v>
       </c>
       <c r="E18" t="n">
-        <v>1890154858</v>
+        <v>2287578574</v>
       </c>
       <c r="F18" t="n">
-        <v>18.47482</v>
+        <v>2.74334</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Sui</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>sui</t>
+          <t>bch</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3.51</v>
+        <v>494.5</v>
       </c>
       <c r="D19" t="n">
-        <v>9896089381</v>
+        <v>9798830623</v>
       </c>
       <c r="E19" t="n">
-        <v>2126206238</v>
+        <v>2350395615</v>
       </c>
       <c r="F19" t="n">
-        <v>-3.78567</v>
+        <v>7.71998</v>
       </c>
     </row>
     <row r="20">
@@ -911,16 +911,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3160.71</v>
+        <v>3373.33</v>
       </c>
       <c r="D20" t="n">
-        <v>9195712021</v>
+        <v>9708765975</v>
       </c>
       <c r="E20" t="n">
-        <v>1770808471</v>
+        <v>519332627</v>
       </c>
       <c r="F20" t="n">
-        <v>1.92404</v>
+        <v>8.80829</v>
       </c>
     </row>
     <row r="21">
@@ -935,160 +935,160 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>14.69</v>
+        <v>15.12</v>
       </c>
       <c r="D21" t="n">
-        <v>9157158419</v>
+        <v>9500220377</v>
       </c>
       <c r="E21" t="n">
-        <v>1073188284</v>
+        <v>1223424068</v>
       </c>
       <c r="F21" t="n">
-        <v>0.08366</v>
+        <v>6.34317</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>dot</t>
+          <t>pepe</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>5.75</v>
+        <v>2.142e-05</v>
       </c>
       <c r="D22" t="n">
-        <v>8245861199</v>
+        <v>9014421360</v>
       </c>
       <c r="E22" t="n">
-        <v>671714275</v>
+        <v>7032492661</v>
       </c>
       <c r="F22" t="n">
-        <v>-4.55732</v>
+        <v>13.29684</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>LEO Token</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>leo</t>
+          <t>dot</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>8.83</v>
+        <v>6.17</v>
       </c>
       <c r="D23" t="n">
-        <v>8186360457</v>
+        <v>8881549580</v>
       </c>
       <c r="E23" t="n">
-        <v>3913167</v>
+        <v>814547946</v>
       </c>
       <c r="F23" t="n">
-        <v>4.69699</v>
+        <v>9.85849</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>Stellar</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>pepe</t>
+          <t>xlm</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1.943e-05</v>
+        <v>0.283117</v>
       </c>
       <c r="D24" t="n">
-        <v>8093531301</v>
+        <v>8501860012</v>
       </c>
       <c r="E24" t="n">
-        <v>4850054190</v>
+        <v>2311728073</v>
       </c>
       <c r="F24" t="n">
-        <v>-2.88375</v>
+        <v>17.79302</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Stellar</t>
+          <t>LEO Token</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>xlm</t>
+          <t>leo</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.239688</v>
+        <v>8.76</v>
       </c>
       <c r="D25" t="n">
-        <v>7121541826</v>
+        <v>8078033416</v>
       </c>
       <c r="E25" t="n">
-        <v>1569913276</v>
+        <v>3517774</v>
       </c>
       <c r="F25" t="n">
-        <v>-4.24358</v>
+        <v>2.67332</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Litecoin</t>
+          <t>NEAR Protocol</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ltc</t>
+          <t>near</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>90.29000000000001</v>
+        <v>5.78</v>
       </c>
       <c r="D26" t="n">
-        <v>6755149389</v>
+        <v>7035895518</v>
       </c>
       <c r="E26" t="n">
-        <v>1332786393</v>
+        <v>968924810</v>
       </c>
       <c r="F26" t="n">
-        <v>4.8345</v>
+        <v>5.61817</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>NEAR Protocol</t>
+          <t>Litecoin</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>near</t>
+          <t>ltc</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>5.5</v>
+        <v>90.19</v>
       </c>
       <c r="D27" t="n">
-        <v>6655386617</v>
+        <v>6784076065</v>
       </c>
       <c r="E27" t="n">
-        <v>680101326</v>
+        <v>1460843275</v>
       </c>
       <c r="F27" t="n">
-        <v>-3.89567</v>
+        <v>6.54217</v>
       </c>
     </row>
     <row r="28">
@@ -1103,16 +1103,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>11.68</v>
+        <v>12.1</v>
       </c>
       <c r="D28" t="n">
-        <v>6198704697</v>
+        <v>6453451196</v>
       </c>
       <c r="E28" t="n">
-        <v>908310604</v>
+        <v>895334881</v>
       </c>
       <c r="F28" t="n">
-        <v>-8.379709999999999</v>
+        <v>5.04982</v>
       </c>
     </row>
     <row r="29">
@@ -1127,16 +1127,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3345.98</v>
+        <v>3544.81</v>
       </c>
       <c r="D29" t="n">
-        <v>5683987943</v>
+        <v>6101083612</v>
       </c>
       <c r="E29" t="n">
-        <v>111784419</v>
+        <v>96814193</v>
       </c>
       <c r="F29" t="n">
-        <v>2.5439</v>
+        <v>9.20321</v>
       </c>
     </row>
     <row r="30">
@@ -1151,64 +1151,64 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>8.890000000000001</v>
+        <v>9.35</v>
       </c>
       <c r="D30" t="n">
-        <v>5297583699</v>
+        <v>5609709607</v>
       </c>
       <c r="E30" t="n">
-        <v>440780676</v>
+        <v>847563217</v>
       </c>
       <c r="F30" t="n">
-        <v>-1.33817</v>
+        <v>7.90214</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>USDS</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>usds</t>
+          <t>cro</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1.004</v>
+        <v>0.196843</v>
       </c>
       <c r="D31" t="n">
-        <v>5255519354</v>
+        <v>5336019451</v>
       </c>
       <c r="E31" t="n">
-        <v>8355016</v>
+        <v>115416917</v>
       </c>
       <c r="F31" t="n">
-        <v>0.36985</v>
+        <v>10.11105</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>USDS</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>cro</t>
+          <t>usds</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.179144</v>
+        <v>1.008</v>
       </c>
       <c r="D32" t="n">
-        <v>4820562091</v>
+        <v>5286602021</v>
       </c>
       <c r="E32" t="n">
-        <v>81212018</v>
+        <v>16038564</v>
       </c>
       <c r="F32" t="n">
-        <v>-1.91228</v>
+        <v>0.24725</v>
       </c>
     </row>
     <row r="33">
@@ -1223,16 +1223,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.121671</v>
+        <v>0.129052</v>
       </c>
       <c r="D33" t="n">
-        <v>4576564220</v>
+        <v>4902210451</v>
       </c>
       <c r="E33" t="n">
-        <v>1147120402</v>
+        <v>842541829</v>
       </c>
       <c r="F33" t="n">
-        <v>-2.34665</v>
+        <v>1.16109</v>
       </c>
     </row>
     <row r="34">
@@ -1247,16 +1247,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9.050000000000001</v>
+        <v>9.609999999999999</v>
       </c>
       <c r="D34" t="n">
-        <v>4276447974</v>
+        <v>4560151261</v>
       </c>
       <c r="E34" t="n">
-        <v>243408719</v>
+        <v>272383770</v>
       </c>
       <c r="F34" t="n">
-        <v>-1.82355</v>
+        <v>8.18369</v>
       </c>
     </row>
     <row r="35">
@@ -1271,256 +1271,256 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>27.11</v>
+        <v>27.83</v>
       </c>
       <c r="D35" t="n">
-        <v>3997235093</v>
+        <v>4164131514</v>
       </c>
       <c r="E35" t="n">
-        <v>544602880</v>
+        <v>919838112</v>
       </c>
       <c r="F35" t="n">
-        <v>4.49785</v>
+        <v>8.69515</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Bonk</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>kas</t>
+          <t>bonk</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.152439</v>
+        <v>5.245e-05</v>
       </c>
       <c r="D36" t="n">
-        <v>3819883023</v>
+        <v>3920752548</v>
       </c>
       <c r="E36" t="n">
-        <v>157285828</v>
+        <v>1818347499</v>
       </c>
       <c r="F36" t="n">
-        <v>-3.75046</v>
+        <v>8.48047</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Bonk</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>bonk</t>
+          <t>render</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>5.083e-05</v>
+        <v>7.42</v>
       </c>
       <c r="D37" t="n">
-        <v>3802638214</v>
+        <v>3842357119</v>
       </c>
       <c r="E37" t="n">
-        <v>2264795895</v>
+        <v>447271818</v>
       </c>
       <c r="F37" t="n">
-        <v>-5.80249</v>
+        <v>2.09978</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>render</t>
+          <t>kas</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>7.28</v>
+        <v>0.150282</v>
       </c>
       <c r="D38" t="n">
-        <v>3740774037</v>
+        <v>3786320788</v>
       </c>
       <c r="E38" t="n">
-        <v>461217796</v>
+        <v>156046143</v>
       </c>
       <c r="F38" t="n">
-        <v>-8.3857</v>
+        <v>1.04022</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Ethena USDe</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>usde</t>
+          <t>tao</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1.003</v>
+        <v>509.21</v>
       </c>
       <c r="D39" t="n">
-        <v>3610343405</v>
+        <v>3761174767</v>
       </c>
       <c r="E39" t="n">
-        <v>234838692</v>
+        <v>268386450</v>
       </c>
       <c r="F39" t="n">
-        <v>0.1142</v>
+        <v>5.3129</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>WhiteBIT Coin</t>
+          <t>POL (ex-MATIC)</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>wbt</t>
+          <t>pol</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>24.34</v>
+        <v>0.469057</v>
       </c>
       <c r="D40" t="n">
-        <v>3499917895</v>
+        <v>3735128446</v>
       </c>
       <c r="E40" t="n">
-        <v>32243072</v>
+        <v>448961333</v>
       </c>
       <c r="F40" t="n">
-        <v>1.34249</v>
+        <v>8.945919999999999</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>POL (ex-MATIC)</t>
+          <t>Ethena USDe</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>pol</t>
+          <t>usde</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.437581</v>
+        <v>1.001</v>
       </c>
       <c r="D41" t="n">
-        <v>3471892075</v>
+        <v>3683475691</v>
       </c>
       <c r="E41" t="n">
-        <v>396338676</v>
+        <v>241476759</v>
       </c>
       <c r="F41" t="n">
-        <v>-3.14596</v>
+        <v>-0.74746</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>WhiteBIT Coin</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>tao</t>
+          <t>wbt</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>468.76</v>
+        <v>24.8</v>
       </c>
       <c r="D42" t="n">
-        <v>3442951590</v>
+        <v>3573075283</v>
       </c>
       <c r="E42" t="n">
-        <v>312282940</v>
+        <v>39356445</v>
       </c>
       <c r="F42" t="n">
-        <v>-1.41425</v>
+        <v>2.5274</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>MANTRA</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>dai</t>
+          <t>om</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1.001</v>
+        <v>3.9</v>
       </c>
       <c r="D43" t="n">
-        <v>3431816523</v>
+        <v>3506831676</v>
       </c>
       <c r="E43" t="n">
-        <v>148264128</v>
+        <v>303461473</v>
       </c>
       <c r="F43" t="n">
-        <v>0.20634</v>
+        <v>6.54558</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Artificial Superintelligence Alliance</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>fet</t>
+          <t>dai</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1.22</v>
+        <v>1.001</v>
       </c>
       <c r="D44" t="n">
-        <v>3170274451</v>
+        <v>3447798190</v>
       </c>
       <c r="E44" t="n">
-        <v>476266617</v>
+        <v>190616435</v>
       </c>
       <c r="F44" t="n">
-        <v>-4.79002</v>
+        <v>-0.27302</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>MANTRA</t>
+          <t>Artificial Superintelligence Alliance</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>om</t>
+          <t>fet</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3.54</v>
+        <v>1.28</v>
       </c>
       <c r="D45" t="n">
-        <v>3163983423</v>
+        <v>3348828073</v>
       </c>
       <c r="E45" t="n">
-        <v>290254166</v>
+        <v>499729195</v>
       </c>
       <c r="F45" t="n">
-        <v>-9.84259</v>
+        <v>5.2388</v>
       </c>
     </row>
     <row r="46">
@@ -1535,136 +1535,136 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>3.12</v>
+        <v>3.34</v>
       </c>
       <c r="D46" t="n">
-        <v>3099771503</v>
+        <v>3328766836</v>
       </c>
       <c r="E46" t="n">
-        <v>1081763550</v>
+        <v>1254384009</v>
       </c>
       <c r="F46" t="n">
-        <v>-4.47428</v>
+        <v>7.44185</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Monero</t>
+          <t>Arbitrum</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>xmr</t>
+          <t>arb</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>162.19</v>
+        <v>0.772594</v>
       </c>
       <c r="D47" t="n">
-        <v>2992996871</v>
+        <v>3165596310</v>
       </c>
       <c r="E47" t="n">
-        <v>80315182</v>
+        <v>1666852762</v>
       </c>
       <c r="F47" t="n">
-        <v>1.66498</v>
+        <v>14.65999</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Stacks</t>
+          <t>Monero</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>stx</t>
+          <t>xmr</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1.94</v>
+        <v>160.43</v>
       </c>
       <c r="D48" t="n">
-        <v>2904566939</v>
+        <v>2960160649</v>
       </c>
       <c r="E48" t="n">
-        <v>346848909</v>
+        <v>84063512</v>
       </c>
       <c r="F48" t="n">
-        <v>4.77567</v>
+        <v>-0.91329</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Arbitrum</t>
+          <t>Stacks</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>arb</t>
+          <t>stx</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.706659</v>
+        <v>1.95</v>
       </c>
       <c r="D49" t="n">
-        <v>2860377640</v>
+        <v>2922681927</v>
       </c>
       <c r="E49" t="n">
-        <v>816488352</v>
+        <v>435064718</v>
       </c>
       <c r="F49" t="n">
-        <v>0.72129</v>
+        <v>4.65692</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>fil</t>
+          <t>okb</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>4.61</v>
+        <v>46.63</v>
       </c>
       <c r="D50" t="n">
-        <v>2747439693</v>
+        <v>2800201189</v>
       </c>
       <c r="E50" t="n">
-        <v>573539595</v>
+        <v>20274712</v>
       </c>
       <c r="F50" t="n">
-        <v>5.65481</v>
+        <v>6.08207</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>mnt</t>
+          <t>fil</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.795197</v>
+        <v>4.66</v>
       </c>
       <c r="D51" t="n">
-        <v>2674621151</v>
+        <v>2795603507</v>
       </c>
       <c r="E51" t="n">
-        <v>160101806</v>
+        <v>583510661</v>
       </c>
       <c r="F51" t="n">
-        <v>9.06292</v>
+        <v>9.148809999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1937942266754</v>
+        <v>1957410186256</v>
       </c>
     </row>
     <row r="3">
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>379068348709</v>
+        <v>406015687428</v>
       </c>
     </row>
     <row r="4">
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>130187884714</v>
+        <v>130920758489</v>
       </c>
     </row>
     <row r="5">
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>114196457382</v>
+        <v>124821488522</v>
       </c>
     </row>
     <row r="6">
@@ -1745,7 +1745,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>88935613146</v>
+        <v>92924369009</v>
       </c>
     </row>
   </sheetData>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$4296.03</t>
+          <t>$4351.32</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Bitcoin Cash (18.47%)</t>
+          <t>XRP (25.02%)</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MANTRA (-9.84%)</t>
+          <t>Monero (-0.91%)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Excel data - 2024-11-22 04:16:10
</commit_message>
<xml_diff>
--- a/crypto_live_data.xlsx
+++ b/crypto_live_data.xlsx
@@ -479,16 +479,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>98936</v>
+        <v>98908</v>
       </c>
       <c r="D2" t="n">
-        <v>1957410186256</v>
+        <v>1959097766308</v>
       </c>
       <c r="E2" t="n">
-        <v>115913150141</v>
+        <v>117523219357</v>
       </c>
       <c r="F2" t="n">
-        <v>2.57984</v>
+        <v>1.99672</v>
       </c>
     </row>
     <row r="3">
@@ -503,16 +503,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3371.17</v>
+        <v>3368.9</v>
       </c>
       <c r="D3" t="n">
-        <v>406015687428</v>
+        <v>405800320131</v>
       </c>
       <c r="E3" t="n">
-        <v>57864085710</v>
+        <v>57542450103</v>
       </c>
       <c r="F3" t="n">
-        <v>8.711589999999999</v>
+        <v>8.200049999999999</v>
       </c>
     </row>
     <row r="4">
@@ -527,16 +527,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.002</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>130920758489</v>
+        <v>130852749175</v>
       </c>
       <c r="E4" t="n">
-        <v>180658001561</v>
+        <v>130067665585</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.33176</v>
+        <v>-0.22882</v>
       </c>
     </row>
     <row r="5">
@@ -551,16 +551,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>262.94</v>
+        <v>262.46</v>
       </c>
       <c r="D5" t="n">
-        <v>124821488522</v>
+        <v>124608104880</v>
       </c>
       <c r="E5" t="n">
-        <v>15497913447</v>
+        <v>15419995084</v>
       </c>
       <c r="F5" t="n">
-        <v>10.74741</v>
+        <v>10.2062</v>
       </c>
     </row>
     <row r="6">
@@ -575,16 +575,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>636.66</v>
+        <v>635.28</v>
       </c>
       <c r="D6" t="n">
-        <v>92924369009</v>
+        <v>92807675426</v>
       </c>
       <c r="E6" t="n">
-        <v>2560789290</v>
+        <v>2516065309</v>
       </c>
       <c r="F6" t="n">
-        <v>5.02412</v>
+        <v>4.67069</v>
       </c>
     </row>
     <row r="7">
@@ -599,16 +599,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.38</v>
+        <v>1.41</v>
       </c>
       <c r="D7" t="n">
-        <v>78666166648</v>
+        <v>79540572467</v>
       </c>
       <c r="E7" t="n">
-        <v>17004059380</v>
+        <v>17360543557</v>
       </c>
       <c r="F7" t="n">
-        <v>25.01952</v>
+        <v>27.87191</v>
       </c>
     </row>
     <row r="8">
@@ -623,16 +623,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.393894</v>
+        <v>0.39439</v>
       </c>
       <c r="D8" t="n">
-        <v>57853509205</v>
+        <v>58022297417</v>
       </c>
       <c r="E8" t="n">
-        <v>10366188434</v>
+        <v>10350503719</v>
       </c>
       <c r="F8" t="n">
-        <v>3.63818</v>
+        <v>3.64119</v>
       </c>
     </row>
     <row r="9">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0.999438</v>
       </c>
       <c r="D9" t="n">
-        <v>38253314257</v>
+        <v>38245803318</v>
       </c>
       <c r="E9" t="n">
-        <v>17378138495</v>
+        <v>15337728230</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.29745</v>
+        <v>-0.36921</v>
       </c>
     </row>
     <row r="10">
@@ -671,16 +671,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3367.64</v>
+        <v>3369.5</v>
       </c>
       <c r="D10" t="n">
-        <v>32985342102</v>
+        <v>33013322092</v>
       </c>
       <c r="E10" t="n">
-        <v>149669851</v>
+        <v>148862892</v>
       </c>
       <c r="F10" t="n">
-        <v>8.403560000000001</v>
+        <v>8.480880000000001</v>
       </c>
     </row>
     <row r="11">
@@ -695,16 +695,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.869827</v>
+        <v>0.875708</v>
       </c>
       <c r="D11" t="n">
-        <v>31086812023</v>
+        <v>31240593922</v>
       </c>
       <c r="E11" t="n">
-        <v>3350520127</v>
+        <v>3600505014</v>
       </c>
       <c r="F11" t="n">
-        <v>11.21959</v>
+        <v>11.54925</v>
       </c>
     </row>
     <row r="12">
@@ -719,16 +719,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.200809</v>
+        <v>0.200701</v>
       </c>
       <c r="D12" t="n">
-        <v>17337544762</v>
+        <v>17345913079</v>
       </c>
       <c r="E12" t="n">
-        <v>1063110796</v>
+        <v>1083382796</v>
       </c>
       <c r="F12" t="n">
-        <v>2.15375</v>
+        <v>2.01243</v>
       </c>
     </row>
     <row r="13">
@@ -743,16 +743,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>36.29</v>
+        <v>36.31</v>
       </c>
       <c r="D13" t="n">
-        <v>14842978811</v>
+        <v>14847880210</v>
       </c>
       <c r="E13" t="n">
-        <v>1056089658</v>
+        <v>1051213844</v>
       </c>
       <c r="F13" t="n">
-        <v>8.61652</v>
+        <v>8.219150000000001</v>
       </c>
     </row>
     <row r="14">
@@ -767,16 +767,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.499e-05</v>
+        <v>2.497e-05</v>
       </c>
       <c r="D14" t="n">
-        <v>14710554787</v>
+        <v>14731569383</v>
       </c>
       <c r="E14" t="n">
-        <v>1616603700</v>
+        <v>1612892764</v>
       </c>
       <c r="F14" t="n">
-        <v>5.48248</v>
+        <v>4.98286</v>
       </c>
     </row>
     <row r="15">
@@ -791,16 +791,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>98586</v>
+        <v>98573</v>
       </c>
       <c r="D15" t="n">
-        <v>14398896989</v>
+        <v>14416601502</v>
       </c>
       <c r="E15" t="n">
-        <v>921826657</v>
+        <v>906539844</v>
       </c>
       <c r="F15" t="n">
-        <v>2.38183</v>
+        <v>2.03488</v>
       </c>
     </row>
     <row r="16">
@@ -815,16 +815,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3988.96</v>
+        <v>3986.68</v>
       </c>
       <c r="D16" t="n">
-        <v>14386360829</v>
+        <v>14404222176</v>
       </c>
       <c r="E16" t="n">
-        <v>167163549</v>
+        <v>170561570</v>
       </c>
       <c r="F16" t="n">
-        <v>8.905950000000001</v>
+        <v>8.663069999999999</v>
       </c>
     </row>
     <row r="17">
@@ -842,13 +842,13 @@
         <v>5.55</v>
       </c>
       <c r="D17" t="n">
-        <v>14144705757</v>
+        <v>14132776098</v>
       </c>
       <c r="E17" t="n">
-        <v>621432219</v>
+        <v>620294970</v>
       </c>
       <c r="F17" t="n">
-        <v>4.44313</v>
+        <v>4.18105</v>
       </c>
     </row>
     <row r="18">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3.6</v>
+        <v>3.63</v>
       </c>
       <c r="D18" t="n">
-        <v>10231629493</v>
+        <v>10344756784</v>
       </c>
       <c r="E18" t="n">
-        <v>2287578574</v>
+        <v>2290801051</v>
       </c>
       <c r="F18" t="n">
-        <v>2.74334</v>
+        <v>3.47325</v>
       </c>
     </row>
     <row r="19">
@@ -887,16 +887,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>494.5</v>
+        <v>492.32</v>
       </c>
       <c r="D19" t="n">
-        <v>9798830623</v>
+        <v>9747842327</v>
       </c>
       <c r="E19" t="n">
-        <v>2350395615</v>
+        <v>2304543250</v>
       </c>
       <c r="F19" t="n">
-        <v>7.71998</v>
+        <v>5.4817</v>
       </c>
     </row>
     <row r="20">
@@ -911,16 +911,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3373.33</v>
+        <v>3369.49</v>
       </c>
       <c r="D20" t="n">
-        <v>9708765975</v>
+        <v>9689653263</v>
       </c>
       <c r="E20" t="n">
-        <v>519332627</v>
+        <v>2280080043</v>
       </c>
       <c r="F20" t="n">
-        <v>8.80829</v>
+        <v>8.377230000000001</v>
       </c>
     </row>
     <row r="21">
@@ -935,16 +935,16 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>15.12</v>
+        <v>15.1</v>
       </c>
       <c r="D21" t="n">
-        <v>9500220377</v>
+        <v>9464894293</v>
       </c>
       <c r="E21" t="n">
-        <v>1223424068</v>
+        <v>1224865617</v>
       </c>
       <c r="F21" t="n">
-        <v>6.34317</v>
+        <v>5.4432</v>
       </c>
     </row>
     <row r="22">
@@ -959,16 +959,16 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.142e-05</v>
+        <v>2.143e-05</v>
       </c>
       <c r="D22" t="n">
-        <v>9014421360</v>
+        <v>9017977603</v>
       </c>
       <c r="E22" t="n">
-        <v>7032492661</v>
+        <v>7053073138</v>
       </c>
       <c r="F22" t="n">
-        <v>13.29684</v>
+        <v>13.76133</v>
       </c>
     </row>
     <row r="23">
@@ -983,16 +983,16 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>6.17</v>
+        <v>6.18</v>
       </c>
       <c r="D23" t="n">
-        <v>8881549580</v>
+        <v>8890725340</v>
       </c>
       <c r="E23" t="n">
-        <v>814547946</v>
+        <v>813834898</v>
       </c>
       <c r="F23" t="n">
-        <v>9.85849</v>
+        <v>9.62811</v>
       </c>
     </row>
     <row r="24">
@@ -1007,16 +1007,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.283117</v>
+        <v>0.287069</v>
       </c>
       <c r="D24" t="n">
-        <v>8501860012</v>
+        <v>8573585584</v>
       </c>
       <c r="E24" t="n">
-        <v>2311728073</v>
+        <v>2350798434</v>
       </c>
       <c r="F24" t="n">
-        <v>17.79302</v>
+        <v>20.15183</v>
       </c>
     </row>
     <row r="25">
@@ -1031,16 +1031,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>8.76</v>
+        <v>8.74</v>
       </c>
       <c r="D25" t="n">
-        <v>8078033416</v>
+        <v>8086736861</v>
       </c>
       <c r="E25" t="n">
-        <v>3517774</v>
+        <v>3486171</v>
       </c>
       <c r="F25" t="n">
-        <v>2.67332</v>
+        <v>2.21077</v>
       </c>
     </row>
     <row r="26">
@@ -1058,13 +1058,13 @@
         <v>5.78</v>
       </c>
       <c r="D26" t="n">
-        <v>7035895518</v>
+        <v>7044182679</v>
       </c>
       <c r="E26" t="n">
-        <v>968924810</v>
+        <v>1020700272</v>
       </c>
       <c r="F26" t="n">
-        <v>5.61817</v>
+        <v>5.52506</v>
       </c>
     </row>
     <row r="27">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>90.19</v>
+        <v>90.17</v>
       </c>
       <c r="D27" t="n">
-        <v>6784076065</v>
+        <v>6785098387</v>
       </c>
       <c r="E27" t="n">
-        <v>1460843275</v>
+        <v>1470715698</v>
       </c>
       <c r="F27" t="n">
-        <v>6.54217</v>
+        <v>5.87394</v>
       </c>
     </row>
     <row r="28">
@@ -1106,13 +1106,13 @@
         <v>12.1</v>
       </c>
       <c r="D28" t="n">
-        <v>6453451196</v>
+        <v>6453178954</v>
       </c>
       <c r="E28" t="n">
-        <v>895334881</v>
+        <v>896912955</v>
       </c>
       <c r="F28" t="n">
-        <v>5.04982</v>
+        <v>5.1022</v>
       </c>
     </row>
     <row r="29">
@@ -1127,16 +1127,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3544.81</v>
+        <v>3550.07</v>
       </c>
       <c r="D29" t="n">
-        <v>6101083612</v>
+        <v>6115781119</v>
       </c>
       <c r="E29" t="n">
-        <v>96814193</v>
+        <v>99952442</v>
       </c>
       <c r="F29" t="n">
-        <v>9.20321</v>
+        <v>8.49728</v>
       </c>
     </row>
     <row r="30">
@@ -1154,13 +1154,13 @@
         <v>9.35</v>
       </c>
       <c r="D30" t="n">
-        <v>5609709607</v>
+        <v>5618106680</v>
       </c>
       <c r="E30" t="n">
-        <v>847563217</v>
+        <v>843765851</v>
       </c>
       <c r="F30" t="n">
-        <v>7.90214</v>
+        <v>7.27596</v>
       </c>
     </row>
     <row r="31">
@@ -1175,16 +1175,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.196843</v>
+        <v>0.195965</v>
       </c>
       <c r="D31" t="n">
-        <v>5336019451</v>
+        <v>5329889908</v>
       </c>
       <c r="E31" t="n">
-        <v>115416917</v>
+        <v>115257302</v>
       </c>
       <c r="F31" t="n">
-        <v>10.11105</v>
+        <v>10.52595</v>
       </c>
     </row>
     <row r="32">
@@ -1199,16 +1199,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1.008</v>
+        <v>0.999322</v>
       </c>
       <c r="D32" t="n">
-        <v>5286602021</v>
+        <v>5247228065</v>
       </c>
       <c r="E32" t="n">
-        <v>16038564</v>
+        <v>15845976</v>
       </c>
       <c r="F32" t="n">
-        <v>0.24725</v>
+        <v>-0.27986</v>
       </c>
     </row>
     <row r="33">
@@ -1223,16 +1223,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.129052</v>
+        <v>0.129255</v>
       </c>
       <c r="D33" t="n">
-        <v>4902210451</v>
+        <v>4971045961</v>
       </c>
       <c r="E33" t="n">
-        <v>842541829</v>
+        <v>837343150</v>
       </c>
       <c r="F33" t="n">
-        <v>1.16109</v>
+        <v>2.23502</v>
       </c>
     </row>
     <row r="34">
@@ -1247,16 +1247,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9.609999999999999</v>
+        <v>9.640000000000001</v>
       </c>
       <c r="D34" t="n">
-        <v>4560151261</v>
+        <v>4574014220</v>
       </c>
       <c r="E34" t="n">
-        <v>272383770</v>
+        <v>271213610</v>
       </c>
       <c r="F34" t="n">
-        <v>8.18369</v>
+        <v>8.047980000000001</v>
       </c>
     </row>
     <row r="35">
@@ -1271,16 +1271,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>27.83</v>
+        <v>27.84</v>
       </c>
       <c r="D35" t="n">
-        <v>4164131514</v>
+        <v>4162099848</v>
       </c>
       <c r="E35" t="n">
-        <v>919838112</v>
+        <v>908771366</v>
       </c>
       <c r="F35" t="n">
-        <v>8.69515</v>
+        <v>6.91992</v>
       </c>
     </row>
     <row r="36">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>5.245e-05</v>
+        <v>5.231e-05</v>
       </c>
       <c r="D36" t="n">
-        <v>3920752548</v>
+        <v>3935128733</v>
       </c>
       <c r="E36" t="n">
-        <v>1818347499</v>
+        <v>1815144801</v>
       </c>
       <c r="F36" t="n">
-        <v>8.48047</v>
+        <v>7.91315</v>
       </c>
     </row>
     <row r="37">
@@ -1319,16 +1319,16 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>7.42</v>
+        <v>7.41</v>
       </c>
       <c r="D37" t="n">
-        <v>3842357119</v>
+        <v>3836472884</v>
       </c>
       <c r="E37" t="n">
-        <v>447271818</v>
+        <v>443348294</v>
       </c>
       <c r="F37" t="n">
-        <v>2.09978</v>
+        <v>1.65585</v>
       </c>
     </row>
     <row r="38">
@@ -1343,16 +1343,16 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.150282</v>
+        <v>0.150396</v>
       </c>
       <c r="D38" t="n">
-        <v>3786320788</v>
+        <v>3792375092</v>
       </c>
       <c r="E38" t="n">
-        <v>156046143</v>
+        <v>155813335</v>
       </c>
       <c r="F38" t="n">
-        <v>1.04022</v>
+        <v>0.70825</v>
       </c>
     </row>
     <row r="39">
@@ -1367,16 +1367,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>509.21</v>
+        <v>509.73</v>
       </c>
       <c r="D39" t="n">
-        <v>3761174767</v>
+        <v>3763333252</v>
       </c>
       <c r="E39" t="n">
-        <v>268386450</v>
+        <v>288200562</v>
       </c>
       <c r="F39" t="n">
-        <v>5.3129</v>
+        <v>4.82107</v>
       </c>
     </row>
     <row r="40">
@@ -1391,16 +1391,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.469057</v>
+        <v>0.467259</v>
       </c>
       <c r="D40" t="n">
-        <v>3735128446</v>
+        <v>3724428423</v>
       </c>
       <c r="E40" t="n">
-        <v>448961333</v>
+        <v>473813459</v>
       </c>
       <c r="F40" t="n">
-        <v>8.945919999999999</v>
+        <v>8.26056</v>
       </c>
     </row>
     <row r="41">
@@ -1418,13 +1418,13 @@
         <v>1.001</v>
       </c>
       <c r="D41" t="n">
-        <v>3683475691</v>
+        <v>3687567717</v>
       </c>
       <c r="E41" t="n">
-        <v>241476759</v>
+        <v>237089640</v>
       </c>
       <c r="F41" t="n">
-        <v>-0.74746</v>
+        <v>-0.17128</v>
       </c>
     </row>
     <row r="42">
@@ -1439,16 +1439,16 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>24.8</v>
+        <v>24.78</v>
       </c>
       <c r="D42" t="n">
-        <v>3573075283</v>
+        <v>3573423906</v>
       </c>
       <c r="E42" t="n">
-        <v>39356445</v>
+        <v>38290921</v>
       </c>
       <c r="F42" t="n">
-        <v>2.5274</v>
+        <v>2.73603</v>
       </c>
     </row>
     <row r="43">
@@ -1463,16 +1463,16 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>3.9</v>
+        <v>3.91</v>
       </c>
       <c r="D43" t="n">
-        <v>3506831676</v>
+        <v>3529178084</v>
       </c>
       <c r="E43" t="n">
-        <v>303461473</v>
+        <v>306842077</v>
       </c>
       <c r="F43" t="n">
-        <v>6.54558</v>
+        <v>6.83721</v>
       </c>
     </row>
     <row r="44">
@@ -1487,64 +1487,64 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1.001</v>
+        <v>0.999465</v>
       </c>
       <c r="D44" t="n">
-        <v>3447798190</v>
+        <v>3441616760</v>
       </c>
       <c r="E44" t="n">
-        <v>190616435</v>
+        <v>163474938</v>
       </c>
       <c r="F44" t="n">
-        <v>-0.27302</v>
+        <v>-0.28609</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Artificial Superintelligence Alliance</t>
+          <t>dogwifhat</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>fet</t>
+          <t>wif</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1.28</v>
+        <v>3.37</v>
       </c>
       <c r="D45" t="n">
-        <v>3348828073</v>
+        <v>3367531542</v>
       </c>
       <c r="E45" t="n">
-        <v>499729195</v>
+        <v>1269991304</v>
       </c>
       <c r="F45" t="n">
-        <v>5.2388</v>
+        <v>8.123480000000001</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>dogwifhat</t>
+          <t>Artificial Superintelligence Alliance</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>wif</t>
+          <t>fet</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>3.34</v>
+        <v>1.28</v>
       </c>
       <c r="D46" t="n">
-        <v>3328766836</v>
+        <v>3343687076</v>
       </c>
       <c r="E46" t="n">
-        <v>1254384009</v>
+        <v>496379708</v>
       </c>
       <c r="F46" t="n">
-        <v>7.44185</v>
+        <v>4.92834</v>
       </c>
     </row>
     <row r="47">
@@ -1559,16 +1559,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.772594</v>
+        <v>0.773817</v>
       </c>
       <c r="D47" t="n">
-        <v>3165596310</v>
+        <v>3171101048</v>
       </c>
       <c r="E47" t="n">
-        <v>1666852762</v>
+        <v>1667534686</v>
       </c>
       <c r="F47" t="n">
-        <v>14.65999</v>
+        <v>14.03529</v>
       </c>
     </row>
     <row r="48">
@@ -1583,16 +1583,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>160.43</v>
+        <v>160.25</v>
       </c>
       <c r="D48" t="n">
-        <v>2960160649</v>
+        <v>2957759868</v>
       </c>
       <c r="E48" t="n">
-        <v>84063512</v>
+        <v>84034592</v>
       </c>
       <c r="F48" t="n">
-        <v>-0.91329</v>
+        <v>-1.14394</v>
       </c>
     </row>
     <row r="49">
@@ -1607,64 +1607,64 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1.95</v>
+        <v>1.94</v>
       </c>
       <c r="D49" t="n">
-        <v>2922681927</v>
+        <v>2918415642</v>
       </c>
       <c r="E49" t="n">
-        <v>435064718</v>
+        <v>422364809</v>
       </c>
       <c r="F49" t="n">
-        <v>4.65692</v>
+        <v>2.84764</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>okb</t>
+          <t>fil</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>46.63</v>
+        <v>4.67</v>
       </c>
       <c r="D50" t="n">
-        <v>2800201189</v>
+        <v>2805339303</v>
       </c>
       <c r="E50" t="n">
-        <v>20274712</v>
+        <v>584722236</v>
       </c>
       <c r="F50" t="n">
-        <v>6.08207</v>
+        <v>8.904389999999999</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>OKB</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>fil</t>
+          <t>okb</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>4.66</v>
+        <v>46.56</v>
       </c>
       <c r="D51" t="n">
-        <v>2795603507</v>
+        <v>2795155174</v>
       </c>
       <c r="E51" t="n">
-        <v>583510661</v>
+        <v>20372276</v>
       </c>
       <c r="F51" t="n">
-        <v>9.148809999999999</v>
+        <v>6.04536</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1957410186256</v>
+        <v>1959097766308</v>
       </c>
     </row>
     <row r="3">
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>406015687428</v>
+        <v>405800320131</v>
       </c>
     </row>
     <row r="4">
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>130920758489</v>
+        <v>130852749175</v>
       </c>
     </row>
     <row r="5">
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>124821488522</v>
+        <v>124608104880</v>
       </c>
     </row>
     <row r="6">
@@ -1745,7 +1745,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>92924369009</v>
+        <v>92807675426</v>
       </c>
     </row>
   </sheetData>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$4351.32</t>
+          <t>$4350.40</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>XRP (25.02%)</t>
+          <t>XRP (27.87%)</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Monero (-0.91%)</t>
+          <t>Monero (-1.14%)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Excel data - 2024-11-22 04:26:12
</commit_message>
<xml_diff>
--- a/crypto_live_data.xlsx
+++ b/crypto_live_data.xlsx
@@ -479,16 +479,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>98908</v>
+        <v>99002</v>
       </c>
       <c r="D2" t="n">
-        <v>1959097766308</v>
+        <v>1957894470032</v>
       </c>
       <c r="E2" t="n">
-        <v>117523219357</v>
+        <v>118089762693</v>
       </c>
       <c r="F2" t="n">
-        <v>1.99672</v>
+        <v>2.41144</v>
       </c>
     </row>
     <row r="3">
@@ -503,16 +503,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3368.9</v>
+        <v>3381.18</v>
       </c>
       <c r="D3" t="n">
-        <v>405800320131</v>
+        <v>406862764584</v>
       </c>
       <c r="E3" t="n">
-        <v>57542450103</v>
+        <v>57938597348</v>
       </c>
       <c r="F3" t="n">
-        <v>8.200049999999999</v>
+        <v>9.056800000000001</v>
       </c>
     </row>
     <row r="4">
@@ -527,16 +527,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>1.002</v>
       </c>
       <c r="D4" t="n">
-        <v>130852749175</v>
+        <v>130949157622</v>
       </c>
       <c r="E4" t="n">
-        <v>130067665585</v>
+        <v>173551742236</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.22882</v>
+        <v>0.11938</v>
       </c>
     </row>
     <row r="5">
@@ -551,16 +551,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>262.46</v>
+        <v>262.44</v>
       </c>
       <c r="D5" t="n">
-        <v>124608104880</v>
+        <v>124220173708</v>
       </c>
       <c r="E5" t="n">
-        <v>15419995084</v>
+        <v>15298491107</v>
       </c>
       <c r="F5" t="n">
-        <v>10.2062</v>
+        <v>10.80211</v>
       </c>
     </row>
     <row r="6">
@@ -575,16 +575,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>635.28</v>
+        <v>635.4</v>
       </c>
       <c r="D6" t="n">
-        <v>92807675426</v>
+        <v>92659978087</v>
       </c>
       <c r="E6" t="n">
-        <v>2516065309</v>
+        <v>2511013877</v>
       </c>
       <c r="F6" t="n">
-        <v>4.67069</v>
+        <v>5.36731</v>
       </c>
     </row>
     <row r="7">
@@ -599,16 +599,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.41</v>
+        <v>1.42</v>
       </c>
       <c r="D7" t="n">
-        <v>79540572467</v>
+        <v>80591370672</v>
       </c>
       <c r="E7" t="n">
-        <v>17360543557</v>
+        <v>17643086232</v>
       </c>
       <c r="F7" t="n">
-        <v>27.87191</v>
+        <v>29.46279</v>
       </c>
     </row>
     <row r="8">
@@ -623,16 +623,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.39439</v>
+        <v>0.395552</v>
       </c>
       <c r="D8" t="n">
-        <v>58022297417</v>
+        <v>58058582415</v>
       </c>
       <c r="E8" t="n">
-        <v>10350503719</v>
+        <v>10368763281</v>
       </c>
       <c r="F8" t="n">
-        <v>3.64119</v>
+        <v>4.5807</v>
       </c>
     </row>
     <row r="9">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.999438</v>
+        <v>1.001</v>
       </c>
       <c r="D9" t="n">
-        <v>38245803318</v>
+        <v>38260938357</v>
       </c>
       <c r="E9" t="n">
-        <v>15337728230</v>
+        <v>10560509915</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.36921</v>
+        <v>0.04934</v>
       </c>
     </row>
     <row r="10">
@@ -671,16 +671,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3369.5</v>
+        <v>3383.67</v>
       </c>
       <c r="D10" t="n">
-        <v>33013322092</v>
+        <v>33041881744</v>
       </c>
       <c r="E10" t="n">
-        <v>148862892</v>
+        <v>148028738</v>
       </c>
       <c r="F10" t="n">
-        <v>8.480880000000001</v>
+        <v>9.25051</v>
       </c>
     </row>
     <row r="11">
@@ -695,16 +695,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.875708</v>
+        <v>0.891699</v>
       </c>
       <c r="D11" t="n">
-        <v>31240593922</v>
+        <v>31872011634</v>
       </c>
       <c r="E11" t="n">
-        <v>3600505014</v>
+        <v>3682783069</v>
       </c>
       <c r="F11" t="n">
-        <v>11.54925</v>
+        <v>14.8535</v>
       </c>
     </row>
     <row r="12">
@@ -719,16 +719,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.200701</v>
+        <v>0.20108</v>
       </c>
       <c r="D12" t="n">
-        <v>17345913079</v>
+        <v>17356540142</v>
       </c>
       <c r="E12" t="n">
-        <v>1083382796</v>
+        <v>1103322051</v>
       </c>
       <c r="F12" t="n">
-        <v>2.01243</v>
+        <v>2.57305</v>
       </c>
     </row>
     <row r="13">
@@ -743,16 +743,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>36.31</v>
+        <v>36.36</v>
       </c>
       <c r="D13" t="n">
-        <v>14847880210</v>
+        <v>14842131964</v>
       </c>
       <c r="E13" t="n">
-        <v>1051213844</v>
+        <v>1050149638</v>
       </c>
       <c r="F13" t="n">
-        <v>8.219150000000001</v>
+        <v>9.352589999999999</v>
       </c>
     </row>
     <row r="14">
@@ -767,16 +767,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.497e-05</v>
+        <v>2.501e-05</v>
       </c>
       <c r="D14" t="n">
-        <v>14731569383</v>
+        <v>14692282099</v>
       </c>
       <c r="E14" t="n">
-        <v>1612892764</v>
+        <v>1619515324</v>
       </c>
       <c r="F14" t="n">
-        <v>4.98286</v>
+        <v>5.795</v>
       </c>
     </row>
     <row r="15">
@@ -791,16 +791,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>98573</v>
+        <v>98749</v>
       </c>
       <c r="D15" t="n">
-        <v>14416601502</v>
+        <v>14410037964</v>
       </c>
       <c r="E15" t="n">
-        <v>906539844</v>
+        <v>901639215</v>
       </c>
       <c r="F15" t="n">
-        <v>2.03488</v>
+        <v>2.73716</v>
       </c>
     </row>
     <row r="16">
@@ -815,16 +815,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3986.68</v>
+        <v>4000.57</v>
       </c>
       <c r="D16" t="n">
-        <v>14404222176</v>
+        <v>14392682837</v>
       </c>
       <c r="E16" t="n">
-        <v>170561570</v>
+        <v>167702447</v>
       </c>
       <c r="F16" t="n">
-        <v>8.663069999999999</v>
+        <v>9.100989999999999</v>
       </c>
     </row>
     <row r="17">
@@ -839,16 +839,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5.55</v>
+        <v>5.56</v>
       </c>
       <c r="D17" t="n">
-        <v>14132776098</v>
+        <v>14148936409</v>
       </c>
       <c r="E17" t="n">
-        <v>620294970</v>
+        <v>619899192</v>
       </c>
       <c r="F17" t="n">
-        <v>4.18105</v>
+        <v>4.88377</v>
       </c>
     </row>
     <row r="18">
@@ -866,13 +866,13 @@
         <v>3.63</v>
       </c>
       <c r="D18" t="n">
-        <v>10344756784</v>
+        <v>10308929159</v>
       </c>
       <c r="E18" t="n">
-        <v>2290801051</v>
+        <v>2225166820</v>
       </c>
       <c r="F18" t="n">
-        <v>3.47325</v>
+        <v>4.19795</v>
       </c>
     </row>
     <row r="19">
@@ -887,16 +887,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>492.32</v>
+        <v>494.24</v>
       </c>
       <c r="D19" t="n">
-        <v>9747842327</v>
+        <v>9777605296</v>
       </c>
       <c r="E19" t="n">
-        <v>2304543250</v>
+        <v>2283872731</v>
       </c>
       <c r="F19" t="n">
-        <v>5.4817</v>
+        <v>6.40315</v>
       </c>
     </row>
     <row r="20">
@@ -911,16 +911,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3369.49</v>
+        <v>3377.99</v>
       </c>
       <c r="D20" t="n">
-        <v>9689653263</v>
+        <v>9686429221</v>
       </c>
       <c r="E20" t="n">
-        <v>2280080043</v>
+        <v>2254650087</v>
       </c>
       <c r="F20" t="n">
-        <v>8.377230000000001</v>
+        <v>9.13232</v>
       </c>
     </row>
     <row r="21">
@@ -935,16 +935,16 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>15.1</v>
+        <v>15.15</v>
       </c>
       <c r="D21" t="n">
-        <v>9464894293</v>
+        <v>9490558072</v>
       </c>
       <c r="E21" t="n">
-        <v>1224865617</v>
+        <v>1228707366</v>
       </c>
       <c r="F21" t="n">
-        <v>5.4432</v>
+        <v>6.48594</v>
       </c>
     </row>
     <row r="22">
@@ -959,16 +959,16 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.143e-05</v>
+        <v>2.141e-05</v>
       </c>
       <c r="D22" t="n">
-        <v>9017977603</v>
+        <v>8987945059</v>
       </c>
       <c r="E22" t="n">
-        <v>7053073138</v>
+        <v>7056904336</v>
       </c>
       <c r="F22" t="n">
-        <v>13.76133</v>
+        <v>15.03015</v>
       </c>
     </row>
     <row r="23">
@@ -983,16 +983,16 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>6.18</v>
+        <v>6.23</v>
       </c>
       <c r="D23" t="n">
-        <v>8890725340</v>
+        <v>8921157612</v>
       </c>
       <c r="E23" t="n">
-        <v>813834898</v>
+        <v>821158717</v>
       </c>
       <c r="F23" t="n">
-        <v>9.62811</v>
+        <v>11.8257</v>
       </c>
     </row>
     <row r="24">
@@ -1007,16 +1007,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.287069</v>
+        <v>0.287482</v>
       </c>
       <c r="D24" t="n">
-        <v>8573585584</v>
+        <v>8619859512</v>
       </c>
       <c r="E24" t="n">
-        <v>2350798434</v>
+        <v>2353187735</v>
       </c>
       <c r="F24" t="n">
-        <v>20.15183</v>
+        <v>22.54928</v>
       </c>
     </row>
     <row r="25">
@@ -1031,16 +1031,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>8.74</v>
+        <v>8.73</v>
       </c>
       <c r="D25" t="n">
-        <v>8086736861</v>
+        <v>8070751002</v>
       </c>
       <c r="E25" t="n">
-        <v>3486171</v>
+        <v>3455613</v>
       </c>
       <c r="F25" t="n">
-        <v>2.21077</v>
+        <v>2.38203</v>
       </c>
     </row>
     <row r="26">
@@ -1055,16 +1055,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>5.78</v>
+        <v>5.8</v>
       </c>
       <c r="D26" t="n">
-        <v>7044182679</v>
+        <v>7040976947</v>
       </c>
       <c r="E26" t="n">
-        <v>1020700272</v>
+        <v>1021697502</v>
       </c>
       <c r="F26" t="n">
-        <v>5.52506</v>
+        <v>7.08168</v>
       </c>
     </row>
     <row r="27">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>90.17</v>
+        <v>90.36</v>
       </c>
       <c r="D27" t="n">
-        <v>6785098387</v>
+        <v>6794019549</v>
       </c>
       <c r="E27" t="n">
-        <v>1470715698</v>
+        <v>1430474849</v>
       </c>
       <c r="F27" t="n">
-        <v>5.87394</v>
+        <v>6.60149</v>
       </c>
     </row>
     <row r="28">
@@ -1106,13 +1106,13 @@
         <v>12.1</v>
       </c>
       <c r="D28" t="n">
-        <v>6453178954</v>
+        <v>6439611393</v>
       </c>
       <c r="E28" t="n">
-        <v>896912955</v>
+        <v>899442878</v>
       </c>
       <c r="F28" t="n">
-        <v>5.1022</v>
+        <v>6.00717</v>
       </c>
     </row>
     <row r="29">
@@ -1127,16 +1127,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3550.07</v>
+        <v>3551.03</v>
       </c>
       <c r="D29" t="n">
-        <v>6115781119</v>
+        <v>6104576415</v>
       </c>
       <c r="E29" t="n">
-        <v>99952442</v>
+        <v>99949949</v>
       </c>
       <c r="F29" t="n">
-        <v>8.49728</v>
+        <v>8.69844</v>
       </c>
     </row>
     <row r="30">
@@ -1151,16 +1151,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9.35</v>
+        <v>9.369999999999999</v>
       </c>
       <c r="D30" t="n">
-        <v>5618106680</v>
+        <v>5606275386</v>
       </c>
       <c r="E30" t="n">
-        <v>843765851</v>
+        <v>844571896</v>
       </c>
       <c r="F30" t="n">
-        <v>7.27596</v>
+        <v>8.29304</v>
       </c>
     </row>
     <row r="31">
@@ -1175,16 +1175,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.195965</v>
+        <v>0.195206</v>
       </c>
       <c r="D31" t="n">
-        <v>5329889908</v>
+        <v>5297479520</v>
       </c>
       <c r="E31" t="n">
-        <v>115257302</v>
+        <v>115772728</v>
       </c>
       <c r="F31" t="n">
-        <v>10.52595</v>
+        <v>11.89512</v>
       </c>
     </row>
     <row r="32">
@@ -1199,16 +1199,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.999322</v>
+        <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>5247228065</v>
+        <v>5243513951</v>
       </c>
       <c r="E32" t="n">
-        <v>15845976</v>
+        <v>15727350</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.27986</v>
+        <v>-0.10343</v>
       </c>
     </row>
     <row r="33">
@@ -1223,16 +1223,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.129255</v>
+        <v>0.132078</v>
       </c>
       <c r="D33" t="n">
-        <v>4971045961</v>
+        <v>5038922708</v>
       </c>
       <c r="E33" t="n">
-        <v>837343150</v>
+        <v>855228186</v>
       </c>
       <c r="F33" t="n">
-        <v>2.23502</v>
+        <v>5.7654</v>
       </c>
     </row>
     <row r="34">
@@ -1247,16 +1247,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9.640000000000001</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="D34" t="n">
-        <v>4574014220</v>
+        <v>4588051994</v>
       </c>
       <c r="E34" t="n">
-        <v>271213610</v>
+        <v>272484306</v>
       </c>
       <c r="F34" t="n">
-        <v>8.047980000000001</v>
+        <v>9.55508</v>
       </c>
     </row>
     <row r="35">
@@ -1271,16 +1271,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>27.84</v>
+        <v>27.95</v>
       </c>
       <c r="D35" t="n">
-        <v>4162099848</v>
+        <v>4176985543</v>
       </c>
       <c r="E35" t="n">
-        <v>908771366</v>
+        <v>904902335</v>
       </c>
       <c r="F35" t="n">
-        <v>6.91992</v>
+        <v>7.9547</v>
       </c>
     </row>
     <row r="36">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>5.231e-05</v>
+        <v>5.227e-05</v>
       </c>
       <c r="D36" t="n">
-        <v>3935128733</v>
+        <v>3918665466</v>
       </c>
       <c r="E36" t="n">
-        <v>1815144801</v>
+        <v>1811077711</v>
       </c>
       <c r="F36" t="n">
-        <v>7.91315</v>
+        <v>8.74653</v>
       </c>
     </row>
     <row r="37">
@@ -1322,13 +1322,13 @@
         <v>7.41</v>
       </c>
       <c r="D37" t="n">
-        <v>3836472884</v>
+        <v>3820237069</v>
       </c>
       <c r="E37" t="n">
-        <v>443348294</v>
+        <v>445811950</v>
       </c>
       <c r="F37" t="n">
-        <v>1.65585</v>
+        <v>2.8475</v>
       </c>
     </row>
     <row r="38">
@@ -1343,16 +1343,16 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.150396</v>
+        <v>0.150729</v>
       </c>
       <c r="D38" t="n">
-        <v>3792375092</v>
+        <v>3790237689</v>
       </c>
       <c r="E38" t="n">
-        <v>155813335</v>
+        <v>155893008</v>
       </c>
       <c r="F38" t="n">
-        <v>0.70825</v>
+        <v>1.53851</v>
       </c>
     </row>
     <row r="39">
@@ -1367,16 +1367,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>509.73</v>
+        <v>510.19</v>
       </c>
       <c r="D39" t="n">
-        <v>3763333252</v>
+        <v>3755619000</v>
       </c>
       <c r="E39" t="n">
-        <v>288200562</v>
+        <v>288147466</v>
       </c>
       <c r="F39" t="n">
-        <v>4.82107</v>
+        <v>6.01131</v>
       </c>
     </row>
     <row r="40">
@@ -1391,16 +1391,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.467259</v>
+        <v>0.470041</v>
       </c>
       <c r="D40" t="n">
-        <v>3724428423</v>
+        <v>3732725346</v>
       </c>
       <c r="E40" t="n">
-        <v>473813459</v>
+        <v>477379599</v>
       </c>
       <c r="F40" t="n">
-        <v>8.26056</v>
+        <v>9.45964</v>
       </c>
     </row>
     <row r="41">
@@ -1415,16 +1415,16 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1.001</v>
+        <v>1.004</v>
       </c>
       <c r="D41" t="n">
-        <v>3687567717</v>
+        <v>3687081210</v>
       </c>
       <c r="E41" t="n">
-        <v>237089640</v>
+        <v>234094476</v>
       </c>
       <c r="F41" t="n">
-        <v>-0.17128</v>
+        <v>0.20564</v>
       </c>
     </row>
     <row r="42">
@@ -1439,16 +1439,16 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>24.78</v>
+        <v>24.82</v>
       </c>
       <c r="D42" t="n">
-        <v>3573423906</v>
+        <v>3568902481</v>
       </c>
       <c r="E42" t="n">
-        <v>38290921</v>
+        <v>42268168</v>
       </c>
       <c r="F42" t="n">
-        <v>2.73603</v>
+        <v>3.171</v>
       </c>
     </row>
     <row r="43">
@@ -1463,16 +1463,16 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>3.91</v>
+        <v>3.87</v>
       </c>
       <c r="D43" t="n">
-        <v>3529178084</v>
+        <v>3509830666</v>
       </c>
       <c r="E43" t="n">
-        <v>306842077</v>
+        <v>307919878</v>
       </c>
       <c r="F43" t="n">
-        <v>6.83721</v>
+        <v>7.07413</v>
       </c>
     </row>
     <row r="44">
@@ -1487,16 +1487,16 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.999465</v>
+        <v>1.001</v>
       </c>
       <c r="D44" t="n">
-        <v>3441616760</v>
+        <v>3437170730</v>
       </c>
       <c r="E44" t="n">
-        <v>163474938</v>
+        <v>162604667</v>
       </c>
       <c r="F44" t="n">
-        <v>-0.28609</v>
+        <v>0.09223000000000001</v>
       </c>
     </row>
     <row r="45">
@@ -1511,16 +1511,16 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3.37</v>
+        <v>3.39</v>
       </c>
       <c r="D45" t="n">
-        <v>3367531542</v>
+        <v>3376536344</v>
       </c>
       <c r="E45" t="n">
-        <v>1269991304</v>
+        <v>1277498925</v>
       </c>
       <c r="F45" t="n">
-        <v>8.123480000000001</v>
+        <v>9.75545</v>
       </c>
     </row>
     <row r="46">
@@ -1535,16 +1535,16 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1.28</v>
+        <v>1.29</v>
       </c>
       <c r="D46" t="n">
-        <v>3343687076</v>
+        <v>3350856732</v>
       </c>
       <c r="E46" t="n">
-        <v>496379708</v>
+        <v>496633305</v>
       </c>
       <c r="F46" t="n">
-        <v>4.92834</v>
+        <v>6.08043</v>
       </c>
     </row>
     <row r="47">
@@ -1559,16 +1559,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.773817</v>
+        <v>0.77889</v>
       </c>
       <c r="D47" t="n">
-        <v>3171101048</v>
+        <v>3189387025</v>
       </c>
       <c r="E47" t="n">
-        <v>1667534686</v>
+        <v>1680163823</v>
       </c>
       <c r="F47" t="n">
-        <v>14.03529</v>
+        <v>15.18927</v>
       </c>
     </row>
     <row r="48">
@@ -1583,16 +1583,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>160.25</v>
+        <v>160.55</v>
       </c>
       <c r="D48" t="n">
-        <v>2957759868</v>
+        <v>2960163016</v>
       </c>
       <c r="E48" t="n">
-        <v>84034592</v>
+        <v>83785159</v>
       </c>
       <c r="F48" t="n">
-        <v>-1.14394</v>
+        <v>-0.64177</v>
       </c>
     </row>
     <row r="49">
@@ -1607,16 +1607,16 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1.94</v>
+        <v>1.95</v>
       </c>
       <c r="D49" t="n">
-        <v>2918415642</v>
+        <v>2930298939</v>
       </c>
       <c r="E49" t="n">
-        <v>422364809</v>
+        <v>407497415</v>
       </c>
       <c r="F49" t="n">
-        <v>2.84764</v>
+        <v>4.39563</v>
       </c>
     </row>
     <row r="50">
@@ -1631,16 +1631,16 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>4.67</v>
+        <v>4.7</v>
       </c>
       <c r="D50" t="n">
-        <v>2805339303</v>
+        <v>2810230521</v>
       </c>
       <c r="E50" t="n">
-        <v>584722236</v>
+        <v>589963526</v>
       </c>
       <c r="F50" t="n">
-        <v>8.904389999999999</v>
+        <v>10.18223</v>
       </c>
     </row>
     <row r="51">
@@ -1655,16 +1655,16 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>46.56</v>
+        <v>46.64</v>
       </c>
       <c r="D51" t="n">
-        <v>2795155174</v>
+        <v>2798490620</v>
       </c>
       <c r="E51" t="n">
-        <v>20372276</v>
+        <v>20268743</v>
       </c>
       <c r="F51" t="n">
-        <v>6.04536</v>
+        <v>6.34523</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1959097766308</v>
+        <v>1957894470032</v>
       </c>
     </row>
     <row r="3">
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>405800320131</v>
+        <v>406862764584</v>
       </c>
     </row>
     <row r="4">
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>130852749175</v>
+        <v>130949157622</v>
       </c>
     </row>
     <row r="5">
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>124608104880</v>
+        <v>124220173708</v>
       </c>
     </row>
     <row r="6">
@@ -1745,7 +1745,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>92807675426</v>
+        <v>92659978087</v>
       </c>
     </row>
   </sheetData>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$4350.40</t>
+          <t>$4356.86</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>XRP (27.87%)</t>
+          <t>XRP (29.46%)</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Monero (-1.14%)</t>
+          <t>Monero (-0.64%)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Excel data - 2024-11-22 04:36:14
</commit_message>
<xml_diff>
--- a/crypto_live_data.xlsx
+++ b/crypto_live_data.xlsx
@@ -479,16 +479,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>99002</v>
+        <v>98971</v>
       </c>
       <c r="D2" t="n">
-        <v>1957894470032</v>
+        <v>1958688961585</v>
       </c>
       <c r="E2" t="n">
-        <v>118089762693</v>
+        <v>90706112783</v>
       </c>
       <c r="F2" t="n">
-        <v>2.41144</v>
+        <v>2.72787</v>
       </c>
     </row>
     <row r="3">
@@ -503,16 +503,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3381.18</v>
+        <v>3414.69</v>
       </c>
       <c r="D3" t="n">
-        <v>406862764584</v>
+        <v>409915509517</v>
       </c>
       <c r="E3" t="n">
-        <v>57938597348</v>
+        <v>58463062946</v>
       </c>
       <c r="F3" t="n">
-        <v>9.056800000000001</v>
+        <v>9.616110000000001</v>
       </c>
     </row>
     <row r="4">
@@ -527,16 +527,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.002</v>
+        <v>1.001</v>
       </c>
       <c r="D4" t="n">
-        <v>130949157622</v>
+        <v>130869523334</v>
       </c>
       <c r="E4" t="n">
-        <v>173551742236</v>
+        <v>144923567712</v>
       </c>
       <c r="F4" t="n">
-        <v>0.11938</v>
+        <v>0.16594</v>
       </c>
     </row>
     <row r="5">
@@ -551,16 +551,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>262.44</v>
+        <v>261.97</v>
       </c>
       <c r="D5" t="n">
-        <v>124220173708</v>
+        <v>124533585904</v>
       </c>
       <c r="E5" t="n">
-        <v>15298491107</v>
+        <v>14798492535</v>
       </c>
       <c r="F5" t="n">
-        <v>10.80211</v>
+        <v>10.07209</v>
       </c>
     </row>
     <row r="6">
@@ -575,16 +575,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>635.4</v>
+        <v>635.71</v>
       </c>
       <c r="D6" t="n">
-        <v>92659978087</v>
+        <v>92659855271</v>
       </c>
       <c r="E6" t="n">
-        <v>2511013877</v>
+        <v>2505513002</v>
       </c>
       <c r="F6" t="n">
-        <v>5.36731</v>
+        <v>5.36418</v>
       </c>
     </row>
     <row r="7">
@@ -599,16 +599,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.42</v>
+        <v>1.4</v>
       </c>
       <c r="D7" t="n">
-        <v>80591370672</v>
+        <v>80057199926</v>
       </c>
       <c r="E7" t="n">
-        <v>17643086232</v>
+        <v>17726236905</v>
       </c>
       <c r="F7" t="n">
-        <v>29.46279</v>
+        <v>27.44776</v>
       </c>
     </row>
     <row r="8">
@@ -623,16 +623,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.395552</v>
+        <v>0.395193</v>
       </c>
       <c r="D8" t="n">
-        <v>58058582415</v>
+        <v>58107129028</v>
       </c>
       <c r="E8" t="n">
-        <v>10368763281</v>
+        <v>10365661625</v>
       </c>
       <c r="F8" t="n">
-        <v>4.5807</v>
+        <v>3.48193</v>
       </c>
     </row>
     <row r="9">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1.001</v>
+        <v>0.999896</v>
       </c>
       <c r="D9" t="n">
-        <v>38260938357</v>
+        <v>38235535434</v>
       </c>
       <c r="E9" t="n">
-        <v>10560509915</v>
+        <v>14818752221</v>
       </c>
       <c r="F9" t="n">
-        <v>0.04934</v>
+        <v>0.09767000000000001</v>
       </c>
     </row>
     <row r="10">
@@ -671,16 +671,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3383.67</v>
+        <v>3413.2</v>
       </c>
       <c r="D10" t="n">
-        <v>33041881744</v>
+        <v>33428135997</v>
       </c>
       <c r="E10" t="n">
-        <v>148028738</v>
+        <v>148487025</v>
       </c>
       <c r="F10" t="n">
-        <v>9.25051</v>
+        <v>9.59801</v>
       </c>
     </row>
     <row r="11">
@@ -695,16 +695,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.891699</v>
+        <v>0.890408</v>
       </c>
       <c r="D11" t="n">
-        <v>31872011634</v>
+        <v>31913200608</v>
       </c>
       <c r="E11" t="n">
-        <v>3682783069</v>
+        <v>3611716130</v>
       </c>
       <c r="F11" t="n">
-        <v>14.8535</v>
+        <v>14.09951</v>
       </c>
     </row>
     <row r="12">
@@ -719,16 +719,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.20108</v>
+        <v>0.20109</v>
       </c>
       <c r="D12" t="n">
-        <v>17356540142</v>
+        <v>17365839559</v>
       </c>
       <c r="E12" t="n">
-        <v>1103322051</v>
+        <v>1101570407</v>
       </c>
       <c r="F12" t="n">
-        <v>2.57305</v>
+        <v>2.44591</v>
       </c>
     </row>
     <row r="13">
@@ -743,16 +743,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>36.36</v>
+        <v>36.47</v>
       </c>
       <c r="D13" t="n">
-        <v>14842131964</v>
+        <v>14930904597</v>
       </c>
       <c r="E13" t="n">
-        <v>1050149638</v>
+        <v>1055426491</v>
       </c>
       <c r="F13" t="n">
-        <v>9.352589999999999</v>
+        <v>8.78505</v>
       </c>
     </row>
     <row r="14">
@@ -767,16 +767,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.501e-05</v>
+        <v>2.507e-05</v>
       </c>
       <c r="D14" t="n">
-        <v>14692282099</v>
+        <v>14768662928</v>
       </c>
       <c r="E14" t="n">
-        <v>1619515324</v>
+        <v>1622090425</v>
       </c>
       <c r="F14" t="n">
-        <v>5.795</v>
+        <v>5.69772</v>
       </c>
     </row>
     <row r="15">
@@ -791,16 +791,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>98749</v>
+        <v>98944</v>
       </c>
       <c r="D15" t="n">
-        <v>14410037964</v>
+        <v>14459289342</v>
       </c>
       <c r="E15" t="n">
-        <v>901639215</v>
+        <v>903720736</v>
       </c>
       <c r="F15" t="n">
-        <v>2.73716</v>
+        <v>3.29476</v>
       </c>
     </row>
     <row r="16">
@@ -815,16 +815,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4000.57</v>
+        <v>4003.17</v>
       </c>
       <c r="D16" t="n">
-        <v>14392682837</v>
+        <v>14446765079</v>
       </c>
       <c r="E16" t="n">
-        <v>167702447</v>
+        <v>167820354</v>
       </c>
       <c r="F16" t="n">
-        <v>9.100989999999999</v>
+        <v>9.105029999999999</v>
       </c>
     </row>
     <row r="17">
@@ -839,16 +839,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5.56</v>
+        <v>5.57</v>
       </c>
       <c r="D17" t="n">
-        <v>14148936409</v>
+        <v>14197408302</v>
       </c>
       <c r="E17" t="n">
-        <v>619899192</v>
+        <v>626468405</v>
       </c>
       <c r="F17" t="n">
-        <v>4.88377</v>
+        <v>4.87141</v>
       </c>
     </row>
     <row r="18">
@@ -863,64 +863,64 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3.63</v>
+        <v>3.64</v>
       </c>
       <c r="D18" t="n">
-        <v>10308929159</v>
+        <v>10370586662</v>
       </c>
       <c r="E18" t="n">
-        <v>2225166820</v>
+        <v>2130512817</v>
       </c>
       <c r="F18" t="n">
-        <v>4.19795</v>
+        <v>3.49773</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>WETH</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>bch</t>
+          <t>weth</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>494.24</v>
+        <v>3411.88</v>
       </c>
       <c r="D19" t="n">
-        <v>9777605296</v>
+        <v>9816635144</v>
       </c>
       <c r="E19" t="n">
-        <v>2283872731</v>
+        <v>2314023127</v>
       </c>
       <c r="F19" t="n">
-        <v>6.40315</v>
+        <v>9.716889999999999</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>WETH</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>weth</t>
+          <t>bch</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3377.99</v>
+        <v>494.21</v>
       </c>
       <c r="D20" t="n">
-        <v>9686429221</v>
+        <v>9777189234</v>
       </c>
       <c r="E20" t="n">
-        <v>2254650087</v>
+        <v>2240429444</v>
       </c>
       <c r="F20" t="n">
-        <v>9.13232</v>
+        <v>5.43251</v>
       </c>
     </row>
     <row r="21">
@@ -935,16 +935,16 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>15.15</v>
+        <v>15.26</v>
       </c>
       <c r="D21" t="n">
-        <v>9490558072</v>
+        <v>9535373196</v>
       </c>
       <c r="E21" t="n">
-        <v>1228707366</v>
+        <v>1235242963</v>
       </c>
       <c r="F21" t="n">
-        <v>6.48594</v>
+        <v>6.50221</v>
       </c>
     </row>
     <row r="22">
@@ -959,16 +959,16 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.141e-05</v>
+        <v>2.171e-05</v>
       </c>
       <c r="D22" t="n">
-        <v>8987945059</v>
+        <v>9133951966</v>
       </c>
       <c r="E22" t="n">
-        <v>7056904336</v>
+        <v>7119159661</v>
       </c>
       <c r="F22" t="n">
-        <v>15.03015</v>
+        <v>14.42217</v>
       </c>
     </row>
     <row r="23">
@@ -983,16 +983,16 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>6.23</v>
+        <v>6.24</v>
       </c>
       <c r="D23" t="n">
-        <v>8921157612</v>
+        <v>8987217277</v>
       </c>
       <c r="E23" t="n">
-        <v>821158717</v>
+        <v>821172786</v>
       </c>
       <c r="F23" t="n">
-        <v>11.8257</v>
+        <v>11.20861</v>
       </c>
     </row>
     <row r="24">
@@ -1007,16 +1007,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.287482</v>
+        <v>0.285872</v>
       </c>
       <c r="D24" t="n">
-        <v>8619859512</v>
+        <v>8586479712</v>
       </c>
       <c r="E24" t="n">
-        <v>2353187735</v>
+        <v>2347001161</v>
       </c>
       <c r="F24" t="n">
-        <v>22.54928</v>
+        <v>21.45542</v>
       </c>
     </row>
     <row r="25">
@@ -1034,13 +1034,13 @@
         <v>8.73</v>
       </c>
       <c r="D25" t="n">
-        <v>8070751002</v>
+        <v>8073392142</v>
       </c>
       <c r="E25" t="n">
-        <v>3455613</v>
+        <v>3453877</v>
       </c>
       <c r="F25" t="n">
-        <v>2.38203</v>
+        <v>2.58685</v>
       </c>
     </row>
     <row r="26">
@@ -1055,16 +1055,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>5.8</v>
+        <v>5.85</v>
       </c>
       <c r="D26" t="n">
-        <v>7040976947</v>
+        <v>7116535637</v>
       </c>
       <c r="E26" t="n">
-        <v>1021697502</v>
+        <v>1022382381</v>
       </c>
       <c r="F26" t="n">
-        <v>7.08168</v>
+        <v>6.4557</v>
       </c>
     </row>
     <row r="27">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>90.36</v>
+        <v>90.47</v>
       </c>
       <c r="D27" t="n">
-        <v>6794019549</v>
+        <v>6802702646</v>
       </c>
       <c r="E27" t="n">
-        <v>1430474849</v>
+        <v>1425441937</v>
       </c>
       <c r="F27" t="n">
-        <v>6.60149</v>
+        <v>6.36019</v>
       </c>
     </row>
     <row r="28">
@@ -1103,16 +1103,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>12.1</v>
+        <v>12.14</v>
       </c>
       <c r="D28" t="n">
-        <v>6439611393</v>
+        <v>6472704885</v>
       </c>
       <c r="E28" t="n">
-        <v>899442878</v>
+        <v>897409636</v>
       </c>
       <c r="F28" t="n">
-        <v>6.00717</v>
+        <v>5.02701</v>
       </c>
     </row>
     <row r="29">
@@ -1127,16 +1127,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3551.03</v>
+        <v>3591.76</v>
       </c>
       <c r="D29" t="n">
-        <v>6104576415</v>
+        <v>6158488048</v>
       </c>
       <c r="E29" t="n">
-        <v>99949949</v>
+        <v>103343723</v>
       </c>
       <c r="F29" t="n">
-        <v>8.69844</v>
+        <v>10.11175</v>
       </c>
     </row>
     <row r="30">
@@ -1151,16 +1151,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9.369999999999999</v>
+        <v>9.49</v>
       </c>
       <c r="D30" t="n">
-        <v>5606275386</v>
+        <v>5685341830</v>
       </c>
       <c r="E30" t="n">
-        <v>844571896</v>
+        <v>854581222</v>
       </c>
       <c r="F30" t="n">
-        <v>8.29304</v>
+        <v>8.99269</v>
       </c>
     </row>
     <row r="31">
@@ -1175,16 +1175,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.195206</v>
+        <v>0.195381</v>
       </c>
       <c r="D31" t="n">
-        <v>5297479520</v>
+        <v>5297070073</v>
       </c>
       <c r="E31" t="n">
-        <v>115772728</v>
+        <v>116770671</v>
       </c>
       <c r="F31" t="n">
-        <v>11.89512</v>
+        <v>10.9334</v>
       </c>
     </row>
     <row r="32">
@@ -1199,16 +1199,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1</v>
+        <v>0.997246</v>
       </c>
       <c r="D32" t="n">
-        <v>5243513951</v>
+        <v>5236377315</v>
       </c>
       <c r="E32" t="n">
-        <v>15727350</v>
+        <v>91094</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.10343</v>
+        <v>-0.13942</v>
       </c>
     </row>
     <row r="33">
@@ -1223,16 +1223,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.132078</v>
+        <v>0.132292</v>
       </c>
       <c r="D33" t="n">
-        <v>5038922708</v>
+        <v>5045007831</v>
       </c>
       <c r="E33" t="n">
-        <v>855228186</v>
+        <v>870484679</v>
       </c>
       <c r="F33" t="n">
-        <v>5.7654</v>
+        <v>5.95544</v>
       </c>
     </row>
     <row r="34">
@@ -1250,13 +1250,13 @@
         <v>9.699999999999999</v>
       </c>
       <c r="D34" t="n">
-        <v>4588051994</v>
+        <v>4601900585</v>
       </c>
       <c r="E34" t="n">
-        <v>272484306</v>
+        <v>269764293</v>
       </c>
       <c r="F34" t="n">
-        <v>9.55508</v>
+        <v>8.44617</v>
       </c>
     </row>
     <row r="35">
@@ -1271,16 +1271,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>27.95</v>
+        <v>28.28</v>
       </c>
       <c r="D35" t="n">
-        <v>4176985543</v>
+        <v>4216363242</v>
       </c>
       <c r="E35" t="n">
-        <v>904902335</v>
+        <v>905292354</v>
       </c>
       <c r="F35" t="n">
-        <v>7.9547</v>
+        <v>8.049530000000001</v>
       </c>
     </row>
     <row r="36">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>5.227e-05</v>
+        <v>5.229e-05</v>
       </c>
       <c r="D36" t="n">
-        <v>3918665466</v>
+        <v>3926993569</v>
       </c>
       <c r="E36" t="n">
-        <v>1811077711</v>
+        <v>1801299053</v>
       </c>
       <c r="F36" t="n">
-        <v>8.74653</v>
+        <v>6.7522</v>
       </c>
     </row>
     <row r="37">
@@ -1319,16 +1319,16 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>7.41</v>
+        <v>7.45</v>
       </c>
       <c r="D37" t="n">
-        <v>3820237069</v>
+        <v>3853285644</v>
       </c>
       <c r="E37" t="n">
-        <v>445811950</v>
+        <v>447297571</v>
       </c>
       <c r="F37" t="n">
-        <v>2.8475</v>
+        <v>2.48477</v>
       </c>
     </row>
     <row r="38">
@@ -1343,16 +1343,16 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.150729</v>
+        <v>0.151479</v>
       </c>
       <c r="D38" t="n">
-        <v>3790237689</v>
+        <v>3820698917</v>
       </c>
       <c r="E38" t="n">
-        <v>155893008</v>
+        <v>155603978</v>
       </c>
       <c r="F38" t="n">
-        <v>1.53851</v>
+        <v>1.39954</v>
       </c>
     </row>
     <row r="39">
@@ -1367,16 +1367,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>510.19</v>
+        <v>513.33</v>
       </c>
       <c r="D39" t="n">
-        <v>3755619000</v>
+        <v>3789399208</v>
       </c>
       <c r="E39" t="n">
-        <v>288147466</v>
+        <v>287599186</v>
       </c>
       <c r="F39" t="n">
-        <v>6.01131</v>
+        <v>6.01779</v>
       </c>
     </row>
     <row r="40">
@@ -1391,16 +1391,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.470041</v>
+        <v>0.475024</v>
       </c>
       <c r="D40" t="n">
-        <v>3732725346</v>
+        <v>3775430360</v>
       </c>
       <c r="E40" t="n">
-        <v>477379599</v>
+        <v>483340643</v>
       </c>
       <c r="F40" t="n">
-        <v>9.45964</v>
+        <v>9.5351</v>
       </c>
     </row>
     <row r="41">
@@ -1415,16 +1415,16 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1.004</v>
+        <v>1.002</v>
       </c>
       <c r="D41" t="n">
-        <v>3687081210</v>
+        <v>3687437906</v>
       </c>
       <c r="E41" t="n">
-        <v>234094476</v>
+        <v>230417226</v>
       </c>
       <c r="F41" t="n">
-        <v>0.20564</v>
+        <v>0.1649</v>
       </c>
     </row>
     <row r="42">
@@ -1439,16 +1439,16 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>24.82</v>
+        <v>24.79</v>
       </c>
       <c r="D42" t="n">
-        <v>3568902481</v>
+        <v>3573536978</v>
       </c>
       <c r="E42" t="n">
-        <v>42268168</v>
+        <v>42132678</v>
       </c>
       <c r="F42" t="n">
-        <v>3.171</v>
+        <v>3.22954</v>
       </c>
     </row>
     <row r="43">
@@ -1463,16 +1463,16 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>3.87</v>
+        <v>3.84</v>
       </c>
       <c r="D43" t="n">
-        <v>3509830666</v>
+        <v>3470901788</v>
       </c>
       <c r="E43" t="n">
-        <v>307919878</v>
+        <v>307312059</v>
       </c>
       <c r="F43" t="n">
-        <v>7.07413</v>
+        <v>6.63508</v>
       </c>
     </row>
     <row r="44">
@@ -1487,16 +1487,16 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1.001</v>
+        <v>1</v>
       </c>
       <c r="D44" t="n">
-        <v>3437170730</v>
+        <v>3443844748</v>
       </c>
       <c r="E44" t="n">
-        <v>162604667</v>
+        <v>161352064</v>
       </c>
       <c r="F44" t="n">
-        <v>0.09223000000000001</v>
+        <v>0.29964</v>
       </c>
     </row>
     <row r="45">
@@ -1511,16 +1511,16 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3.39</v>
+        <v>3.41</v>
       </c>
       <c r="D45" t="n">
-        <v>3376536344</v>
+        <v>3403124441</v>
       </c>
       <c r="E45" t="n">
-        <v>1277498925</v>
+        <v>1289304237</v>
       </c>
       <c r="F45" t="n">
-        <v>9.75545</v>
+        <v>9.82887</v>
       </c>
     </row>
     <row r="46">
@@ -1538,13 +1538,13 @@
         <v>1.29</v>
       </c>
       <c r="D46" t="n">
-        <v>3350856732</v>
+        <v>3362395368</v>
       </c>
       <c r="E46" t="n">
-        <v>496633305</v>
+        <v>497643432</v>
       </c>
       <c r="F46" t="n">
-        <v>6.08043</v>
+        <v>5.78979</v>
       </c>
     </row>
     <row r="47">
@@ -1559,16 +1559,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.77889</v>
+        <v>0.79455</v>
       </c>
       <c r="D47" t="n">
-        <v>3189387025</v>
+        <v>3247225217</v>
       </c>
       <c r="E47" t="n">
-        <v>1680163823</v>
+        <v>1700971452</v>
       </c>
       <c r="F47" t="n">
-        <v>15.18927</v>
+        <v>15.00628</v>
       </c>
     </row>
     <row r="48">
@@ -1583,16 +1583,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>160.55</v>
+        <v>160.49</v>
       </c>
       <c r="D48" t="n">
-        <v>2960163016</v>
+        <v>2959603040</v>
       </c>
       <c r="E48" t="n">
-        <v>83785159</v>
+        <v>83651753</v>
       </c>
       <c r="F48" t="n">
-        <v>-0.64177</v>
+        <v>-0.51831</v>
       </c>
     </row>
     <row r="49">
@@ -1607,16 +1607,16 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1.95</v>
+        <v>1.96</v>
       </c>
       <c r="D49" t="n">
-        <v>2930298939</v>
+        <v>2947490991</v>
       </c>
       <c r="E49" t="n">
-        <v>407497415</v>
+        <v>398272260</v>
       </c>
       <c r="F49" t="n">
-        <v>4.39563</v>
+        <v>4.18586</v>
       </c>
     </row>
     <row r="50">
@@ -1631,16 +1631,16 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>4.7</v>
+        <v>4.71</v>
       </c>
       <c r="D50" t="n">
-        <v>2810230521</v>
+        <v>2827521355</v>
       </c>
       <c r="E50" t="n">
-        <v>589963526</v>
+        <v>590206830</v>
       </c>
       <c r="F50" t="n">
-        <v>10.18223</v>
+        <v>9.32207</v>
       </c>
     </row>
     <row r="51">
@@ -1655,16 +1655,16 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>46.64</v>
+        <v>46.75</v>
       </c>
       <c r="D51" t="n">
-        <v>2798490620</v>
+        <v>2799927722</v>
       </c>
       <c r="E51" t="n">
-        <v>20268743</v>
+        <v>20401183</v>
       </c>
       <c r="F51" t="n">
-        <v>6.34523</v>
+        <v>6.80962</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1957894470032</v>
+        <v>1958688961585</v>
       </c>
     </row>
     <row r="3">
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>406862764584</v>
+        <v>409915509517</v>
       </c>
     </row>
     <row r="4">
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>130949157622</v>
+        <v>130869523334</v>
       </c>
     </row>
     <row r="5">
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>124220173708</v>
+        <v>124533585904</v>
       </c>
     </row>
     <row r="6">
@@ -1745,7 +1745,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>92659978087</v>
+        <v>92659855271</v>
       </c>
     </row>
   </sheetData>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$4356.86</t>
+          <t>$4363.03</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>XRP (29.46%)</t>
+          <t>XRP (27.45%)</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Monero (-0.64%)</t>
+          <t>Monero (-0.52%)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Excel data - 2024-11-22 04:46:16
</commit_message>
<xml_diff>
--- a/crypto_live_data.xlsx
+++ b/crypto_live_data.xlsx
@@ -479,16 +479,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>98971</v>
+        <v>99149</v>
       </c>
       <c r="D2" t="n">
-        <v>1958688961585</v>
+        <v>1961769311574</v>
       </c>
       <c r="E2" t="n">
-        <v>90706112783</v>
+        <v>98540898109</v>
       </c>
       <c r="F2" t="n">
-        <v>2.72787</v>
+        <v>2.39324</v>
       </c>
     </row>
     <row r="3">
@@ -503,16 +503,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3414.69</v>
+        <v>3414.08</v>
       </c>
       <c r="D3" t="n">
-        <v>409915509517</v>
+        <v>411523313271</v>
       </c>
       <c r="E3" t="n">
-        <v>58463062946</v>
+        <v>55309814282</v>
       </c>
       <c r="F3" t="n">
-        <v>9.616110000000001</v>
+        <v>8.865119999999999</v>
       </c>
     </row>
     <row r="4">
@@ -527,16 +527,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.001</v>
+        <v>1.002</v>
       </c>
       <c r="D4" t="n">
-        <v>130869523334</v>
+        <v>130924741778</v>
       </c>
       <c r="E4" t="n">
-        <v>144923567712</v>
+        <v>105189143813</v>
       </c>
       <c r="F4" t="n">
-        <v>0.16594</v>
+        <v>-0.00751</v>
       </c>
     </row>
     <row r="5">
@@ -551,16 +551,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>261.97</v>
+        <v>261.82</v>
       </c>
       <c r="D5" t="n">
-        <v>124533585904</v>
+        <v>124291615827</v>
       </c>
       <c r="E5" t="n">
-        <v>14798492535</v>
+        <v>15188480023</v>
       </c>
       <c r="F5" t="n">
-        <v>10.07209</v>
+        <v>8.75882</v>
       </c>
     </row>
     <row r="6">
@@ -575,16 +575,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>635.71</v>
+        <v>635.84</v>
       </c>
       <c r="D6" t="n">
-        <v>92659855271</v>
+        <v>92854694727</v>
       </c>
       <c r="E6" t="n">
-        <v>2505513002</v>
+        <v>2507906945</v>
       </c>
       <c r="F6" t="n">
-        <v>5.36418</v>
+        <v>4.3857</v>
       </c>
     </row>
     <row r="7">
@@ -602,13 +602,13 @@
         <v>1.4</v>
       </c>
       <c r="D7" t="n">
-        <v>80057199926</v>
+        <v>79880606217</v>
       </c>
       <c r="E7" t="n">
-        <v>17726236905</v>
+        <v>17813777637</v>
       </c>
       <c r="F7" t="n">
-        <v>27.44776</v>
+        <v>26.04755</v>
       </c>
     </row>
     <row r="8">
@@ -623,16 +623,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.395193</v>
+        <v>0.396717</v>
       </c>
       <c r="D8" t="n">
-        <v>58107129028</v>
+        <v>58283012455</v>
       </c>
       <c r="E8" t="n">
-        <v>10365661625</v>
+        <v>10244606719</v>
       </c>
       <c r="F8" t="n">
-        <v>3.48193</v>
+        <v>2.18157</v>
       </c>
     </row>
     <row r="9">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.999896</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>38235535434</v>
+        <v>38326204577</v>
       </c>
       <c r="E9" t="n">
-        <v>14818752221</v>
+        <v>15125096053</v>
       </c>
       <c r="F9" t="n">
-        <v>0.09767000000000001</v>
+        <v>-0.09701</v>
       </c>
     </row>
     <row r="10">
@@ -671,16 +671,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3413.2</v>
+        <v>3412.1</v>
       </c>
       <c r="D10" t="n">
-        <v>33428135997</v>
+        <v>33430993756</v>
       </c>
       <c r="E10" t="n">
-        <v>148487025</v>
+        <v>147143004</v>
       </c>
       <c r="F10" t="n">
-        <v>9.59801</v>
+        <v>8.99408</v>
       </c>
     </row>
     <row r="11">
@@ -695,16 +695,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.890408</v>
+        <v>0.8925380000000001</v>
       </c>
       <c r="D11" t="n">
-        <v>31913200608</v>
+        <v>31989342572</v>
       </c>
       <c r="E11" t="n">
-        <v>3611716130</v>
+        <v>2843145921</v>
       </c>
       <c r="F11" t="n">
-        <v>14.09951</v>
+        <v>12.53038</v>
       </c>
     </row>
     <row r="12">
@@ -719,16 +719,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.20109</v>
+        <v>0.201062</v>
       </c>
       <c r="D12" t="n">
-        <v>17365839559</v>
+        <v>17366628805</v>
       </c>
       <c r="E12" t="n">
-        <v>1101570407</v>
+        <v>1099122463</v>
       </c>
       <c r="F12" t="n">
-        <v>2.44591</v>
+        <v>1.75848</v>
       </c>
     </row>
     <row r="13">
@@ -743,16 +743,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>36.47</v>
+        <v>36.57</v>
       </c>
       <c r="D13" t="n">
-        <v>14930904597</v>
+        <v>14963010321</v>
       </c>
       <c r="E13" t="n">
-        <v>1055426491</v>
+        <v>1052962960</v>
       </c>
       <c r="F13" t="n">
-        <v>8.78505</v>
+        <v>7.13683</v>
       </c>
     </row>
     <row r="14">
@@ -767,64 +767,64 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.507e-05</v>
+        <v>2.514e-05</v>
       </c>
       <c r="D14" t="n">
-        <v>14768662928</v>
+        <v>14817582167</v>
       </c>
       <c r="E14" t="n">
-        <v>1622090425</v>
+        <v>1622034870</v>
       </c>
       <c r="F14" t="n">
-        <v>5.69772</v>
+        <v>4.32907</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Wrapped stETH</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>wbtc</t>
+          <t>wsteth</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>98944</v>
+        <v>4010.15</v>
       </c>
       <c r="D15" t="n">
-        <v>14459289342</v>
+        <v>14476726400</v>
       </c>
       <c r="E15" t="n">
-        <v>903720736</v>
+        <v>166791664</v>
       </c>
       <c r="F15" t="n">
-        <v>3.29476</v>
+        <v>8.59362</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Wrapped stETH</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>wsteth</t>
+          <t>wbtc</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4003.17</v>
+        <v>98631</v>
       </c>
       <c r="D16" t="n">
-        <v>14446765079</v>
+        <v>14410603666</v>
       </c>
       <c r="E16" t="n">
-        <v>167820354</v>
+        <v>886179449</v>
       </c>
       <c r="F16" t="n">
-        <v>9.105029999999999</v>
+        <v>2.50796</v>
       </c>
     </row>
     <row r="17">
@@ -839,16 +839,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5.57</v>
+        <v>5.59</v>
       </c>
       <c r="D17" t="n">
-        <v>14197408302</v>
+        <v>14218996814</v>
       </c>
       <c r="E17" t="n">
-        <v>626468405</v>
+        <v>630148511</v>
       </c>
       <c r="F17" t="n">
-        <v>4.87141</v>
+        <v>4.15114</v>
       </c>
     </row>
     <row r="18">
@@ -866,61 +866,61 @@
         <v>3.64</v>
       </c>
       <c r="D18" t="n">
-        <v>10370586662</v>
+        <v>10374254368</v>
       </c>
       <c r="E18" t="n">
-        <v>2130512817</v>
+        <v>2412961752</v>
       </c>
       <c r="F18" t="n">
-        <v>3.49773</v>
+        <v>0.9307</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>WETH</t>
+          <t>Bitcoin Cash</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>weth</t>
+          <t>bch</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3411.88</v>
+        <v>496.39</v>
       </c>
       <c r="D19" t="n">
-        <v>9816635144</v>
+        <v>9814281450</v>
       </c>
       <c r="E19" t="n">
-        <v>2314023127</v>
+        <v>2241782063</v>
       </c>
       <c r="F19" t="n">
-        <v>9.716889999999999</v>
+        <v>4.02434</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Bitcoin Cash</t>
+          <t>WETH</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>bch</t>
+          <t>weth</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>494.21</v>
+        <v>3414.38</v>
       </c>
       <c r="D20" t="n">
-        <v>9777189234</v>
+        <v>9729290944</v>
       </c>
       <c r="E20" t="n">
-        <v>2240429444</v>
+        <v>1145242149</v>
       </c>
       <c r="F20" t="n">
-        <v>5.43251</v>
+        <v>9.15644</v>
       </c>
     </row>
     <row r="21">
@@ -935,16 +935,16 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>15.26</v>
+        <v>15.37</v>
       </c>
       <c r="D21" t="n">
-        <v>9535373196</v>
+        <v>9636166601</v>
       </c>
       <c r="E21" t="n">
-        <v>1235242963</v>
+        <v>1249094715</v>
       </c>
       <c r="F21" t="n">
-        <v>6.50221</v>
+        <v>6.17806</v>
       </c>
     </row>
     <row r="22">
@@ -959,16 +959,16 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.171e-05</v>
+        <v>2.149e-05</v>
       </c>
       <c r="D22" t="n">
-        <v>9133951966</v>
+        <v>9079218772</v>
       </c>
       <c r="E22" t="n">
-        <v>7119159661</v>
+        <v>7071683603</v>
       </c>
       <c r="F22" t="n">
-        <v>14.42217</v>
+        <v>10.8927</v>
       </c>
     </row>
     <row r="23">
@@ -983,16 +983,16 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>6.24</v>
+        <v>6.26</v>
       </c>
       <c r="D23" t="n">
-        <v>8987217277</v>
+        <v>9008856710</v>
       </c>
       <c r="E23" t="n">
-        <v>821172786</v>
+        <v>821046539</v>
       </c>
       <c r="F23" t="n">
-        <v>11.20861</v>
+        <v>9.63602</v>
       </c>
     </row>
     <row r="24">
@@ -1007,16 +1007,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.285872</v>
+        <v>0.288277</v>
       </c>
       <c r="D24" t="n">
-        <v>8586479712</v>
+        <v>8632018977</v>
       </c>
       <c r="E24" t="n">
-        <v>2347001161</v>
+        <v>2350324462</v>
       </c>
       <c r="F24" t="n">
-        <v>21.45542</v>
+        <v>20.85285</v>
       </c>
     </row>
     <row r="25">
@@ -1031,16 +1031,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>8.73</v>
+        <v>8.76</v>
       </c>
       <c r="D25" t="n">
-        <v>8073392142</v>
+        <v>8097734319</v>
       </c>
       <c r="E25" t="n">
-        <v>3453877</v>
+        <v>3467097</v>
       </c>
       <c r="F25" t="n">
-        <v>2.58685</v>
+        <v>2.69848</v>
       </c>
     </row>
     <row r="26">
@@ -1058,13 +1058,13 @@
         <v>5.85</v>
       </c>
       <c r="D26" t="n">
-        <v>7116535637</v>
+        <v>7124913275</v>
       </c>
       <c r="E26" t="n">
-        <v>1022382381</v>
+        <v>1016659437</v>
       </c>
       <c r="F26" t="n">
-        <v>6.4557</v>
+        <v>4.39655</v>
       </c>
     </row>
     <row r="27">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>90.47</v>
+        <v>91.06999999999999</v>
       </c>
       <c r="D27" t="n">
-        <v>6802702646</v>
+        <v>6847657317</v>
       </c>
       <c r="E27" t="n">
-        <v>1425441937</v>
+        <v>1465484425</v>
       </c>
       <c r="F27" t="n">
-        <v>6.36019</v>
+        <v>5.62763</v>
       </c>
     </row>
     <row r="28">
@@ -1103,16 +1103,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>12.14</v>
+        <v>12.17</v>
       </c>
       <c r="D28" t="n">
-        <v>6472704885</v>
+        <v>6486163977</v>
       </c>
       <c r="E28" t="n">
-        <v>897409636</v>
+        <v>892733968</v>
       </c>
       <c r="F28" t="n">
-        <v>5.02701</v>
+        <v>3.53089</v>
       </c>
     </row>
     <row r="29">
@@ -1127,16 +1127,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3591.76</v>
+        <v>3556.65</v>
       </c>
       <c r="D29" t="n">
-        <v>6158488048</v>
+        <v>6189609043</v>
       </c>
       <c r="E29" t="n">
-        <v>103343723</v>
+        <v>100989166</v>
       </c>
       <c r="F29" t="n">
-        <v>10.11175</v>
+        <v>7.64083</v>
       </c>
     </row>
     <row r="30">
@@ -1151,16 +1151,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9.49</v>
+        <v>9.5</v>
       </c>
       <c r="D30" t="n">
-        <v>5685341830</v>
+        <v>5704273647</v>
       </c>
       <c r="E30" t="n">
-        <v>854581222</v>
+        <v>857998246</v>
       </c>
       <c r="F30" t="n">
-        <v>8.99269</v>
+        <v>8.047700000000001</v>
       </c>
     </row>
     <row r="31">
@@ -1175,16 +1175,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.195381</v>
+        <v>0.193386</v>
       </c>
       <c r="D31" t="n">
-        <v>5297070073</v>
+        <v>5241773560</v>
       </c>
       <c r="E31" t="n">
-        <v>116770671</v>
+        <v>116796609</v>
       </c>
       <c r="F31" t="n">
-        <v>10.9334</v>
+        <v>9.25628</v>
       </c>
     </row>
     <row r="32">
@@ -1199,16 +1199,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.997246</v>
+        <v>1.001</v>
       </c>
       <c r="D32" t="n">
-        <v>5236377315</v>
+        <v>5240540218</v>
       </c>
       <c r="E32" t="n">
-        <v>91094</v>
+        <v>16261713</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.13942</v>
+        <v>0.19536</v>
       </c>
     </row>
     <row r="33">
@@ -1223,16 +1223,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.132292</v>
+        <v>0.134935</v>
       </c>
       <c r="D33" t="n">
-        <v>5045007831</v>
+        <v>5109436515</v>
       </c>
       <c r="E33" t="n">
-        <v>870484679</v>
+        <v>885897353</v>
       </c>
       <c r="F33" t="n">
-        <v>5.95544</v>
+        <v>6.79599</v>
       </c>
     </row>
     <row r="34">
@@ -1247,16 +1247,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9.699999999999999</v>
+        <v>9.77</v>
       </c>
       <c r="D34" t="n">
-        <v>4601900585</v>
+        <v>4634790671</v>
       </c>
       <c r="E34" t="n">
-        <v>269764293</v>
+        <v>273253536</v>
       </c>
       <c r="F34" t="n">
-        <v>8.44617</v>
+        <v>7.39788</v>
       </c>
     </row>
     <row r="35">
@@ -1271,16 +1271,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>28.28</v>
+        <v>28.22</v>
       </c>
       <c r="D35" t="n">
-        <v>4216363242</v>
+        <v>4223356412</v>
       </c>
       <c r="E35" t="n">
-        <v>905292354</v>
+        <v>895949110</v>
       </c>
       <c r="F35" t="n">
-        <v>8.049530000000001</v>
+        <v>7.09025</v>
       </c>
     </row>
     <row r="36">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>5.229e-05</v>
+        <v>5.249e-05</v>
       </c>
       <c r="D36" t="n">
-        <v>3926993569</v>
+        <v>3932666747</v>
       </c>
       <c r="E36" t="n">
-        <v>1801299053</v>
+        <v>1777055738</v>
       </c>
       <c r="F36" t="n">
-        <v>6.7522</v>
+        <v>4.15601</v>
       </c>
     </row>
     <row r="37">
@@ -1319,16 +1319,16 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>7.45</v>
+        <v>7.46</v>
       </c>
       <c r="D37" t="n">
-        <v>3853285644</v>
+        <v>3863154821</v>
       </c>
       <c r="E37" t="n">
-        <v>447297571</v>
+        <v>444152804</v>
       </c>
       <c r="F37" t="n">
-        <v>2.48477</v>
+        <v>1.04288</v>
       </c>
     </row>
     <row r="38">
@@ -1343,64 +1343,64 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.151479</v>
+        <v>0.150858</v>
       </c>
       <c r="D38" t="n">
-        <v>3820698917</v>
+        <v>3808781070</v>
       </c>
       <c r="E38" t="n">
-        <v>155603978</v>
+        <v>154293525</v>
       </c>
       <c r="F38" t="n">
-        <v>1.39954</v>
+        <v>-0.2823</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Bittensor</t>
+          <t>POL (ex-MATIC)</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>tao</t>
+          <t>pol</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>513.33</v>
+        <v>0.477072</v>
       </c>
       <c r="D39" t="n">
-        <v>3789399208</v>
+        <v>3802839938</v>
       </c>
       <c r="E39" t="n">
-        <v>287599186</v>
+        <v>486060217</v>
       </c>
       <c r="F39" t="n">
-        <v>6.01779</v>
+        <v>8.22479</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>POL (ex-MATIC)</t>
+          <t>Bittensor</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>pol</t>
+          <t>tao</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.475024</v>
+        <v>510.62</v>
       </c>
       <c r="D40" t="n">
-        <v>3775430360</v>
+        <v>3768031715</v>
       </c>
       <c r="E40" t="n">
-        <v>483340643</v>
+        <v>287161985</v>
       </c>
       <c r="F40" t="n">
-        <v>9.5351</v>
+        <v>4.16779</v>
       </c>
     </row>
     <row r="41">
@@ -1418,13 +1418,13 @@
         <v>1.002</v>
       </c>
       <c r="D41" t="n">
-        <v>3687437906</v>
+        <v>3689043815</v>
       </c>
       <c r="E41" t="n">
-        <v>230417226</v>
+        <v>228245435</v>
       </c>
       <c r="F41" t="n">
-        <v>0.1649</v>
+        <v>-0.08268</v>
       </c>
     </row>
     <row r="42">
@@ -1439,16 +1439,16 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>24.79</v>
+        <v>24.84</v>
       </c>
       <c r="D42" t="n">
-        <v>3573536978</v>
+        <v>3580056600</v>
       </c>
       <c r="E42" t="n">
-        <v>42132678</v>
+        <v>42172745</v>
       </c>
       <c r="F42" t="n">
-        <v>3.22954</v>
+        <v>2.81733</v>
       </c>
     </row>
     <row r="43">
@@ -1466,13 +1466,13 @@
         <v>3.84</v>
       </c>
       <c r="D43" t="n">
-        <v>3470901788</v>
+        <v>3462791802</v>
       </c>
       <c r="E43" t="n">
-        <v>307312059</v>
+        <v>305531810</v>
       </c>
       <c r="F43" t="n">
-        <v>6.63508</v>
+        <v>5.79364</v>
       </c>
     </row>
     <row r="44">
@@ -1487,16 +1487,16 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1</v>
+        <v>1.001</v>
       </c>
       <c r="D44" t="n">
-        <v>3443844748</v>
+        <v>3444417149</v>
       </c>
       <c r="E44" t="n">
-        <v>161352064</v>
+        <v>160828033</v>
       </c>
       <c r="F44" t="n">
-        <v>0.29964</v>
+        <v>-0.19239</v>
       </c>
     </row>
     <row r="45">
@@ -1514,13 +1514,13 @@
         <v>3.41</v>
       </c>
       <c r="D45" t="n">
-        <v>3403124441</v>
+        <v>3406645100</v>
       </c>
       <c r="E45" t="n">
-        <v>1289304237</v>
+        <v>1283305572</v>
       </c>
       <c r="F45" t="n">
-        <v>9.82887</v>
+        <v>5.93067</v>
       </c>
     </row>
     <row r="46">
@@ -1538,13 +1538,13 @@
         <v>1.29</v>
       </c>
       <c r="D46" t="n">
-        <v>3362395368</v>
+        <v>3367500054</v>
       </c>
       <c r="E46" t="n">
-        <v>497643432</v>
+        <v>477414502</v>
       </c>
       <c r="F46" t="n">
-        <v>5.78979</v>
+        <v>4.08397</v>
       </c>
     </row>
     <row r="47">
@@ -1559,16 +1559,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.79455</v>
+        <v>0.794326</v>
       </c>
       <c r="D47" t="n">
-        <v>3247225217</v>
+        <v>3255030415</v>
       </c>
       <c r="E47" t="n">
-        <v>1700971452</v>
+        <v>1679348260</v>
       </c>
       <c r="F47" t="n">
-        <v>15.00628</v>
+        <v>12.9665</v>
       </c>
     </row>
     <row r="48">
@@ -1583,16 +1583,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>160.49</v>
+        <v>160.74</v>
       </c>
       <c r="D48" t="n">
-        <v>2959603040</v>
+        <v>2965017866</v>
       </c>
       <c r="E48" t="n">
-        <v>83651753</v>
+        <v>86598350</v>
       </c>
       <c r="F48" t="n">
-        <v>-0.51831</v>
+        <v>-0.70978</v>
       </c>
     </row>
     <row r="49">
@@ -1610,13 +1610,13 @@
         <v>1.96</v>
       </c>
       <c r="D49" t="n">
-        <v>2947490991</v>
+        <v>2941212034</v>
       </c>
       <c r="E49" t="n">
-        <v>398272260</v>
+        <v>390052677</v>
       </c>
       <c r="F49" t="n">
-        <v>4.18586</v>
+        <v>2.29854</v>
       </c>
     </row>
     <row r="50">
@@ -1631,16 +1631,16 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>4.71</v>
+        <v>4.73</v>
       </c>
       <c r="D50" t="n">
-        <v>2827521355</v>
+        <v>2842098539</v>
       </c>
       <c r="E50" t="n">
-        <v>590206830</v>
+        <v>594063403</v>
       </c>
       <c r="F50" t="n">
-        <v>9.32207</v>
+        <v>8.51863</v>
       </c>
     </row>
     <row r="51">
@@ -1655,16 +1655,16 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>46.75</v>
+        <v>46.73</v>
       </c>
       <c r="D51" t="n">
-        <v>2799927722</v>
+        <v>2804621854</v>
       </c>
       <c r="E51" t="n">
-        <v>20401183</v>
+        <v>20202917</v>
       </c>
       <c r="F51" t="n">
-        <v>6.80962</v>
+        <v>5.99002</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1958688961585</v>
+        <v>1961769311574</v>
       </c>
     </row>
     <row r="3">
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>409915509517</v>
+        <v>411523313271</v>
       </c>
     </row>
     <row r="4">
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>130869523334</v>
+        <v>130924741778</v>
       </c>
     </row>
     <row r="5">
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>124533585904</v>
+        <v>124291615827</v>
       </c>
     </row>
     <row r="6">
@@ -1745,7 +1745,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>92659855271</v>
+        <v>92854694727</v>
       </c>
     </row>
   </sheetData>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$4363.03</t>
+          <t>$4359.79</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>XRP (27.45%)</t>
+          <t>XRP (26.05%)</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Monero (-0.52%)</t>
+          <t>Monero (-0.71%)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Excel data - 2024-11-22 05:01:19
</commit_message>
<xml_diff>
--- a/crypto_live_data.xlsx
+++ b/crypto_live_data.xlsx
@@ -479,16 +479,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>99149</v>
+        <v>98953</v>
       </c>
       <c r="D2" t="n">
-        <v>1961769311574</v>
+        <v>1960055536355</v>
       </c>
       <c r="E2" t="n">
-        <v>98540898109</v>
+        <v>117216670870</v>
       </c>
       <c r="F2" t="n">
-        <v>2.39324</v>
+        <v>2.03171</v>
       </c>
     </row>
     <row r="3">
@@ -503,16 +503,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3414.08</v>
+        <v>3405.98</v>
       </c>
       <c r="D3" t="n">
-        <v>411523313271</v>
+        <v>410371174804</v>
       </c>
       <c r="E3" t="n">
-        <v>55309814282</v>
+        <v>56012115569</v>
       </c>
       <c r="F3" t="n">
-        <v>8.865119999999999</v>
+        <v>8.61162</v>
       </c>
     </row>
     <row r="4">
@@ -527,16 +527,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.002</v>
+        <v>1.001</v>
       </c>
       <c r="D4" t="n">
-        <v>130924741778</v>
+        <v>130826999402</v>
       </c>
       <c r="E4" t="n">
-        <v>105189143813</v>
+        <v>115551101401</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.00751</v>
+        <v>-0.16443</v>
       </c>
     </row>
     <row r="5">
@@ -551,16 +551,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>261.82</v>
+        <v>261.32</v>
       </c>
       <c r="D5" t="n">
-        <v>124291615827</v>
+        <v>124152554628</v>
       </c>
       <c r="E5" t="n">
-        <v>15188480023</v>
+        <v>15095440759</v>
       </c>
       <c r="F5" t="n">
-        <v>8.75882</v>
+        <v>8.61017</v>
       </c>
     </row>
     <row r="6">
@@ -575,16 +575,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>635.84</v>
+        <v>636.05</v>
       </c>
       <c r="D6" t="n">
-        <v>92854694727</v>
+        <v>92809270596</v>
       </c>
       <c r="E6" t="n">
-        <v>2507906945</v>
+        <v>2499467256</v>
       </c>
       <c r="F6" t="n">
-        <v>4.3857</v>
+        <v>4.31081</v>
       </c>
     </row>
     <row r="7">
@@ -602,13 +602,13 @@
         <v>1.4</v>
       </c>
       <c r="D7" t="n">
-        <v>79880606217</v>
+        <v>79939690866</v>
       </c>
       <c r="E7" t="n">
-        <v>17813777637</v>
+        <v>17839941365</v>
       </c>
       <c r="F7" t="n">
-        <v>26.04755</v>
+        <v>25.65458</v>
       </c>
     </row>
     <row r="8">
@@ -623,16 +623,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.396717</v>
+        <v>0.397586</v>
       </c>
       <c r="D8" t="n">
-        <v>58283012455</v>
+        <v>58438525648</v>
       </c>
       <c r="E8" t="n">
-        <v>10244606719</v>
+        <v>10229008017</v>
       </c>
       <c r="F8" t="n">
-        <v>2.18157</v>
+        <v>2.55081</v>
       </c>
     </row>
     <row r="9">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0.999424</v>
       </c>
       <c r="D9" t="n">
-        <v>38326204577</v>
+        <v>38293352460</v>
       </c>
       <c r="E9" t="n">
-        <v>15125096053</v>
+        <v>16171222892</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.09701</v>
+        <v>-0.19814</v>
       </c>
     </row>
     <row r="10">
@@ -671,16 +671,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3412.1</v>
+        <v>3404.14</v>
       </c>
       <c r="D10" t="n">
-        <v>33430993756</v>
+        <v>33379470053</v>
       </c>
       <c r="E10" t="n">
-        <v>147143004</v>
+        <v>148043344</v>
       </c>
       <c r="F10" t="n">
-        <v>8.99408</v>
+        <v>8.945650000000001</v>
       </c>
     </row>
     <row r="11">
@@ -695,16 +695,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.8925380000000001</v>
+        <v>0.89227</v>
       </c>
       <c r="D11" t="n">
-        <v>31989342572</v>
+        <v>31956726304</v>
       </c>
       <c r="E11" t="n">
-        <v>2843145921</v>
+        <v>3233777838</v>
       </c>
       <c r="F11" t="n">
-        <v>12.53038</v>
+        <v>11.80011</v>
       </c>
     </row>
     <row r="12">
@@ -719,16 +719,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.201062</v>
+        <v>0.200695</v>
       </c>
       <c r="D12" t="n">
-        <v>17366628805</v>
+        <v>17339715807</v>
       </c>
       <c r="E12" t="n">
-        <v>1099122463</v>
+        <v>1096809323</v>
       </c>
       <c r="F12" t="n">
-        <v>1.75848</v>
+        <v>1.56179</v>
       </c>
     </row>
     <row r="13">
@@ -743,16 +743,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>36.57</v>
+        <v>36.52</v>
       </c>
       <c r="D13" t="n">
-        <v>14963010321</v>
+        <v>14954843621</v>
       </c>
       <c r="E13" t="n">
-        <v>1052962960</v>
+        <v>1047754060</v>
       </c>
       <c r="F13" t="n">
-        <v>7.13683</v>
+        <v>6.78292</v>
       </c>
     </row>
     <row r="14">
@@ -767,16 +767,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.514e-05</v>
+        <v>2.515e-05</v>
       </c>
       <c r="D14" t="n">
-        <v>14817582167</v>
+        <v>14807481931</v>
       </c>
       <c r="E14" t="n">
-        <v>1622034870</v>
+        <v>1617812388</v>
       </c>
       <c r="F14" t="n">
-        <v>4.32907</v>
+        <v>4.32539</v>
       </c>
     </row>
     <row r="15">
@@ -791,16 +791,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>4010.15</v>
+        <v>4005.5</v>
       </c>
       <c r="D15" t="n">
-        <v>14476726400</v>
+        <v>14464595442</v>
       </c>
       <c r="E15" t="n">
-        <v>166791664</v>
+        <v>167440045</v>
       </c>
       <c r="F15" t="n">
-        <v>8.59362</v>
+        <v>7.863</v>
       </c>
     </row>
     <row r="16">
@@ -815,16 +815,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>98631</v>
+        <v>98855</v>
       </c>
       <c r="D16" t="n">
-        <v>14410603666</v>
+        <v>14370685455</v>
       </c>
       <c r="E16" t="n">
-        <v>886179449</v>
+        <v>855965571</v>
       </c>
       <c r="F16" t="n">
-        <v>2.50796</v>
+        <v>2.29304</v>
       </c>
     </row>
     <row r="17">
@@ -842,13 +842,13 @@
         <v>5.59</v>
       </c>
       <c r="D17" t="n">
-        <v>14218996814</v>
+        <v>14225472670</v>
       </c>
       <c r="E17" t="n">
-        <v>630148511</v>
+        <v>631030859</v>
       </c>
       <c r="F17" t="n">
-        <v>4.15114</v>
+        <v>4.16661</v>
       </c>
     </row>
     <row r="18">
@@ -866,13 +866,13 @@
         <v>3.64</v>
       </c>
       <c r="D18" t="n">
-        <v>10374254368</v>
+        <v>10349961705</v>
       </c>
       <c r="E18" t="n">
-        <v>2412961752</v>
+        <v>2382450464</v>
       </c>
       <c r="F18" t="n">
-        <v>0.9307</v>
+        <v>1.06058</v>
       </c>
     </row>
     <row r="19">
@@ -887,16 +887,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>496.39</v>
+        <v>497.01</v>
       </c>
       <c r="D19" t="n">
-        <v>9814281450</v>
+        <v>9844997186</v>
       </c>
       <c r="E19" t="n">
-        <v>2241782063</v>
+        <v>2191495355</v>
       </c>
       <c r="F19" t="n">
-        <v>4.02434</v>
+        <v>1.75481</v>
       </c>
     </row>
     <row r="20">
@@ -911,16 +911,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3414.38</v>
+        <v>3405.53</v>
       </c>
       <c r="D20" t="n">
-        <v>9729290944</v>
+        <v>9710866412</v>
       </c>
       <c r="E20" t="n">
-        <v>1145242149</v>
+        <v>2043740645</v>
       </c>
       <c r="F20" t="n">
-        <v>9.15644</v>
+        <v>8.840859999999999</v>
       </c>
     </row>
     <row r="21">
@@ -935,64 +935,64 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>15.37</v>
+        <v>15.34</v>
       </c>
       <c r="D21" t="n">
-        <v>9636166601</v>
+        <v>9630736423</v>
       </c>
       <c r="E21" t="n">
-        <v>1249094715</v>
+        <v>1247912196</v>
       </c>
       <c r="F21" t="n">
-        <v>6.17806</v>
+        <v>5.66124</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>pepe</t>
+          <t>dot</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.149e-05</v>
+        <v>6.25</v>
       </c>
       <c r="D22" t="n">
-        <v>9079218772</v>
+        <v>9011225759</v>
       </c>
       <c r="E22" t="n">
-        <v>7071683603</v>
+        <v>820684345</v>
       </c>
       <c r="F22" t="n">
-        <v>10.8927</v>
+        <v>9.504149999999999</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>dot</t>
+          <t>pepe</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>6.26</v>
+        <v>2.14e-05</v>
       </c>
       <c r="D23" t="n">
-        <v>9008856710</v>
+        <v>8995247135</v>
       </c>
       <c r="E23" t="n">
-        <v>821046539</v>
+        <v>7004707459</v>
       </c>
       <c r="F23" t="n">
-        <v>9.63602</v>
+        <v>9.67314</v>
       </c>
     </row>
     <row r="24">
@@ -1007,16 +1007,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.288277</v>
+        <v>0.286757</v>
       </c>
       <c r="D24" t="n">
-        <v>8632018977</v>
+        <v>8635291214</v>
       </c>
       <c r="E24" t="n">
-        <v>2350324462</v>
+        <v>2342672074</v>
       </c>
       <c r="F24" t="n">
-        <v>20.85285</v>
+        <v>19.95186</v>
       </c>
     </row>
     <row r="25">
@@ -1031,16 +1031,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>8.76</v>
+        <v>8.779999999999999</v>
       </c>
       <c r="D25" t="n">
-        <v>8097734319</v>
+        <v>8092311033</v>
       </c>
       <c r="E25" t="n">
-        <v>3467097</v>
+        <v>3449952</v>
       </c>
       <c r="F25" t="n">
-        <v>2.69848</v>
+        <v>2.85493</v>
       </c>
     </row>
     <row r="26">
@@ -1055,16 +1055,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>5.85</v>
+        <v>5.84</v>
       </c>
       <c r="D26" t="n">
-        <v>7124913275</v>
+        <v>7113376462</v>
       </c>
       <c r="E26" t="n">
-        <v>1016659437</v>
+        <v>1011267993</v>
       </c>
       <c r="F26" t="n">
-        <v>4.39655</v>
+        <v>4.81004</v>
       </c>
     </row>
     <row r="27">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>91.06999999999999</v>
+        <v>91</v>
       </c>
       <c r="D27" t="n">
-        <v>6847657317</v>
+        <v>6853292888</v>
       </c>
       <c r="E27" t="n">
-        <v>1465484425</v>
+        <v>1455521572</v>
       </c>
       <c r="F27" t="n">
-        <v>5.62763</v>
+        <v>5.54842</v>
       </c>
     </row>
     <row r="28">
@@ -1103,16 +1103,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>12.17</v>
+        <v>12.2</v>
       </c>
       <c r="D28" t="n">
-        <v>6486163977</v>
+        <v>6501949665</v>
       </c>
       <c r="E28" t="n">
-        <v>892733968</v>
+        <v>887636727</v>
       </c>
       <c r="F28" t="n">
-        <v>3.53089</v>
+        <v>3.75529</v>
       </c>
     </row>
     <row r="29">
@@ -1127,16 +1127,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3556.65</v>
+        <v>3595.01</v>
       </c>
       <c r="D29" t="n">
-        <v>6189609043</v>
+        <v>6246701016</v>
       </c>
       <c r="E29" t="n">
-        <v>100989166</v>
+        <v>103196739</v>
       </c>
       <c r="F29" t="n">
-        <v>7.64083</v>
+        <v>9.221399999999999</v>
       </c>
     </row>
     <row r="30">
@@ -1151,16 +1151,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9.5</v>
+        <v>9.48</v>
       </c>
       <c r="D30" t="n">
-        <v>5704273647</v>
+        <v>5684456629</v>
       </c>
       <c r="E30" t="n">
-        <v>857998246</v>
+        <v>859274420</v>
       </c>
       <c r="F30" t="n">
-        <v>8.047700000000001</v>
+        <v>7.63452</v>
       </c>
     </row>
     <row r="31">
@@ -1175,16 +1175,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.193386</v>
+        <v>0.195162</v>
       </c>
       <c r="D31" t="n">
-        <v>5241773560</v>
+        <v>5275716632</v>
       </c>
       <c r="E31" t="n">
-        <v>116796609</v>
+        <v>118472792</v>
       </c>
       <c r="F31" t="n">
-        <v>9.25628</v>
+        <v>10.57972</v>
       </c>
     </row>
     <row r="32">
@@ -1199,16 +1199,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1.001</v>
+        <v>0.997936</v>
       </c>
       <c r="D32" t="n">
-        <v>5240540218</v>
+        <v>5222818939</v>
       </c>
       <c r="E32" t="n">
-        <v>16261713</v>
+        <v>16029933</v>
       </c>
       <c r="F32" t="n">
-        <v>0.19536</v>
+        <v>-0.41101</v>
       </c>
     </row>
     <row r="33">
@@ -1223,16 +1223,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.134935</v>
+        <v>0.133256</v>
       </c>
       <c r="D33" t="n">
-        <v>5109436515</v>
+        <v>5116781830</v>
       </c>
       <c r="E33" t="n">
-        <v>885897353</v>
+        <v>887310034</v>
       </c>
       <c r="F33" t="n">
-        <v>6.79599</v>
+        <v>6.06212</v>
       </c>
     </row>
     <row r="34">
@@ -1247,16 +1247,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9.77</v>
+        <v>9.73</v>
       </c>
       <c r="D34" t="n">
-        <v>4634790671</v>
+        <v>4617180476</v>
       </c>
       <c r="E34" t="n">
-        <v>273253536</v>
+        <v>271410334</v>
       </c>
       <c r="F34" t="n">
-        <v>7.39788</v>
+        <v>7.07758</v>
       </c>
     </row>
     <row r="35">
@@ -1271,16 +1271,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>28.22</v>
+        <v>28.15</v>
       </c>
       <c r="D35" t="n">
-        <v>4223356412</v>
+        <v>4216502883</v>
       </c>
       <c r="E35" t="n">
-        <v>895949110</v>
+        <v>897048293</v>
       </c>
       <c r="F35" t="n">
-        <v>7.09025</v>
+        <v>6.7889</v>
       </c>
     </row>
     <row r="36">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>5.249e-05</v>
+        <v>5.238e-05</v>
       </c>
       <c r="D36" t="n">
-        <v>3932666747</v>
+        <v>3933453185</v>
       </c>
       <c r="E36" t="n">
-        <v>1777055738</v>
+        <v>1758900842</v>
       </c>
       <c r="F36" t="n">
-        <v>4.15601</v>
+        <v>2.50637</v>
       </c>
     </row>
     <row r="37">
@@ -1319,16 +1319,16 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>7.46</v>
+        <v>7.45</v>
       </c>
       <c r="D37" t="n">
-        <v>3863154821</v>
+        <v>3856984122</v>
       </c>
       <c r="E37" t="n">
-        <v>444152804</v>
+        <v>442272348</v>
       </c>
       <c r="F37" t="n">
-        <v>1.04288</v>
+        <v>0.20977</v>
       </c>
     </row>
     <row r="38">
@@ -1343,16 +1343,16 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.150858</v>
+        <v>0.151111</v>
       </c>
       <c r="D38" t="n">
-        <v>3808781070</v>
+        <v>3808008207</v>
       </c>
       <c r="E38" t="n">
-        <v>154293525</v>
+        <v>153886307</v>
       </c>
       <c r="F38" t="n">
-        <v>-0.2823</v>
+        <v>0.23278</v>
       </c>
     </row>
     <row r="39">
@@ -1367,16 +1367,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.477072</v>
+        <v>0.475975</v>
       </c>
       <c r="D39" t="n">
-        <v>3802839938</v>
+        <v>3800453937</v>
       </c>
       <c r="E39" t="n">
-        <v>486060217</v>
+        <v>486972368</v>
       </c>
       <c r="F39" t="n">
-        <v>8.22479</v>
+        <v>7.86641</v>
       </c>
     </row>
     <row r="40">
@@ -1391,16 +1391,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>510.62</v>
+        <v>509.38</v>
       </c>
       <c r="D40" t="n">
-        <v>3768031715</v>
+        <v>3759806505</v>
       </c>
       <c r="E40" t="n">
-        <v>287161985</v>
+        <v>258992108</v>
       </c>
       <c r="F40" t="n">
-        <v>4.16779</v>
+        <v>3.4544</v>
       </c>
     </row>
     <row r="41">
@@ -1415,16 +1415,16 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1.002</v>
+        <v>1.001</v>
       </c>
       <c r="D41" t="n">
-        <v>3689043815</v>
+        <v>3686526730</v>
       </c>
       <c r="E41" t="n">
-        <v>228245435</v>
+        <v>227406327</v>
       </c>
       <c r="F41" t="n">
-        <v>-0.08268</v>
+        <v>-0.19774</v>
       </c>
     </row>
     <row r="42">
@@ -1439,64 +1439,64 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>24.84</v>
+        <v>24.8</v>
       </c>
       <c r="D42" t="n">
-        <v>3580056600</v>
+        <v>3573124265</v>
       </c>
       <c r="E42" t="n">
-        <v>42172745</v>
+        <v>38721916</v>
       </c>
       <c r="F42" t="n">
-        <v>2.81733</v>
+        <v>2.67548</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>MANTRA</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>om</t>
+          <t>dai</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>3.84</v>
+        <v>0.999326</v>
       </c>
       <c r="D43" t="n">
-        <v>3462791802</v>
+        <v>3441593689</v>
       </c>
       <c r="E43" t="n">
-        <v>305531810</v>
+        <v>160724019</v>
       </c>
       <c r="F43" t="n">
-        <v>5.79364</v>
+        <v>-0.22204</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>MANTRA</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>dai</t>
+          <t>om</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1.001</v>
+        <v>3.8</v>
       </c>
       <c r="D44" t="n">
-        <v>3444417149</v>
+        <v>3435649852</v>
       </c>
       <c r="E44" t="n">
-        <v>160828033</v>
+        <v>305465958</v>
       </c>
       <c r="F44" t="n">
-        <v>-0.19239</v>
+        <v>4.68595</v>
       </c>
     </row>
     <row r="45">
@@ -1511,16 +1511,16 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3.41</v>
+        <v>3.4</v>
       </c>
       <c r="D45" t="n">
-        <v>3406645100</v>
+        <v>3397265421</v>
       </c>
       <c r="E45" t="n">
-        <v>1283305572</v>
+        <v>1279552228</v>
       </c>
       <c r="F45" t="n">
-        <v>5.93067</v>
+        <v>5.6871</v>
       </c>
     </row>
     <row r="46">
@@ -1538,13 +1538,13 @@
         <v>1.29</v>
       </c>
       <c r="D46" t="n">
-        <v>3367500054</v>
+        <v>3360582858</v>
       </c>
       <c r="E46" t="n">
-        <v>477414502</v>
+        <v>476746349</v>
       </c>
       <c r="F46" t="n">
-        <v>4.08397</v>
+        <v>3.77132</v>
       </c>
     </row>
     <row r="47">
@@ -1559,16 +1559,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.794326</v>
+        <v>0.793611</v>
       </c>
       <c r="D47" t="n">
-        <v>3255030415</v>
+        <v>3252551349</v>
       </c>
       <c r="E47" t="n">
-        <v>1679348260</v>
+        <v>1697016111</v>
       </c>
       <c r="F47" t="n">
-        <v>12.9665</v>
+        <v>12.86694</v>
       </c>
     </row>
     <row r="48">
@@ -1583,16 +1583,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>160.74</v>
+        <v>160.53</v>
       </c>
       <c r="D48" t="n">
-        <v>2965017866</v>
+        <v>2961967862</v>
       </c>
       <c r="E48" t="n">
-        <v>86598350</v>
+        <v>84034398</v>
       </c>
       <c r="F48" t="n">
-        <v>-0.70978</v>
+        <v>-1.04901</v>
       </c>
     </row>
     <row r="49">
@@ -1610,13 +1610,13 @@
         <v>1.96</v>
       </c>
       <c r="D49" t="n">
-        <v>2941212034</v>
+        <v>2938800555</v>
       </c>
       <c r="E49" t="n">
-        <v>390052677</v>
+        <v>385861546</v>
       </c>
       <c r="F49" t="n">
-        <v>2.29854</v>
+        <v>1.97972</v>
       </c>
     </row>
     <row r="50">
@@ -1631,16 +1631,16 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>4.73</v>
+        <v>4.72</v>
       </c>
       <c r="D50" t="n">
-        <v>2842098539</v>
+        <v>2837726335</v>
       </c>
       <c r="E50" t="n">
-        <v>594063403</v>
+        <v>592441880</v>
       </c>
       <c r="F50" t="n">
-        <v>8.51863</v>
+        <v>8.15019</v>
       </c>
     </row>
     <row r="51">
@@ -1658,13 +1658,13 @@
         <v>46.73</v>
       </c>
       <c r="D51" t="n">
-        <v>2804621854</v>
+        <v>2806970427</v>
       </c>
       <c r="E51" t="n">
-        <v>20202917</v>
+        <v>20013929</v>
       </c>
       <c r="F51" t="n">
-        <v>5.99002</v>
+        <v>5.40261</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1961769311574</v>
+        <v>1960055536355</v>
       </c>
     </row>
     <row r="3">
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>411523313271</v>
+        <v>410371174804</v>
       </c>
     </row>
     <row r="4">
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>130924741778</v>
+        <v>130826999402</v>
       </c>
     </row>
     <row r="5">
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>124291615827</v>
+        <v>124152554628</v>
       </c>
     </row>
     <row r="6">
@@ -1745,7 +1745,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>92854694727</v>
+        <v>92809270596</v>
       </c>
     </row>
   </sheetData>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$4359.79</t>
+          <t>$4360.50</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>XRP (26.05%)</t>
+          <t>XRP (25.65%)</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Monero (-0.71%)</t>
+          <t>Monero (-1.05%)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Excel data - 2024-11-22 05:06:20
</commit_message>
<xml_diff>
--- a/crypto_live_data.xlsx
+++ b/crypto_live_data.xlsx
@@ -479,16 +479,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>98953</v>
+        <v>98645</v>
       </c>
       <c r="D2" t="n">
-        <v>1960055536355</v>
+        <v>1955265453076</v>
       </c>
       <c r="E2" t="n">
-        <v>117216670870</v>
+        <v>117514916694</v>
       </c>
       <c r="F2" t="n">
-        <v>2.03171</v>
+        <v>1.34105</v>
       </c>
     </row>
     <row r="3">
@@ -503,16 +503,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3405.98</v>
+        <v>3384.98</v>
       </c>
       <c r="D3" t="n">
-        <v>410371174804</v>
+        <v>408743623550</v>
       </c>
       <c r="E3" t="n">
-        <v>56012115569</v>
+        <v>57753690385</v>
       </c>
       <c r="F3" t="n">
-        <v>8.61162</v>
+        <v>7.88246</v>
       </c>
     </row>
     <row r="4">
@@ -527,16 +527,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.001</v>
+        <v>0.9997819999999999</v>
       </c>
       <c r="D4" t="n">
-        <v>130826999402</v>
+        <v>130760277928</v>
       </c>
       <c r="E4" t="n">
-        <v>115551101401</v>
+        <v>104395714518</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.16443</v>
+        <v>-0.11895</v>
       </c>
     </row>
     <row r="5">
@@ -551,16 +551,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>261.32</v>
+        <v>260.36</v>
       </c>
       <c r="D5" t="n">
-        <v>124152554628</v>
+        <v>123643753527</v>
       </c>
       <c r="E5" t="n">
-        <v>15095440759</v>
+        <v>15001244143</v>
       </c>
       <c r="F5" t="n">
-        <v>8.61017</v>
+        <v>8.25719</v>
       </c>
     </row>
     <row r="6">
@@ -575,16 +575,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>636.05</v>
+        <v>634.42</v>
       </c>
       <c r="D6" t="n">
-        <v>92809270596</v>
+        <v>92718719024</v>
       </c>
       <c r="E6" t="n">
-        <v>2499467256</v>
+        <v>2485956984</v>
       </c>
       <c r="F6" t="n">
-        <v>4.31081</v>
+        <v>3.93616</v>
       </c>
     </row>
     <row r="7">
@@ -599,16 +599,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.4</v>
+        <v>1.39</v>
       </c>
       <c r="D7" t="n">
-        <v>79939690866</v>
+        <v>79352461642</v>
       </c>
       <c r="E7" t="n">
-        <v>17839941365</v>
+        <v>17770071804</v>
       </c>
       <c r="F7" t="n">
-        <v>25.65458</v>
+        <v>24.10278</v>
       </c>
     </row>
     <row r="8">
@@ -623,16 +623,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.397586</v>
+        <v>0.395726</v>
       </c>
       <c r="D8" t="n">
-        <v>58438525648</v>
+        <v>58339636274</v>
       </c>
       <c r="E8" t="n">
-        <v>10229008017</v>
+        <v>10048293158</v>
       </c>
       <c r="F8" t="n">
-        <v>2.55081</v>
+        <v>1.76409</v>
       </c>
     </row>
     <row r="9">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.999424</v>
+        <v>0.997682</v>
       </c>
       <c r="D9" t="n">
-        <v>38293352460</v>
+        <v>38285219460</v>
       </c>
       <c r="E9" t="n">
-        <v>16171222892</v>
+        <v>12956047852</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.19814</v>
+        <v>-0.22263</v>
       </c>
     </row>
     <row r="10">
@@ -671,16 +671,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3404.14</v>
+        <v>3382.2</v>
       </c>
       <c r="D10" t="n">
-        <v>33379470053</v>
+        <v>33158319598</v>
       </c>
       <c r="E10" t="n">
-        <v>148043344</v>
+        <v>148069164</v>
       </c>
       <c r="F10" t="n">
-        <v>8.945650000000001</v>
+        <v>7.6953</v>
       </c>
     </row>
     <row r="11">
@@ -695,16 +695,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.89227</v>
+        <v>0.891133</v>
       </c>
       <c r="D11" t="n">
-        <v>31956726304</v>
+        <v>31920708422</v>
       </c>
       <c r="E11" t="n">
-        <v>3233777838</v>
+        <v>1598277482</v>
       </c>
       <c r="F11" t="n">
-        <v>11.80011</v>
+        <v>11.93</v>
       </c>
     </row>
     <row r="12">
@@ -719,16 +719,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.200695</v>
+        <v>0.200196</v>
       </c>
       <c r="D12" t="n">
-        <v>17339715807</v>
+        <v>17321666076</v>
       </c>
       <c r="E12" t="n">
-        <v>1096809323</v>
+        <v>1081275395</v>
       </c>
       <c r="F12" t="n">
-        <v>1.56179</v>
+        <v>1.34399</v>
       </c>
     </row>
     <row r="13">
@@ -743,16 +743,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>36.52</v>
+        <v>36.35</v>
       </c>
       <c r="D13" t="n">
-        <v>14954843621</v>
+        <v>14881045882</v>
       </c>
       <c r="E13" t="n">
-        <v>1047754060</v>
+        <v>1040305471</v>
       </c>
       <c r="F13" t="n">
-        <v>6.78292</v>
+        <v>6.49239</v>
       </c>
     </row>
     <row r="14">
@@ -767,16 +767,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.515e-05</v>
+        <v>2.498e-05</v>
       </c>
       <c r="D14" t="n">
-        <v>14807481931</v>
+        <v>14733733758</v>
       </c>
       <c r="E14" t="n">
-        <v>1617812388</v>
+        <v>1620306454</v>
       </c>
       <c r="F14" t="n">
-        <v>4.32539</v>
+        <v>3.31374</v>
       </c>
     </row>
     <row r="15">
@@ -791,16 +791,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>4005.5</v>
+        <v>4016.6</v>
       </c>
       <c r="D15" t="n">
-        <v>14464595442</v>
+        <v>14529010683</v>
       </c>
       <c r="E15" t="n">
-        <v>167440045</v>
+        <v>168190824</v>
       </c>
       <c r="F15" t="n">
-        <v>7.863</v>
+        <v>7.87481</v>
       </c>
     </row>
     <row r="16">
@@ -815,16 +815,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>98855</v>
+        <v>98635</v>
       </c>
       <c r="D16" t="n">
-        <v>14370685455</v>
+        <v>14437397248</v>
       </c>
       <c r="E16" t="n">
-        <v>855965571</v>
+        <v>866759917</v>
       </c>
       <c r="F16" t="n">
-        <v>2.29304</v>
+        <v>1.49103</v>
       </c>
     </row>
     <row r="17">
@@ -839,16 +839,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5.59</v>
+        <v>5.56</v>
       </c>
       <c r="D17" t="n">
-        <v>14225472670</v>
+        <v>14202717857</v>
       </c>
       <c r="E17" t="n">
-        <v>631030859</v>
+        <v>629342951</v>
       </c>
       <c r="F17" t="n">
-        <v>4.16661</v>
+        <v>3.44887</v>
       </c>
     </row>
     <row r="18">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3.64</v>
+        <v>3.63</v>
       </c>
       <c r="D18" t="n">
-        <v>10349961705</v>
+        <v>10352847787</v>
       </c>
       <c r="E18" t="n">
-        <v>2382450464</v>
+        <v>2397340035</v>
       </c>
       <c r="F18" t="n">
-        <v>1.06058</v>
+        <v>1.18447</v>
       </c>
     </row>
     <row r="19">
@@ -887,16 +887,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>497.01</v>
+        <v>494.09</v>
       </c>
       <c r="D19" t="n">
-        <v>9844997186</v>
+        <v>9808440404</v>
       </c>
       <c r="E19" t="n">
-        <v>2191495355</v>
+        <v>2115012026</v>
       </c>
       <c r="F19" t="n">
-        <v>1.75481</v>
+        <v>-0.90611</v>
       </c>
     </row>
     <row r="20">
@@ -911,16 +911,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3405.53</v>
+        <v>3394.83</v>
       </c>
       <c r="D20" t="n">
-        <v>9710866412</v>
+        <v>9678336190</v>
       </c>
       <c r="E20" t="n">
-        <v>2043740645</v>
+        <v>2233267349</v>
       </c>
       <c r="F20" t="n">
-        <v>8.840859999999999</v>
+        <v>8.261150000000001</v>
       </c>
     </row>
     <row r="21">
@@ -935,64 +935,64 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>15.34</v>
+        <v>15.27</v>
       </c>
       <c r="D21" t="n">
-        <v>9630736423</v>
+        <v>9599024349</v>
       </c>
       <c r="E21" t="n">
-        <v>1247912196</v>
+        <v>1237471114</v>
       </c>
       <c r="F21" t="n">
-        <v>5.66124</v>
+        <v>4.81535</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>dot</t>
+          <t>pepe</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>6.25</v>
+        <v>2.119e-05</v>
       </c>
       <c r="D22" t="n">
-        <v>9011225759</v>
+        <v>8959751961</v>
       </c>
       <c r="E22" t="n">
-        <v>820684345</v>
+        <v>6872754151</v>
       </c>
       <c r="F22" t="n">
-        <v>9.504149999999999</v>
+        <v>7.53254</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>pepe</t>
+          <t>dot</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2.14e-05</v>
+        <v>6.21</v>
       </c>
       <c r="D23" t="n">
-        <v>8995247135</v>
+        <v>8947246366</v>
       </c>
       <c r="E23" t="n">
-        <v>7004707459</v>
+        <v>816079415</v>
       </c>
       <c r="F23" t="n">
-        <v>9.67314</v>
+        <v>8.464359999999999</v>
       </c>
     </row>
     <row r="24">
@@ -1007,16 +1007,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.286757</v>
+        <v>0.284789</v>
       </c>
       <c r="D24" t="n">
-        <v>8635291214</v>
+        <v>8574297810</v>
       </c>
       <c r="E24" t="n">
-        <v>2342672074</v>
+        <v>2311654284</v>
       </c>
       <c r="F24" t="n">
-        <v>19.95186</v>
+        <v>18.48765</v>
       </c>
     </row>
     <row r="25">
@@ -1034,13 +1034,13 @@
         <v>8.779999999999999</v>
       </c>
       <c r="D25" t="n">
-        <v>8092311033</v>
+        <v>8128302174</v>
       </c>
       <c r="E25" t="n">
-        <v>3449952</v>
+        <v>3417394</v>
       </c>
       <c r="F25" t="n">
-        <v>2.85493</v>
+        <v>2.61704</v>
       </c>
     </row>
     <row r="26">
@@ -1055,16 +1055,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>5.84</v>
+        <v>5.8</v>
       </c>
       <c r="D26" t="n">
-        <v>7113376462</v>
+        <v>7066502768</v>
       </c>
       <c r="E26" t="n">
-        <v>1011267993</v>
+        <v>1007516188</v>
       </c>
       <c r="F26" t="n">
-        <v>4.81004</v>
+        <v>3.93636</v>
       </c>
     </row>
     <row r="27">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>91</v>
+        <v>90.45</v>
       </c>
       <c r="D27" t="n">
-        <v>6853292888</v>
+        <v>6818543284</v>
       </c>
       <c r="E27" t="n">
-        <v>1455521572</v>
+        <v>1443342995</v>
       </c>
       <c r="F27" t="n">
-        <v>5.54842</v>
+        <v>4.38062</v>
       </c>
     </row>
     <row r="28">
@@ -1103,16 +1103,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>12.2</v>
+        <v>12.11</v>
       </c>
       <c r="D28" t="n">
-        <v>6501949665</v>
+        <v>6475051493</v>
       </c>
       <c r="E28" t="n">
-        <v>887636727</v>
+        <v>883555179</v>
       </c>
       <c r="F28" t="n">
-        <v>3.75529</v>
+        <v>3.42643</v>
       </c>
     </row>
     <row r="29">
@@ -1127,16 +1127,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3595.01</v>
+        <v>3573.41</v>
       </c>
       <c r="D29" t="n">
-        <v>6246701016</v>
+        <v>6229530875</v>
       </c>
       <c r="E29" t="n">
-        <v>103196739</v>
+        <v>103976595</v>
       </c>
       <c r="F29" t="n">
-        <v>9.221399999999999</v>
+        <v>8.2064</v>
       </c>
     </row>
     <row r="30">
@@ -1151,16 +1151,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9.48</v>
+        <v>9.4</v>
       </c>
       <c r="D30" t="n">
-        <v>5684456629</v>
+        <v>5646687307</v>
       </c>
       <c r="E30" t="n">
-        <v>859274420</v>
+        <v>858637673</v>
       </c>
       <c r="F30" t="n">
-        <v>7.63452</v>
+        <v>6.14347</v>
       </c>
     </row>
     <row r="31">
@@ -1175,16 +1175,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.195162</v>
+        <v>0.197491</v>
       </c>
       <c r="D31" t="n">
-        <v>5275716632</v>
+        <v>5359892708</v>
       </c>
       <c r="E31" t="n">
-        <v>118472792</v>
+        <v>120817872</v>
       </c>
       <c r="F31" t="n">
-        <v>10.57972</v>
+        <v>11.69802</v>
       </c>
     </row>
     <row r="32">
@@ -1199,16 +1199,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.997936</v>
+        <v>0.99435</v>
       </c>
       <c r="D32" t="n">
-        <v>5222818939</v>
+        <v>5217775415</v>
       </c>
       <c r="E32" t="n">
-        <v>16029933</v>
+        <v>16412763</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.41101</v>
+        <v>-0.56931</v>
       </c>
     </row>
     <row r="33">
@@ -1223,16 +1223,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.133256</v>
+        <v>0.133678</v>
       </c>
       <c r="D33" t="n">
-        <v>5116781830</v>
+        <v>5079959544</v>
       </c>
       <c r="E33" t="n">
-        <v>887310034</v>
+        <v>895188955</v>
       </c>
       <c r="F33" t="n">
-        <v>6.06212</v>
+        <v>5.463</v>
       </c>
     </row>
     <row r="34">
@@ -1247,16 +1247,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9.73</v>
+        <v>9.66</v>
       </c>
       <c r="D34" t="n">
-        <v>4617180476</v>
+        <v>4587010509</v>
       </c>
       <c r="E34" t="n">
-        <v>271410334</v>
+        <v>272743635</v>
       </c>
       <c r="F34" t="n">
-        <v>7.07758</v>
+        <v>6.07429</v>
       </c>
     </row>
     <row r="35">
@@ -1271,16 +1271,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>28.15</v>
+        <v>27.94</v>
       </c>
       <c r="D35" t="n">
-        <v>4216502883</v>
+        <v>4201045186</v>
       </c>
       <c r="E35" t="n">
-        <v>897048293</v>
+        <v>893965885</v>
       </c>
       <c r="F35" t="n">
-        <v>6.7889</v>
+        <v>5.76924</v>
       </c>
     </row>
     <row r="36">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>5.238e-05</v>
+        <v>5.2e-05</v>
       </c>
       <c r="D36" t="n">
-        <v>3933453185</v>
+        <v>3925070065</v>
       </c>
       <c r="E36" t="n">
-        <v>1758900842</v>
+        <v>1720283290</v>
       </c>
       <c r="F36" t="n">
-        <v>2.50637</v>
+        <v>1.33985</v>
       </c>
     </row>
     <row r="37">
@@ -1319,16 +1319,16 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>7.45</v>
+        <v>7.39</v>
       </c>
       <c r="D37" t="n">
-        <v>3856984122</v>
+        <v>3830491806</v>
       </c>
       <c r="E37" t="n">
-        <v>442272348</v>
+        <v>438574850</v>
       </c>
       <c r="F37" t="n">
-        <v>0.20977</v>
+        <v>-0.32458</v>
       </c>
     </row>
     <row r="38">
@@ -1343,16 +1343,16 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.151111</v>
+        <v>0.150778</v>
       </c>
       <c r="D38" t="n">
-        <v>3808008207</v>
+        <v>3811511501</v>
       </c>
       <c r="E38" t="n">
-        <v>153886307</v>
+        <v>153122650</v>
       </c>
       <c r="F38" t="n">
-        <v>0.23278</v>
+        <v>-0.5954</v>
       </c>
     </row>
     <row r="39">
@@ -1367,16 +1367,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.475975</v>
+        <v>0.470479</v>
       </c>
       <c r="D39" t="n">
-        <v>3800453937</v>
+        <v>3766297859</v>
       </c>
       <c r="E39" t="n">
-        <v>486972368</v>
+        <v>484661119</v>
       </c>
       <c r="F39" t="n">
-        <v>7.86641</v>
+        <v>6.56518</v>
       </c>
     </row>
     <row r="40">
@@ -1391,16 +1391,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>509.38</v>
+        <v>507.51</v>
       </c>
       <c r="D40" t="n">
-        <v>3759806505</v>
+        <v>3754446505</v>
       </c>
       <c r="E40" t="n">
-        <v>258992108</v>
+        <v>285429218</v>
       </c>
       <c r="F40" t="n">
-        <v>3.4544</v>
+        <v>2.87863</v>
       </c>
     </row>
     <row r="41">
@@ -1415,16 +1415,16 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1.001</v>
+        <v>0.999717</v>
       </c>
       <c r="D41" t="n">
-        <v>3686526730</v>
+        <v>3685665968</v>
       </c>
       <c r="E41" t="n">
-        <v>227406327</v>
+        <v>227695671</v>
       </c>
       <c r="F41" t="n">
-        <v>-0.19774</v>
+        <v>-0.3284</v>
       </c>
     </row>
     <row r="42">
@@ -1439,16 +1439,16 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>24.8</v>
+        <v>24.74</v>
       </c>
       <c r="D42" t="n">
-        <v>3573124265</v>
+        <v>3571018763</v>
       </c>
       <c r="E42" t="n">
-        <v>38721916</v>
+        <v>38464423</v>
       </c>
       <c r="F42" t="n">
-        <v>2.67548</v>
+        <v>2.19327</v>
       </c>
     </row>
     <row r="43">
@@ -1463,64 +1463,64 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.999326</v>
+        <v>0.997967</v>
       </c>
       <c r="D43" t="n">
-        <v>3441593689</v>
+        <v>3436077216</v>
       </c>
       <c r="E43" t="n">
-        <v>160724019</v>
+        <v>157037670</v>
       </c>
       <c r="F43" t="n">
-        <v>-0.22204</v>
+        <v>-0.25013</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>MANTRA</t>
+          <t>dogwifhat</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>om</t>
+          <t>wif</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>3.8</v>
+        <v>3.39</v>
       </c>
       <c r="D44" t="n">
-        <v>3435649852</v>
+        <v>3398407556</v>
       </c>
       <c r="E44" t="n">
-        <v>305465958</v>
+        <v>1279303703</v>
       </c>
       <c r="F44" t="n">
-        <v>4.68595</v>
+        <v>5.02821</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>dogwifhat</t>
+          <t>MANTRA</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>wif</t>
+          <t>om</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3.4</v>
+        <v>3.75</v>
       </c>
       <c r="D45" t="n">
-        <v>3397265421</v>
+        <v>3387528462</v>
       </c>
       <c r="E45" t="n">
-        <v>1279552228</v>
+        <v>296181418</v>
       </c>
       <c r="F45" t="n">
-        <v>5.6871</v>
+        <v>2.84473</v>
       </c>
     </row>
     <row r="46">
@@ -1535,16 +1535,16 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1.29</v>
+        <v>1.28</v>
       </c>
       <c r="D46" t="n">
-        <v>3360582858</v>
+        <v>3346685530</v>
       </c>
       <c r="E46" t="n">
-        <v>476746349</v>
+        <v>490864213</v>
       </c>
       <c r="F46" t="n">
-        <v>3.77132</v>
+        <v>2.65434</v>
       </c>
     </row>
     <row r="47">
@@ -1559,16 +1559,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.793611</v>
+        <v>0.7867</v>
       </c>
       <c r="D47" t="n">
-        <v>3252551349</v>
+        <v>3225646756</v>
       </c>
       <c r="E47" t="n">
-        <v>1697016111</v>
+        <v>1670400289</v>
       </c>
       <c r="F47" t="n">
-        <v>12.86694</v>
+        <v>11.73951</v>
       </c>
     </row>
     <row r="48">
@@ -1583,16 +1583,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>160.53</v>
+        <v>160.85</v>
       </c>
       <c r="D48" t="n">
-        <v>2961967862</v>
+        <v>2968142680</v>
       </c>
       <c r="E48" t="n">
-        <v>84034398</v>
+        <v>86572953</v>
       </c>
       <c r="F48" t="n">
-        <v>-1.04901</v>
+        <v>-1.00593</v>
       </c>
     </row>
     <row r="49">
@@ -1607,16 +1607,16 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1.96</v>
+        <v>1.95</v>
       </c>
       <c r="D49" t="n">
-        <v>2938800555</v>
+        <v>2934163039</v>
       </c>
       <c r="E49" t="n">
-        <v>385861546</v>
+        <v>380160497</v>
       </c>
       <c r="F49" t="n">
-        <v>1.97972</v>
+        <v>0.97964</v>
       </c>
     </row>
     <row r="50">
@@ -1631,16 +1631,16 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>4.72</v>
+        <v>4.69</v>
       </c>
       <c r="D50" t="n">
-        <v>2837726335</v>
+        <v>2821849071</v>
       </c>
       <c r="E50" t="n">
-        <v>592441880</v>
+        <v>588249132</v>
       </c>
       <c r="F50" t="n">
-        <v>8.15019</v>
+        <v>7.04811</v>
       </c>
     </row>
     <row r="51">
@@ -1655,16 +1655,16 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>46.73</v>
+        <v>46.63</v>
       </c>
       <c r="D51" t="n">
-        <v>2806970427</v>
+        <v>2803633244</v>
       </c>
       <c r="E51" t="n">
-        <v>20013929</v>
+        <v>19696267</v>
       </c>
       <c r="F51" t="n">
-        <v>5.40261</v>
+        <v>5.08722</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1960055536355</v>
+        <v>1955265453076</v>
       </c>
     </row>
     <row r="3">
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>410371174804</v>
+        <v>408743623550</v>
       </c>
     </row>
     <row r="4">
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>130826999402</v>
+        <v>130760277928</v>
       </c>
     </row>
     <row r="5">
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>124152554628</v>
+        <v>123643753527</v>
       </c>
     </row>
     <row r="6">
@@ -1745,7 +1745,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>92809270596</v>
+        <v>92718719024</v>
       </c>
     </row>
   </sheetData>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$4360.50</t>
+          <t>$4348.48</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>XRP (25.65%)</t>
+          <t>XRP (24.10%)</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Monero (-1.05%)</t>
+          <t>Monero (-1.01%)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Excel data - 2024-11-22 05:16:22
</commit_message>
<xml_diff>
--- a/crypto_live_data.xlsx
+++ b/crypto_live_data.xlsx
@@ -479,16 +479,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>98645</v>
+        <v>98953</v>
       </c>
       <c r="D2" t="n">
-        <v>1955265453076</v>
+        <v>1957819789649</v>
       </c>
       <c r="E2" t="n">
-        <v>117514916694</v>
+        <v>107473015554</v>
       </c>
       <c r="F2" t="n">
-        <v>1.34105</v>
+        <v>1.48841</v>
       </c>
     </row>
     <row r="3">
@@ -503,16 +503,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3384.98</v>
+        <v>3388.15</v>
       </c>
       <c r="D3" t="n">
-        <v>408743623550</v>
+        <v>408442019407</v>
       </c>
       <c r="E3" t="n">
-        <v>57753690385</v>
+        <v>55538713089</v>
       </c>
       <c r="F3" t="n">
-        <v>7.88246</v>
+        <v>7.89304</v>
       </c>
     </row>
     <row r="4">
@@ -527,16 +527,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.9997819999999999</v>
+        <v>1.001</v>
       </c>
       <c r="D4" t="n">
-        <v>130760277928</v>
+        <v>131041154867</v>
       </c>
       <c r="E4" t="n">
-        <v>104395714518</v>
+        <v>113718779050</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.11895</v>
+        <v>-0.01997</v>
       </c>
     </row>
     <row r="5">
@@ -551,16 +551,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>260.36</v>
+        <v>261.77</v>
       </c>
       <c r="D5" t="n">
-        <v>123643753527</v>
+        <v>124197184685</v>
       </c>
       <c r="E5" t="n">
-        <v>15001244143</v>
+        <v>14991831812</v>
       </c>
       <c r="F5" t="n">
-        <v>8.25719</v>
+        <v>8.79411</v>
       </c>
     </row>
     <row r="6">
@@ -575,16 +575,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>634.42</v>
+        <v>635.35</v>
       </c>
       <c r="D6" t="n">
-        <v>92718719024</v>
+        <v>92741072509</v>
       </c>
       <c r="E6" t="n">
-        <v>2485956984</v>
+        <v>2472723832</v>
       </c>
       <c r="F6" t="n">
-        <v>3.93616</v>
+        <v>3.75845</v>
       </c>
     </row>
     <row r="7">
@@ -599,16 +599,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.39</v>
+        <v>1.38</v>
       </c>
       <c r="D7" t="n">
-        <v>79352461642</v>
+        <v>79105543405</v>
       </c>
       <c r="E7" t="n">
-        <v>17770071804</v>
+        <v>17824065953</v>
       </c>
       <c r="F7" t="n">
-        <v>24.10278</v>
+        <v>23.06077</v>
       </c>
     </row>
     <row r="8">
@@ -623,16 +623,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.395726</v>
+        <v>0.396932</v>
       </c>
       <c r="D8" t="n">
-        <v>58339636274</v>
+        <v>58333135134</v>
       </c>
       <c r="E8" t="n">
-        <v>10048293158</v>
+        <v>9895261537</v>
       </c>
       <c r="F8" t="n">
-        <v>1.76409</v>
+        <v>2.05635</v>
       </c>
     </row>
     <row r="9">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.997682</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>38285219460</v>
+        <v>38340757364</v>
       </c>
       <c r="E9" t="n">
-        <v>12956047852</v>
+        <v>11657194673</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.22263</v>
+        <v>-0.0022</v>
       </c>
     </row>
     <row r="10">
@@ -671,16 +671,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3382.2</v>
+        <v>3387.77</v>
       </c>
       <c r="D10" t="n">
-        <v>33158319598</v>
+        <v>33192243452</v>
       </c>
       <c r="E10" t="n">
-        <v>148069164</v>
+        <v>145663717</v>
       </c>
       <c r="F10" t="n">
-        <v>7.6953</v>
+        <v>8.07043</v>
       </c>
     </row>
     <row r="11">
@@ -695,16 +695,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.891133</v>
+        <v>0.883266</v>
       </c>
       <c r="D11" t="n">
-        <v>31920708422</v>
+        <v>31681558093</v>
       </c>
       <c r="E11" t="n">
-        <v>1598277482</v>
+        <v>3291559390</v>
       </c>
       <c r="F11" t="n">
-        <v>11.93</v>
+        <v>10.80615</v>
       </c>
     </row>
     <row r="12">
@@ -719,16 +719,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.200196</v>
+        <v>0.200654</v>
       </c>
       <c r="D12" t="n">
-        <v>17321666076</v>
+        <v>17337756980</v>
       </c>
       <c r="E12" t="n">
-        <v>1081275395</v>
+        <v>1073293125</v>
       </c>
       <c r="F12" t="n">
-        <v>1.34399</v>
+        <v>1.51007</v>
       </c>
     </row>
     <row r="13">
@@ -743,16 +743,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>36.35</v>
+        <v>36.46</v>
       </c>
       <c r="D13" t="n">
-        <v>14881045882</v>
+        <v>14919274431</v>
       </c>
       <c r="E13" t="n">
-        <v>1040305471</v>
+        <v>1037618086</v>
       </c>
       <c r="F13" t="n">
-        <v>6.49239</v>
+        <v>6.6755</v>
       </c>
     </row>
     <row r="14">
@@ -767,16 +767,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.498e-05</v>
+        <v>2.504e-05</v>
       </c>
       <c r="D14" t="n">
-        <v>14733733758</v>
+        <v>14768327270</v>
       </c>
       <c r="E14" t="n">
-        <v>1620306454</v>
+        <v>1616021481</v>
       </c>
       <c r="F14" t="n">
-        <v>3.31374</v>
+        <v>3.28015</v>
       </c>
     </row>
     <row r="15">
@@ -791,16 +791,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>4016.6</v>
+        <v>4024.97</v>
       </c>
       <c r="D15" t="n">
-        <v>14529010683</v>
+        <v>14527190907</v>
       </c>
       <c r="E15" t="n">
-        <v>168190824</v>
+        <v>168464106</v>
       </c>
       <c r="F15" t="n">
-        <v>7.87481</v>
+        <v>7.91277</v>
       </c>
     </row>
     <row r="16">
@@ -815,16 +815,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>98635</v>
+        <v>98944</v>
       </c>
       <c r="D16" t="n">
-        <v>14437397248</v>
+        <v>14457817201</v>
       </c>
       <c r="E16" t="n">
-        <v>866759917</v>
+        <v>864190786</v>
       </c>
       <c r="F16" t="n">
-        <v>1.49103</v>
+        <v>2.04243</v>
       </c>
     </row>
     <row r="17">
@@ -839,16 +839,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5.56</v>
+        <v>5.57</v>
       </c>
       <c r="D17" t="n">
-        <v>14202717857</v>
+        <v>14197176170</v>
       </c>
       <c r="E17" t="n">
-        <v>629342951</v>
+        <v>637419627</v>
       </c>
       <c r="F17" t="n">
-        <v>3.44887</v>
+        <v>3.39082</v>
       </c>
     </row>
     <row r="18">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3.63</v>
+        <v>3.62</v>
       </c>
       <c r="D18" t="n">
-        <v>10352847787</v>
+        <v>10307866671</v>
       </c>
       <c r="E18" t="n">
-        <v>2397340035</v>
+        <v>2420681201</v>
       </c>
       <c r="F18" t="n">
-        <v>1.18447</v>
+        <v>1.06291</v>
       </c>
     </row>
     <row r="19">
@@ -887,16 +887,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>494.09</v>
+        <v>497.43</v>
       </c>
       <c r="D19" t="n">
-        <v>9808440404</v>
+        <v>9840002010</v>
       </c>
       <c r="E19" t="n">
-        <v>2115012026</v>
+        <v>2055046626</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.90611</v>
+        <v>-1.2951</v>
       </c>
     </row>
     <row r="20">
@@ -911,16 +911,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3394.83</v>
+        <v>3387.27</v>
       </c>
       <c r="D20" t="n">
-        <v>9678336190</v>
+        <v>9654793051</v>
       </c>
       <c r="E20" t="n">
-        <v>2233267349</v>
+        <v>1123693284</v>
       </c>
       <c r="F20" t="n">
-        <v>8.261150000000001</v>
+        <v>7.91282</v>
       </c>
     </row>
     <row r="21">
@@ -938,13 +938,13 @@
         <v>15.27</v>
       </c>
       <c r="D21" t="n">
-        <v>9599024349</v>
+        <v>9580085936</v>
       </c>
       <c r="E21" t="n">
-        <v>1237471114</v>
+        <v>1244740994</v>
       </c>
       <c r="F21" t="n">
-        <v>4.81535</v>
+        <v>4.26916</v>
       </c>
     </row>
     <row r="22">
@@ -959,16 +959,16 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.119e-05</v>
+        <v>2.135e-05</v>
       </c>
       <c r="D22" t="n">
-        <v>8959751961</v>
+        <v>8982335231</v>
       </c>
       <c r="E22" t="n">
-        <v>6872754151</v>
+        <v>6858230993</v>
       </c>
       <c r="F22" t="n">
-        <v>7.53254</v>
+        <v>9.116300000000001</v>
       </c>
     </row>
     <row r="23">
@@ -983,16 +983,16 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>6.21</v>
+        <v>6.23</v>
       </c>
       <c r="D23" t="n">
-        <v>8947246366</v>
+        <v>8964658656</v>
       </c>
       <c r="E23" t="n">
-        <v>816079415</v>
+        <v>818046188</v>
       </c>
       <c r="F23" t="n">
-        <v>8.464359999999999</v>
+        <v>8.81039</v>
       </c>
     </row>
     <row r="24">
@@ -1007,16 +1007,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.284789</v>
+        <v>0.283567</v>
       </c>
       <c r="D24" t="n">
-        <v>8574297810</v>
+        <v>8548224598</v>
       </c>
       <c r="E24" t="n">
-        <v>2311654284</v>
+        <v>2314091514</v>
       </c>
       <c r="F24" t="n">
-        <v>18.48765</v>
+        <v>17.29955</v>
       </c>
     </row>
     <row r="25">
@@ -1031,16 +1031,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>8.779999999999999</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="D25" t="n">
-        <v>8128302174</v>
+        <v>8158757929</v>
       </c>
       <c r="E25" t="n">
-        <v>3417394</v>
+        <v>3462321</v>
       </c>
       <c r="F25" t="n">
-        <v>2.61704</v>
+        <v>3.45041</v>
       </c>
     </row>
     <row r="26">
@@ -1055,16 +1055,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>5.8</v>
+        <v>5.82</v>
       </c>
       <c r="D26" t="n">
-        <v>7066502768</v>
+        <v>7093087429</v>
       </c>
       <c r="E26" t="n">
-        <v>1007516188</v>
+        <v>1014559086</v>
       </c>
       <c r="F26" t="n">
-        <v>3.93636</v>
+        <v>4.56338</v>
       </c>
     </row>
     <row r="27">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>90.45</v>
+        <v>90.79000000000001</v>
       </c>
       <c r="D27" t="n">
-        <v>6818543284</v>
+        <v>6832406054</v>
       </c>
       <c r="E27" t="n">
-        <v>1443342995</v>
+        <v>1428455782</v>
       </c>
       <c r="F27" t="n">
-        <v>4.38062</v>
+        <v>4.19564</v>
       </c>
     </row>
     <row r="28">
@@ -1103,16 +1103,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>12.11</v>
+        <v>12.13</v>
       </c>
       <c r="D28" t="n">
-        <v>6475051493</v>
+        <v>6468582664</v>
       </c>
       <c r="E28" t="n">
-        <v>883555179</v>
+        <v>868473780</v>
       </c>
       <c r="F28" t="n">
-        <v>3.42643</v>
+        <v>4.26232</v>
       </c>
     </row>
     <row r="29">
@@ -1127,16 +1127,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3573.41</v>
+        <v>3594.84</v>
       </c>
       <c r="D29" t="n">
-        <v>6229530875</v>
+        <v>6254075727</v>
       </c>
       <c r="E29" t="n">
-        <v>103976595</v>
+        <v>104599642</v>
       </c>
       <c r="F29" t="n">
-        <v>8.2064</v>
+        <v>8.82516</v>
       </c>
     </row>
     <row r="30">
@@ -1151,16 +1151,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9.4</v>
+        <v>9.42</v>
       </c>
       <c r="D30" t="n">
-        <v>5646687307</v>
+        <v>5659344661</v>
       </c>
       <c r="E30" t="n">
-        <v>858637673</v>
+        <v>858641909</v>
       </c>
       <c r="F30" t="n">
-        <v>6.14347</v>
+        <v>6.26761</v>
       </c>
     </row>
     <row r="31">
@@ -1175,16 +1175,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.197491</v>
+        <v>0.19867</v>
       </c>
       <c r="D31" t="n">
-        <v>5359892708</v>
+        <v>5384790926</v>
       </c>
       <c r="E31" t="n">
-        <v>120817872</v>
+        <v>121634634</v>
       </c>
       <c r="F31" t="n">
-        <v>11.69802</v>
+        <v>12.78974</v>
       </c>
     </row>
     <row r="32">
@@ -1199,16 +1199,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.99435</v>
+        <v>0.9986930000000001</v>
       </c>
       <c r="D32" t="n">
-        <v>5217775415</v>
+        <v>5226843770</v>
       </c>
       <c r="E32" t="n">
-        <v>16412763</v>
+        <v>16451235</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.56931</v>
+        <v>-0.21584</v>
       </c>
     </row>
     <row r="33">
@@ -1223,16 +1223,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.133678</v>
+        <v>0.136986</v>
       </c>
       <c r="D33" t="n">
-        <v>5079959544</v>
+        <v>5220754802</v>
       </c>
       <c r="E33" t="n">
-        <v>895188955</v>
+        <v>901563713</v>
       </c>
       <c r="F33" t="n">
-        <v>5.463</v>
+        <v>8.60918</v>
       </c>
     </row>
     <row r="34">
@@ -1247,16 +1247,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9.66</v>
+        <v>9.710000000000001</v>
       </c>
       <c r="D34" t="n">
-        <v>4587010509</v>
+        <v>4605777921</v>
       </c>
       <c r="E34" t="n">
-        <v>272743635</v>
+        <v>274183142</v>
       </c>
       <c r="F34" t="n">
-        <v>6.07429</v>
+        <v>6.81327</v>
       </c>
     </row>
     <row r="35">
@@ -1271,16 +1271,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>27.94</v>
+        <v>27.99</v>
       </c>
       <c r="D35" t="n">
-        <v>4201045186</v>
+        <v>4191645494</v>
       </c>
       <c r="E35" t="n">
-        <v>893965885</v>
+        <v>889580767</v>
       </c>
       <c r="F35" t="n">
-        <v>5.76924</v>
+        <v>5.49776</v>
       </c>
     </row>
     <row r="36">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>5.2e-05</v>
+        <v>5.236e-05</v>
       </c>
       <c r="D36" t="n">
-        <v>3925070065</v>
+        <v>3931813183</v>
       </c>
       <c r="E36" t="n">
-        <v>1720283290</v>
+        <v>1699923348</v>
       </c>
       <c r="F36" t="n">
-        <v>1.33985</v>
+        <v>2.74062</v>
       </c>
     </row>
     <row r="37">
@@ -1319,16 +1319,16 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>7.39</v>
+        <v>7.4</v>
       </c>
       <c r="D37" t="n">
-        <v>3830491806</v>
+        <v>3831971457</v>
       </c>
       <c r="E37" t="n">
-        <v>438574850</v>
+        <v>436575944</v>
       </c>
       <c r="F37" t="n">
-        <v>-0.32458</v>
+        <v>0.13281</v>
       </c>
     </row>
     <row r="38">
@@ -1343,16 +1343,16 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.150778</v>
+        <v>0.150958</v>
       </c>
       <c r="D38" t="n">
-        <v>3811511501</v>
+        <v>3804917099</v>
       </c>
       <c r="E38" t="n">
-        <v>153122650</v>
+        <v>151965451</v>
       </c>
       <c r="F38" t="n">
-        <v>-0.5954</v>
+        <v>-0.91532</v>
       </c>
     </row>
     <row r="39">
@@ -1367,16 +1367,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.470479</v>
+        <v>0.472086</v>
       </c>
       <c r="D39" t="n">
-        <v>3766297859</v>
+        <v>3760627445</v>
       </c>
       <c r="E39" t="n">
-        <v>484661119</v>
+        <v>489095714</v>
       </c>
       <c r="F39" t="n">
-        <v>6.56518</v>
+        <v>6.98968</v>
       </c>
     </row>
     <row r="40">
@@ -1391,16 +1391,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>507.51</v>
+        <v>508.95</v>
       </c>
       <c r="D40" t="n">
-        <v>3754446505</v>
+        <v>3756554105</v>
       </c>
       <c r="E40" t="n">
-        <v>285429218</v>
+        <v>286529177</v>
       </c>
       <c r="F40" t="n">
-        <v>2.87863</v>
+        <v>3.44413</v>
       </c>
     </row>
     <row r="41">
@@ -1415,16 +1415,16 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.999717</v>
+        <v>1.003</v>
       </c>
       <c r="D41" t="n">
-        <v>3685665968</v>
+        <v>3691719798</v>
       </c>
       <c r="E41" t="n">
-        <v>227695671</v>
+        <v>223910580</v>
       </c>
       <c r="F41" t="n">
-        <v>-0.3284</v>
+        <v>0.06253</v>
       </c>
     </row>
     <row r="42">
@@ -1439,16 +1439,16 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>24.74</v>
+        <v>24.81</v>
       </c>
       <c r="D42" t="n">
-        <v>3571018763</v>
+        <v>3575039972</v>
       </c>
       <c r="E42" t="n">
-        <v>38464423</v>
+        <v>34121584</v>
       </c>
       <c r="F42" t="n">
-        <v>2.19327</v>
+        <v>2.75394</v>
       </c>
     </row>
     <row r="43">
@@ -1463,16 +1463,16 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.997967</v>
+        <v>1</v>
       </c>
       <c r="D43" t="n">
-        <v>3436077216</v>
+        <v>3444337143</v>
       </c>
       <c r="E43" t="n">
-        <v>157037670</v>
+        <v>160350992</v>
       </c>
       <c r="F43" t="n">
-        <v>-0.25013</v>
+        <v>-0.07893</v>
       </c>
     </row>
     <row r="44">
@@ -1487,16 +1487,16 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>3.39</v>
+        <v>3.41</v>
       </c>
       <c r="D44" t="n">
-        <v>3398407556</v>
+        <v>3406244105</v>
       </c>
       <c r="E44" t="n">
-        <v>1279303703</v>
+        <v>1283931088</v>
       </c>
       <c r="F44" t="n">
-        <v>5.02821</v>
+        <v>7.07185</v>
       </c>
     </row>
     <row r="45">
@@ -1511,16 +1511,16 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3.75</v>
+        <v>3.74</v>
       </c>
       <c r="D45" t="n">
-        <v>3387528462</v>
+        <v>3371052995</v>
       </c>
       <c r="E45" t="n">
-        <v>296181418</v>
+        <v>302252483</v>
       </c>
       <c r="F45" t="n">
-        <v>2.84473</v>
+        <v>2.84241</v>
       </c>
     </row>
     <row r="46">
@@ -1538,13 +1538,13 @@
         <v>1.28</v>
       </c>
       <c r="D46" t="n">
-        <v>3346685530</v>
+        <v>3351227825</v>
       </c>
       <c r="E46" t="n">
-        <v>490864213</v>
+        <v>489828536</v>
       </c>
       <c r="F46" t="n">
-        <v>2.65434</v>
+        <v>2.79961</v>
       </c>
     </row>
     <row r="47">
@@ -1559,16 +1559,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.7867</v>
+        <v>0.789357</v>
       </c>
       <c r="D47" t="n">
-        <v>3225646756</v>
+        <v>3237546477</v>
       </c>
       <c r="E47" t="n">
-        <v>1670400289</v>
+        <v>1671213831</v>
       </c>
       <c r="F47" t="n">
-        <v>11.73951</v>
+        <v>11.87906</v>
       </c>
     </row>
     <row r="48">
@@ -1583,16 +1583,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>160.85</v>
+        <v>161.16</v>
       </c>
       <c r="D48" t="n">
-        <v>2968142680</v>
+        <v>2979464717</v>
       </c>
       <c r="E48" t="n">
-        <v>86572953</v>
+        <v>86762393</v>
       </c>
       <c r="F48" t="n">
-        <v>-1.00593</v>
+        <v>-1.29352</v>
       </c>
     </row>
     <row r="49">
@@ -1607,16 +1607,16 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1.95</v>
+        <v>1.96</v>
       </c>
       <c r="D49" t="n">
-        <v>2934163039</v>
+        <v>2946226428</v>
       </c>
       <c r="E49" t="n">
-        <v>380160497</v>
+        <v>376100945</v>
       </c>
       <c r="F49" t="n">
-        <v>0.97964</v>
+        <v>1.27825</v>
       </c>
     </row>
     <row r="50">
@@ -1631,40 +1631,40 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>4.69</v>
+        <v>4.71</v>
       </c>
       <c r="D50" t="n">
-        <v>2821849071</v>
+        <v>2831890252</v>
       </c>
       <c r="E50" t="n">
-        <v>588249132</v>
+        <v>585172344</v>
       </c>
       <c r="F50" t="n">
-        <v>7.04811</v>
+        <v>7.04621</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>OKB</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>okb</t>
+          <t>mnt</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>46.63</v>
+        <v>0.839365</v>
       </c>
       <c r="D51" t="n">
-        <v>2803633244</v>
+        <v>2818599241</v>
       </c>
       <c r="E51" t="n">
-        <v>19696267</v>
+        <v>181518286</v>
       </c>
       <c r="F51" t="n">
-        <v>5.08722</v>
+        <v>13.91175</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1955265453076</v>
+        <v>1957819789649</v>
       </c>
     </row>
     <row r="3">
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>408743623550</v>
+        <v>408442019407</v>
       </c>
     </row>
     <row r="4">
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>130760277928</v>
+        <v>131041154867</v>
       </c>
     </row>
     <row r="5">
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>123643753527</v>
+        <v>124197184685</v>
       </c>
     </row>
     <row r="6">
@@ -1745,7 +1745,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>92718719024</v>
+        <v>92741072509</v>
       </c>
     </row>
   </sheetData>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$4348.48</t>
+          <t>$4360.69</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>XRP (24.10%)</t>
+          <t>XRP (23.06%)</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Monero (-1.01%)</t>
+          <t>Bitcoin Cash (-1.30%)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Excel data - 2024-11-22 05:26:25
</commit_message>
<xml_diff>
--- a/crypto_live_data.xlsx
+++ b/crypto_live_data.xlsx
@@ -479,16 +479,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>98953</v>
+        <v>98817</v>
       </c>
       <c r="D2" t="n">
-        <v>1957819789649</v>
+        <v>1953772577503</v>
       </c>
       <c r="E2" t="n">
-        <v>107473015554</v>
+        <v>111602031886</v>
       </c>
       <c r="F2" t="n">
-        <v>1.48841</v>
+        <v>1.18963</v>
       </c>
     </row>
     <row r="3">
@@ -503,16 +503,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3388.15</v>
+        <v>3383.02</v>
       </c>
       <c r="D3" t="n">
-        <v>408442019407</v>
+        <v>407043413496</v>
       </c>
       <c r="E3" t="n">
-        <v>55538713089</v>
+        <v>56933584709</v>
       </c>
       <c r="F3" t="n">
-        <v>7.89304</v>
+        <v>7.99777</v>
       </c>
     </row>
     <row r="4">
@@ -530,13 +530,13 @@
         <v>1.001</v>
       </c>
       <c r="D4" t="n">
-        <v>131041154867</v>
+        <v>130788831244</v>
       </c>
       <c r="E4" t="n">
-        <v>113718779050</v>
+        <v>95661940820</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.01997</v>
+        <v>-0.01272</v>
       </c>
     </row>
     <row r="5">
@@ -551,16 +551,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>261.77</v>
+        <v>261.91</v>
       </c>
       <c r="D5" t="n">
-        <v>124197184685</v>
+        <v>124075895781</v>
       </c>
       <c r="E5" t="n">
-        <v>14991831812</v>
+        <v>14990065171</v>
       </c>
       <c r="F5" t="n">
-        <v>8.79411</v>
+        <v>8.63114</v>
       </c>
     </row>
     <row r="6">
@@ -575,16 +575,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>635.35</v>
+        <v>635.51</v>
       </c>
       <c r="D6" t="n">
-        <v>92741072509</v>
+        <v>92676534988</v>
       </c>
       <c r="E6" t="n">
-        <v>2472723832</v>
+        <v>2458154483</v>
       </c>
       <c r="F6" t="n">
-        <v>3.75845</v>
+        <v>3.874</v>
       </c>
     </row>
     <row r="7">
@@ -599,16 +599,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.38</v>
+        <v>1.39</v>
       </c>
       <c r="D7" t="n">
-        <v>79105543405</v>
+        <v>78917385028</v>
       </c>
       <c r="E7" t="n">
-        <v>17824065953</v>
+        <v>17890002015</v>
       </c>
       <c r="F7" t="n">
-        <v>23.06077</v>
+        <v>24.17602</v>
       </c>
     </row>
     <row r="8">
@@ -623,16 +623,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.396932</v>
+        <v>0.395961</v>
       </c>
       <c r="D8" t="n">
-        <v>58333135134</v>
+        <v>58130923980</v>
       </c>
       <c r="E8" t="n">
-        <v>9895261537</v>
+        <v>9854138290</v>
       </c>
       <c r="F8" t="n">
-        <v>2.05635</v>
+        <v>1.94918</v>
       </c>
     </row>
     <row r="9">
@@ -650,13 +650,13 @@
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>38340757364</v>
+        <v>38297868428</v>
       </c>
       <c r="E9" t="n">
-        <v>11657194673</v>
+        <v>11136208756</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.0022</v>
+        <v>-0.00488</v>
       </c>
     </row>
     <row r="10">
@@ -671,16 +671,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3387.77</v>
+        <v>3383.35</v>
       </c>
       <c r="D10" t="n">
-        <v>33192243452</v>
+        <v>33126025781</v>
       </c>
       <c r="E10" t="n">
-        <v>145663717</v>
+        <v>144753180</v>
       </c>
       <c r="F10" t="n">
-        <v>8.07043</v>
+        <v>8.165369999999999</v>
       </c>
     </row>
     <row r="11">
@@ -695,16 +695,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.883266</v>
+        <v>0.882933</v>
       </c>
       <c r="D11" t="n">
-        <v>31681558093</v>
+        <v>31575973787</v>
       </c>
       <c r="E11" t="n">
-        <v>3291559390</v>
+        <v>3537099617</v>
       </c>
       <c r="F11" t="n">
-        <v>10.80615</v>
+        <v>10.89773</v>
       </c>
     </row>
     <row r="12">
@@ -719,16 +719,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.200654</v>
+        <v>0.200395</v>
       </c>
       <c r="D12" t="n">
-        <v>17337756980</v>
+        <v>17289684171</v>
       </c>
       <c r="E12" t="n">
-        <v>1073293125</v>
+        <v>1081990781</v>
       </c>
       <c r="F12" t="n">
-        <v>1.51007</v>
+        <v>1.38293</v>
       </c>
     </row>
     <row r="13">
@@ -743,16 +743,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>36.46</v>
+        <v>36.4</v>
       </c>
       <c r="D13" t="n">
-        <v>14919274431</v>
+        <v>14881406931</v>
       </c>
       <c r="E13" t="n">
-        <v>1037618086</v>
+        <v>1037701522</v>
       </c>
       <c r="F13" t="n">
-        <v>6.6755</v>
+        <v>6.53633</v>
       </c>
     </row>
     <row r="14">
@@ -767,16 +767,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.504e-05</v>
+        <v>2.499e-05</v>
       </c>
       <c r="D14" t="n">
-        <v>14768327270</v>
+        <v>14705498503</v>
       </c>
       <c r="E14" t="n">
-        <v>1616021481</v>
+        <v>1610868051</v>
       </c>
       <c r="F14" t="n">
-        <v>3.28015</v>
+        <v>2.95005</v>
       </c>
     </row>
     <row r="15">
@@ -791,16 +791,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>4024.97</v>
+        <v>3998.89</v>
       </c>
       <c r="D15" t="n">
-        <v>14527190907</v>
+        <v>14427358496</v>
       </c>
       <c r="E15" t="n">
-        <v>168464106</v>
+        <v>93745940</v>
       </c>
       <c r="F15" t="n">
-        <v>7.91277</v>
+        <v>7.34263</v>
       </c>
     </row>
     <row r="16">
@@ -815,16 +815,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>98944</v>
+        <v>98913</v>
       </c>
       <c r="D16" t="n">
-        <v>14457817201</v>
+        <v>14395882737</v>
       </c>
       <c r="E16" t="n">
-        <v>864190786</v>
+        <v>842373855</v>
       </c>
       <c r="F16" t="n">
-        <v>2.04243</v>
+        <v>1.97696</v>
       </c>
     </row>
     <row r="17">
@@ -839,16 +839,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5.57</v>
+        <v>5.56</v>
       </c>
       <c r="D17" t="n">
-        <v>14197176170</v>
+        <v>14140396529</v>
       </c>
       <c r="E17" t="n">
-        <v>637419627</v>
+        <v>637922301</v>
       </c>
       <c r="F17" t="n">
-        <v>3.39082</v>
+        <v>3.21844</v>
       </c>
     </row>
     <row r="18">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3.62</v>
+        <v>3.61</v>
       </c>
       <c r="D18" t="n">
-        <v>10307866671</v>
+        <v>10263931784</v>
       </c>
       <c r="E18" t="n">
-        <v>2420681201</v>
+        <v>1893045491</v>
       </c>
       <c r="F18" t="n">
-        <v>1.06291</v>
+        <v>0.7609</v>
       </c>
     </row>
     <row r="19">
@@ -887,16 +887,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>497.43</v>
+        <v>496.39</v>
       </c>
       <c r="D19" t="n">
-        <v>9840002010</v>
+        <v>9820858921</v>
       </c>
       <c r="E19" t="n">
-        <v>2055046626</v>
+        <v>1972327901</v>
       </c>
       <c r="F19" t="n">
-        <v>-1.2951</v>
+        <v>-3.06361</v>
       </c>
     </row>
     <row r="20">
@@ -911,16 +911,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3387.27</v>
+        <v>3383.89</v>
       </c>
       <c r="D20" t="n">
-        <v>9654793051</v>
+        <v>9627349785</v>
       </c>
       <c r="E20" t="n">
-        <v>1123693284</v>
+        <v>1238335912</v>
       </c>
       <c r="F20" t="n">
-        <v>7.91282</v>
+        <v>8.11872</v>
       </c>
     </row>
     <row r="21">
@@ -935,64 +935,64 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>15.27</v>
+        <v>15.28</v>
       </c>
       <c r="D21" t="n">
-        <v>9580085936</v>
+        <v>9558865243</v>
       </c>
       <c r="E21" t="n">
-        <v>1244740994</v>
+        <v>1247144986</v>
       </c>
       <c r="F21" t="n">
-        <v>4.26916</v>
+        <v>4.32433</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>pepe</t>
+          <t>dot</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.135e-05</v>
+        <v>6.23</v>
       </c>
       <c r="D22" t="n">
-        <v>8982335231</v>
+        <v>8966606443</v>
       </c>
       <c r="E22" t="n">
-        <v>6858230993</v>
+        <v>823772180</v>
       </c>
       <c r="F22" t="n">
-        <v>9.116300000000001</v>
+        <v>8.80635</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>dot</t>
+          <t>pepe</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>6.23</v>
+        <v>2.122e-05</v>
       </c>
       <c r="D23" t="n">
-        <v>8964658656</v>
+        <v>8928147587</v>
       </c>
       <c r="E23" t="n">
-        <v>818046188</v>
+        <v>6810977654</v>
       </c>
       <c r="F23" t="n">
-        <v>8.81039</v>
+        <v>8.61903</v>
       </c>
     </row>
     <row r="24">
@@ -1007,16 +1007,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.283567</v>
+        <v>0.283327</v>
       </c>
       <c r="D24" t="n">
-        <v>8548224598</v>
+        <v>8497950433</v>
       </c>
       <c r="E24" t="n">
-        <v>2314091514</v>
+        <v>2292477997</v>
       </c>
       <c r="F24" t="n">
-        <v>17.29955</v>
+        <v>17.93069</v>
       </c>
     </row>
     <row r="25">
@@ -1031,16 +1031,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>8.800000000000001</v>
+        <v>8.76</v>
       </c>
       <c r="D25" t="n">
-        <v>8158757929</v>
+        <v>8102501993</v>
       </c>
       <c r="E25" t="n">
-        <v>3462321</v>
+        <v>3436944</v>
       </c>
       <c r="F25" t="n">
-        <v>3.45041</v>
+        <v>2.93876</v>
       </c>
     </row>
     <row r="26">
@@ -1055,16 +1055,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>5.82</v>
+        <v>5.81</v>
       </c>
       <c r="D26" t="n">
-        <v>7093087429</v>
+        <v>7068507828</v>
       </c>
       <c r="E26" t="n">
-        <v>1014559086</v>
+        <v>1011665226</v>
       </c>
       <c r="F26" t="n">
-        <v>4.56338</v>
+        <v>4.38588</v>
       </c>
     </row>
     <row r="27">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>90.79000000000001</v>
+        <v>90.5</v>
       </c>
       <c r="D27" t="n">
-        <v>6832406054</v>
+        <v>6802345942</v>
       </c>
       <c r="E27" t="n">
-        <v>1428455782</v>
+        <v>1416854551</v>
       </c>
       <c r="F27" t="n">
-        <v>4.19564</v>
+        <v>4.09299</v>
       </c>
     </row>
     <row r="28">
@@ -1103,16 +1103,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>12.13</v>
+        <v>12.14</v>
       </c>
       <c r="D28" t="n">
-        <v>6468582664</v>
+        <v>6466066532</v>
       </c>
       <c r="E28" t="n">
-        <v>868473780</v>
+        <v>865453610</v>
       </c>
       <c r="F28" t="n">
-        <v>4.26232</v>
+        <v>4.19963</v>
       </c>
     </row>
     <row r="29">
@@ -1127,16 +1127,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3594.84</v>
+        <v>3562.66</v>
       </c>
       <c r="D29" t="n">
-        <v>6254075727</v>
+        <v>6191810117</v>
       </c>
       <c r="E29" t="n">
-        <v>104599642</v>
+        <v>102355778</v>
       </c>
       <c r="F29" t="n">
-        <v>8.82516</v>
+        <v>8.005269999999999</v>
       </c>
     </row>
     <row r="30">
@@ -1154,13 +1154,13 @@
         <v>9.42</v>
       </c>
       <c r="D30" t="n">
-        <v>5659344661</v>
+        <v>5647368459</v>
       </c>
       <c r="E30" t="n">
-        <v>858641909</v>
+        <v>858974039</v>
       </c>
       <c r="F30" t="n">
-        <v>6.26761</v>
+        <v>6.04675</v>
       </c>
     </row>
     <row r="31">
@@ -1175,16 +1175,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.19867</v>
+        <v>0.199016</v>
       </c>
       <c r="D31" t="n">
-        <v>5384790926</v>
+        <v>5400717796</v>
       </c>
       <c r="E31" t="n">
-        <v>121634634</v>
+        <v>124320291</v>
       </c>
       <c r="F31" t="n">
-        <v>12.78974</v>
+        <v>13.2041</v>
       </c>
     </row>
     <row r="32">
@@ -1199,16 +1199,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.9986930000000001</v>
+        <v>0.998515</v>
       </c>
       <c r="D32" t="n">
-        <v>5226843770</v>
+        <v>5222825181</v>
       </c>
       <c r="E32" t="n">
-        <v>16451235</v>
+        <v>16300713</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.21584</v>
+        <v>-0.78412</v>
       </c>
     </row>
     <row r="33">
@@ -1223,16 +1223,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.136986</v>
+        <v>0.134483</v>
       </c>
       <c r="D33" t="n">
-        <v>5220754802</v>
+        <v>5137474725</v>
       </c>
       <c r="E33" t="n">
-        <v>901563713</v>
+        <v>874776333</v>
       </c>
       <c r="F33" t="n">
-        <v>8.60918</v>
+        <v>6.51209</v>
       </c>
     </row>
     <row r="34">
@@ -1247,16 +1247,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9.710000000000001</v>
+        <v>9.69</v>
       </c>
       <c r="D34" t="n">
-        <v>4605777921</v>
+        <v>4598987074</v>
       </c>
       <c r="E34" t="n">
-        <v>274183142</v>
+        <v>273681702</v>
       </c>
       <c r="F34" t="n">
-        <v>6.81327</v>
+        <v>6.55566</v>
       </c>
     </row>
     <row r="35">
@@ -1271,16 +1271,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>27.99</v>
+        <v>27.94</v>
       </c>
       <c r="D35" t="n">
-        <v>4191645494</v>
+        <v>4178731627</v>
       </c>
       <c r="E35" t="n">
-        <v>889580767</v>
+        <v>884770184</v>
       </c>
       <c r="F35" t="n">
-        <v>5.49776</v>
+        <v>5.19909</v>
       </c>
     </row>
     <row r="36">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>5.236e-05</v>
+        <v>5.199e-05</v>
       </c>
       <c r="D36" t="n">
-        <v>3931813183</v>
+        <v>3901948320</v>
       </c>
       <c r="E36" t="n">
-        <v>1699923348</v>
+        <v>1688917428</v>
       </c>
       <c r="F36" t="n">
-        <v>2.74062</v>
+        <v>1.89678</v>
       </c>
     </row>
     <row r="37">
@@ -1319,16 +1319,16 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>7.4</v>
+        <v>7.38</v>
       </c>
       <c r="D37" t="n">
-        <v>3831971457</v>
+        <v>3815241912</v>
       </c>
       <c r="E37" t="n">
-        <v>436575944</v>
+        <v>434605828</v>
       </c>
       <c r="F37" t="n">
-        <v>0.13281</v>
+        <v>-0.28555</v>
       </c>
     </row>
     <row r="38">
@@ -1343,16 +1343,16 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.150958</v>
+        <v>0.151407</v>
       </c>
       <c r="D38" t="n">
-        <v>3804917099</v>
+        <v>3808608303</v>
       </c>
       <c r="E38" t="n">
-        <v>151965451</v>
+        <v>152035278</v>
       </c>
       <c r="F38" t="n">
-        <v>-0.91532</v>
+        <v>-0.54395</v>
       </c>
     </row>
     <row r="39">
@@ -1367,16 +1367,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.472086</v>
+        <v>0.47192</v>
       </c>
       <c r="D39" t="n">
-        <v>3760627445</v>
+        <v>3760540435</v>
       </c>
       <c r="E39" t="n">
-        <v>489095714</v>
+        <v>489495021</v>
       </c>
       <c r="F39" t="n">
-        <v>6.98968</v>
+        <v>7.29274</v>
       </c>
     </row>
     <row r="40">
@@ -1391,16 +1391,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>508.95</v>
+        <v>508.17</v>
       </c>
       <c r="D40" t="n">
-        <v>3756554105</v>
+        <v>3750000473</v>
       </c>
       <c r="E40" t="n">
-        <v>286529177</v>
+        <v>286015428</v>
       </c>
       <c r="F40" t="n">
-        <v>3.44413</v>
+        <v>3.47623</v>
       </c>
     </row>
     <row r="41">
@@ -1418,13 +1418,13 @@
         <v>1.003</v>
       </c>
       <c r="D41" t="n">
-        <v>3691719798</v>
+        <v>3687728228</v>
       </c>
       <c r="E41" t="n">
-        <v>223910580</v>
+        <v>223922865</v>
       </c>
       <c r="F41" t="n">
-        <v>0.06253</v>
+        <v>0.06525</v>
       </c>
     </row>
     <row r="42">
@@ -1442,13 +1442,13 @@
         <v>24.81</v>
       </c>
       <c r="D42" t="n">
-        <v>3575039972</v>
+        <v>3582963813</v>
       </c>
       <c r="E42" t="n">
-        <v>34121584</v>
+        <v>33496946</v>
       </c>
       <c r="F42" t="n">
-        <v>2.75394</v>
+        <v>2.63912</v>
       </c>
     </row>
     <row r="43">
@@ -1466,13 +1466,13 @@
         <v>1</v>
       </c>
       <c r="D43" t="n">
-        <v>3444337143</v>
+        <v>3439078996</v>
       </c>
       <c r="E43" t="n">
-        <v>160350992</v>
+        <v>154364886</v>
       </c>
       <c r="F43" t="n">
-        <v>-0.07893</v>
+        <v>-0.00669</v>
       </c>
     </row>
     <row r="44">
@@ -1487,16 +1487,16 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>3.41</v>
+        <v>3.4</v>
       </c>
       <c r="D44" t="n">
-        <v>3406244105</v>
+        <v>3396851368</v>
       </c>
       <c r="E44" t="n">
-        <v>1283931088</v>
+        <v>1281631615</v>
       </c>
       <c r="F44" t="n">
-        <v>7.07185</v>
+        <v>6.78171</v>
       </c>
     </row>
     <row r="45">
@@ -1511,16 +1511,16 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3.74</v>
+        <v>3.72</v>
       </c>
       <c r="D45" t="n">
-        <v>3371052995</v>
+        <v>3361552390</v>
       </c>
       <c r="E45" t="n">
-        <v>302252483</v>
+        <v>301693729</v>
       </c>
       <c r="F45" t="n">
-        <v>2.84241</v>
+        <v>2.64148</v>
       </c>
     </row>
     <row r="46">
@@ -1538,13 +1538,13 @@
         <v>1.28</v>
       </c>
       <c r="D46" t="n">
-        <v>3351227825</v>
+        <v>3337822225</v>
       </c>
       <c r="E46" t="n">
-        <v>489828536</v>
+        <v>488298136</v>
       </c>
       <c r="F46" t="n">
-        <v>2.79961</v>
+        <v>2.42598</v>
       </c>
     </row>
     <row r="47">
@@ -1559,16 +1559,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.789357</v>
+        <v>0.787967</v>
       </c>
       <c r="D47" t="n">
-        <v>3237546477</v>
+        <v>3226906040</v>
       </c>
       <c r="E47" t="n">
-        <v>1671213831</v>
+        <v>1668181094</v>
       </c>
       <c r="F47" t="n">
-        <v>11.87906</v>
+        <v>12.37254</v>
       </c>
     </row>
     <row r="48">
@@ -1583,16 +1583,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>161.16</v>
+        <v>160.67</v>
       </c>
       <c r="D48" t="n">
-        <v>2979464717</v>
+        <v>2963867990</v>
       </c>
       <c r="E48" t="n">
-        <v>86762393</v>
+        <v>83352737</v>
       </c>
       <c r="F48" t="n">
-        <v>-1.29352</v>
+        <v>-1.78004</v>
       </c>
     </row>
     <row r="49">
@@ -1607,64 +1607,64 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1.96</v>
+        <v>1.95</v>
       </c>
       <c r="D49" t="n">
-        <v>2946226428</v>
+        <v>2933339796</v>
       </c>
       <c r="E49" t="n">
-        <v>376100945</v>
+        <v>368223956</v>
       </c>
       <c r="F49" t="n">
-        <v>1.27825</v>
+        <v>0.21023</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>fil</t>
+          <t>mnt</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>4.71</v>
+        <v>0.846624</v>
       </c>
       <c r="D50" t="n">
-        <v>2831890252</v>
+        <v>2850586086</v>
       </c>
       <c r="E50" t="n">
-        <v>585172344</v>
+        <v>183686556</v>
       </c>
       <c r="F50" t="n">
-        <v>7.04621</v>
+        <v>15.21575</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>mnt</t>
+          <t>fil</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.839365</v>
+        <v>4.71</v>
       </c>
       <c r="D51" t="n">
-        <v>2818599241</v>
+        <v>2828845966</v>
       </c>
       <c r="E51" t="n">
-        <v>181518286</v>
+        <v>583490036</v>
       </c>
       <c r="F51" t="n">
-        <v>13.91175</v>
+        <v>7.03179</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1957819789649</v>
+        <v>1953772577503</v>
       </c>
     </row>
     <row r="3">
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>408442019407</v>
+        <v>407043413496</v>
       </c>
     </row>
     <row r="4">
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>131041154867</v>
+        <v>130788831244</v>
       </c>
     </row>
     <row r="5">
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>124197184685</v>
+        <v>124075895781</v>
       </c>
     </row>
     <row r="6">
@@ -1745,7 +1745,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>92741072509</v>
+        <v>92676534988</v>
       </c>
     </row>
   </sheetData>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$4360.69</t>
+          <t>$4355.88</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>XRP (23.06%)</t>
+          <t>XRP (24.18%)</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bitcoin Cash (-1.30%)</t>
+          <t>Bitcoin Cash (-3.06%)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Excel data - 2024-11-22 05:36:27
</commit_message>
<xml_diff>
--- a/crypto_live_data.xlsx
+++ b/crypto_live_data.xlsx
@@ -479,16 +479,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>98817</v>
+        <v>99049</v>
       </c>
       <c r="D2" t="n">
-        <v>1953772577503</v>
+        <v>1959195618520</v>
       </c>
       <c r="E2" t="n">
-        <v>111602031886</v>
+        <v>112637342948</v>
       </c>
       <c r="F2" t="n">
-        <v>1.18963</v>
+        <v>1.23955</v>
       </c>
     </row>
     <row r="3">
@@ -503,16 +503,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3383.02</v>
+        <v>3387.32</v>
       </c>
       <c r="D3" t="n">
-        <v>407043413496</v>
+        <v>408077072603</v>
       </c>
       <c r="E3" t="n">
-        <v>56933584709</v>
+        <v>56006401370</v>
       </c>
       <c r="F3" t="n">
-        <v>7.99777</v>
+        <v>8.157629999999999</v>
       </c>
     </row>
     <row r="4">
@@ -530,13 +530,13 @@
         <v>1.001</v>
       </c>
       <c r="D4" t="n">
-        <v>130788831244</v>
+        <v>130946260507</v>
       </c>
       <c r="E4" t="n">
-        <v>95661940820</v>
+        <v>118643630134</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.01272</v>
+        <v>-0.04242</v>
       </c>
     </row>
     <row r="5">
@@ -551,16 +551,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>261.91</v>
+        <v>262.45</v>
       </c>
       <c r="D5" t="n">
-        <v>124075895781</v>
+        <v>124537701624</v>
       </c>
       <c r="E5" t="n">
-        <v>14990065171</v>
+        <v>14996288932</v>
       </c>
       <c r="F5" t="n">
-        <v>8.63114</v>
+        <v>8.74217</v>
       </c>
     </row>
     <row r="6">
@@ -575,16 +575,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>635.51</v>
+        <v>635.4299999999999</v>
       </c>
       <c r="D6" t="n">
-        <v>92676534988</v>
+        <v>92774471217</v>
       </c>
       <c r="E6" t="n">
-        <v>2458154483</v>
+        <v>2471223191</v>
       </c>
       <c r="F6" t="n">
-        <v>3.874</v>
+        <v>3.69055</v>
       </c>
     </row>
     <row r="7">
@@ -602,13 +602,13 @@
         <v>1.39</v>
       </c>
       <c r="D7" t="n">
-        <v>78917385028</v>
+        <v>79043620118</v>
       </c>
       <c r="E7" t="n">
-        <v>17890002015</v>
+        <v>17986070520</v>
       </c>
       <c r="F7" t="n">
-        <v>24.17602</v>
+        <v>24.44778</v>
       </c>
     </row>
     <row r="8">
@@ -623,16 +623,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.395961</v>
+        <v>0.396036</v>
       </c>
       <c r="D8" t="n">
-        <v>58130923980</v>
+        <v>58263803542</v>
       </c>
       <c r="E8" t="n">
-        <v>9854138290</v>
+        <v>9818155855</v>
       </c>
       <c r="F8" t="n">
-        <v>1.94918</v>
+        <v>2.05484</v>
       </c>
     </row>
     <row r="9">
@@ -650,13 +650,13 @@
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>38297868428</v>
+        <v>38333818068</v>
       </c>
       <c r="E9" t="n">
-        <v>11136208756</v>
+        <v>10390110683</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.00488</v>
+        <v>-0.05674</v>
       </c>
     </row>
     <row r="10">
@@ -671,16 +671,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3383.35</v>
+        <v>3386.1</v>
       </c>
       <c r="D10" t="n">
-        <v>33126025781</v>
+        <v>33167306357</v>
       </c>
       <c r="E10" t="n">
-        <v>144753180</v>
+        <v>148210338</v>
       </c>
       <c r="F10" t="n">
-        <v>8.165369999999999</v>
+        <v>8.32367</v>
       </c>
     </row>
     <row r="11">
@@ -695,16 +695,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.882933</v>
+        <v>0.884086</v>
       </c>
       <c r="D11" t="n">
-        <v>31575973787</v>
+        <v>31689028378</v>
       </c>
       <c r="E11" t="n">
-        <v>3537099617</v>
+        <v>3620403635</v>
       </c>
       <c r="F11" t="n">
-        <v>10.89773</v>
+        <v>12.00104</v>
       </c>
     </row>
     <row r="12">
@@ -719,16 +719,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.200395</v>
+        <v>0.20032</v>
       </c>
       <c r="D12" t="n">
-        <v>17289684171</v>
+        <v>17312612565</v>
       </c>
       <c r="E12" t="n">
-        <v>1081990781</v>
+        <v>1068387702</v>
       </c>
       <c r="F12" t="n">
-        <v>1.38293</v>
+        <v>1.32711</v>
       </c>
     </row>
     <row r="13">
@@ -743,16 +743,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>36.4</v>
+        <v>36.33</v>
       </c>
       <c r="D13" t="n">
-        <v>14881406931</v>
+        <v>14861570205</v>
       </c>
       <c r="E13" t="n">
-        <v>1037701522</v>
+        <v>1050610416</v>
       </c>
       <c r="F13" t="n">
-        <v>6.53633</v>
+        <v>6.52267</v>
       </c>
     </row>
     <row r="14">
@@ -770,13 +770,13 @@
         <v>2.499e-05</v>
       </c>
       <c r="D14" t="n">
-        <v>14705498503</v>
+        <v>14719052047</v>
       </c>
       <c r="E14" t="n">
-        <v>1610868051</v>
+        <v>1610749228</v>
       </c>
       <c r="F14" t="n">
-        <v>2.95005</v>
+        <v>2.89691</v>
       </c>
     </row>
     <row r="15">
@@ -791,16 +791,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>3998.89</v>
+        <v>4011.57</v>
       </c>
       <c r="D15" t="n">
-        <v>14427358496</v>
+        <v>14487656085</v>
       </c>
       <c r="E15" t="n">
-        <v>93745940</v>
+        <v>157676278</v>
       </c>
       <c r="F15" t="n">
-        <v>7.34263</v>
+        <v>8.152979999999999</v>
       </c>
     </row>
     <row r="16">
@@ -815,16 +815,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>98913</v>
+        <v>99016</v>
       </c>
       <c r="D16" t="n">
-        <v>14395882737</v>
+        <v>14437890938</v>
       </c>
       <c r="E16" t="n">
-        <v>842373855</v>
+        <v>854187820</v>
       </c>
       <c r="F16" t="n">
-        <v>1.97696</v>
+        <v>1.62661</v>
       </c>
     </row>
     <row r="17">
@@ -842,13 +842,13 @@
         <v>5.56</v>
       </c>
       <c r="D17" t="n">
-        <v>14140396529</v>
+        <v>14174714359</v>
       </c>
       <c r="E17" t="n">
-        <v>637922301</v>
+        <v>638662056</v>
       </c>
       <c r="F17" t="n">
-        <v>3.21844</v>
+        <v>3.18693</v>
       </c>
     </row>
     <row r="18">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3.61</v>
+        <v>3.62</v>
       </c>
       <c r="D18" t="n">
-        <v>10263931784</v>
+        <v>10296343269</v>
       </c>
       <c r="E18" t="n">
-        <v>1893045491</v>
+        <v>2081734581</v>
       </c>
       <c r="F18" t="n">
-        <v>0.7609</v>
+        <v>0.5196</v>
       </c>
     </row>
     <row r="19">
@@ -887,16 +887,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>496.39</v>
+        <v>497.01</v>
       </c>
       <c r="D19" t="n">
-        <v>9820858921</v>
+        <v>9820919497</v>
       </c>
       <c r="E19" t="n">
-        <v>1972327901</v>
+        <v>1936718320</v>
       </c>
       <c r="F19" t="n">
-        <v>-3.06361</v>
+        <v>-3.23961</v>
       </c>
     </row>
     <row r="20">
@@ -911,16 +911,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3383.89</v>
+        <v>3386.67</v>
       </c>
       <c r="D20" t="n">
-        <v>9627349785</v>
+        <v>9647766380</v>
       </c>
       <c r="E20" t="n">
-        <v>1238335912</v>
+        <v>1272082578</v>
       </c>
       <c r="F20" t="n">
-        <v>8.11872</v>
+        <v>8.148099999999999</v>
       </c>
     </row>
     <row r="21">
@@ -935,16 +935,16 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>15.28</v>
+        <v>15.29</v>
       </c>
       <c r="D21" t="n">
-        <v>9558865243</v>
+        <v>9589028913</v>
       </c>
       <c r="E21" t="n">
-        <v>1247144986</v>
+        <v>1250243694</v>
       </c>
       <c r="F21" t="n">
-        <v>4.32433</v>
+        <v>4.19627</v>
       </c>
     </row>
     <row r="22">
@@ -959,16 +959,16 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>6.23</v>
+        <v>6.22</v>
       </c>
       <c r="D22" t="n">
-        <v>8966606443</v>
+        <v>8950792803</v>
       </c>
       <c r="E22" t="n">
-        <v>823772180</v>
+        <v>828809348</v>
       </c>
       <c r="F22" t="n">
-        <v>8.80635</v>
+        <v>8.66395</v>
       </c>
     </row>
     <row r="23">
@@ -983,16 +983,16 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2.122e-05</v>
+        <v>2.129e-05</v>
       </c>
       <c r="D23" t="n">
-        <v>8928147587</v>
+        <v>8947854713</v>
       </c>
       <c r="E23" t="n">
-        <v>6810977654</v>
+        <v>6816364706</v>
       </c>
       <c r="F23" t="n">
-        <v>8.61903</v>
+        <v>9.08339</v>
       </c>
     </row>
     <row r="24">
@@ -1007,16 +1007,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.283327</v>
+        <v>0.283467</v>
       </c>
       <c r="D24" t="n">
-        <v>8497950433</v>
+        <v>8476827049</v>
       </c>
       <c r="E24" t="n">
-        <v>2292477997</v>
+        <v>2299577623</v>
       </c>
       <c r="F24" t="n">
-        <v>17.93069</v>
+        <v>18.22379</v>
       </c>
     </row>
     <row r="25">
@@ -1031,16 +1031,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>8.76</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="D25" t="n">
-        <v>8102501993</v>
+        <v>8141138033</v>
       </c>
       <c r="E25" t="n">
-        <v>3436944</v>
+        <v>3450901</v>
       </c>
       <c r="F25" t="n">
-        <v>2.93876</v>
+        <v>3.34373</v>
       </c>
     </row>
     <row r="26">
@@ -1055,16 +1055,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>5.81</v>
+        <v>5.8</v>
       </c>
       <c r="D26" t="n">
-        <v>7068507828</v>
+        <v>7070338866</v>
       </c>
       <c r="E26" t="n">
-        <v>1011665226</v>
+        <v>1011815621</v>
       </c>
       <c r="F26" t="n">
-        <v>4.38588</v>
+        <v>4.29611</v>
       </c>
     </row>
     <row r="27">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>90.5</v>
+        <v>90.54000000000001</v>
       </c>
       <c r="D27" t="n">
-        <v>6802345942</v>
+        <v>6809385663</v>
       </c>
       <c r="E27" t="n">
-        <v>1416854551</v>
+        <v>1413117460</v>
       </c>
       <c r="F27" t="n">
-        <v>4.09299</v>
+        <v>4.08485</v>
       </c>
     </row>
     <row r="28">
@@ -1103,16 +1103,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>12.14</v>
+        <v>12.13</v>
       </c>
       <c r="D28" t="n">
-        <v>6466066532</v>
+        <v>6470864453</v>
       </c>
       <c r="E28" t="n">
-        <v>865453610</v>
+        <v>865197468</v>
       </c>
       <c r="F28" t="n">
-        <v>4.19963</v>
+        <v>3.80178</v>
       </c>
     </row>
     <row r="29">
@@ -1127,16 +1127,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3562.66</v>
+        <v>3568.39</v>
       </c>
       <c r="D29" t="n">
-        <v>6191810117</v>
+        <v>6207201257</v>
       </c>
       <c r="E29" t="n">
-        <v>102355778</v>
+        <v>104283760</v>
       </c>
       <c r="F29" t="n">
-        <v>8.005269999999999</v>
+        <v>8.14161</v>
       </c>
     </row>
     <row r="30">
@@ -1151,16 +1151,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9.42</v>
+        <v>9.41</v>
       </c>
       <c r="D30" t="n">
-        <v>5647368459</v>
+        <v>5652647882</v>
       </c>
       <c r="E30" t="n">
-        <v>858974039</v>
+        <v>861384256</v>
       </c>
       <c r="F30" t="n">
-        <v>6.04675</v>
+        <v>5.93018</v>
       </c>
     </row>
     <row r="31">
@@ -1175,16 +1175,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.199016</v>
+        <v>0.200382</v>
       </c>
       <c r="D31" t="n">
-        <v>5400717796</v>
+        <v>5446042457</v>
       </c>
       <c r="E31" t="n">
-        <v>124320291</v>
+        <v>126658464</v>
       </c>
       <c r="F31" t="n">
-        <v>13.2041</v>
+        <v>14.08539</v>
       </c>
     </row>
     <row r="32">
@@ -1199,16 +1199,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.998515</v>
+        <v>1.002</v>
       </c>
       <c r="D32" t="n">
-        <v>5222825181</v>
+        <v>5226148199</v>
       </c>
       <c r="E32" t="n">
-        <v>16300713</v>
+        <v>16537152</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.78412</v>
+        <v>0.00528</v>
       </c>
     </row>
     <row r="33">
@@ -1223,16 +1223,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.134483</v>
+        <v>0.133661</v>
       </c>
       <c r="D33" t="n">
-        <v>5137474725</v>
+        <v>5102145955</v>
       </c>
       <c r="E33" t="n">
-        <v>874776333</v>
+        <v>895575078</v>
       </c>
       <c r="F33" t="n">
-        <v>6.51209</v>
+        <v>5.98247</v>
       </c>
     </row>
     <row r="34">
@@ -1247,16 +1247,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9.69</v>
+        <v>9.630000000000001</v>
       </c>
       <c r="D34" t="n">
-        <v>4598987074</v>
+        <v>4568754468</v>
       </c>
       <c r="E34" t="n">
-        <v>273681702</v>
+        <v>274366712</v>
       </c>
       <c r="F34" t="n">
-        <v>6.55566</v>
+        <v>5.80122</v>
       </c>
     </row>
     <row r="35">
@@ -1271,16 +1271,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>27.94</v>
+        <v>27.99</v>
       </c>
       <c r="D35" t="n">
-        <v>4178731627</v>
+        <v>4188436495</v>
       </c>
       <c r="E35" t="n">
-        <v>884770184</v>
+        <v>882892358</v>
       </c>
       <c r="F35" t="n">
-        <v>5.19909</v>
+        <v>5.20897</v>
       </c>
     </row>
     <row r="36">
@@ -1295,64 +1295,64 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>5.199e-05</v>
+        <v>5.195e-05</v>
       </c>
       <c r="D36" t="n">
-        <v>3901948320</v>
+        <v>3901989396</v>
       </c>
       <c r="E36" t="n">
-        <v>1688917428</v>
+        <v>1682777811</v>
       </c>
       <c r="F36" t="n">
-        <v>1.89678</v>
+        <v>2.20426</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>render</t>
+          <t>kas</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>7.38</v>
+        <v>0.151353</v>
       </c>
       <c r="D37" t="n">
-        <v>3815241912</v>
+        <v>3817573608</v>
       </c>
       <c r="E37" t="n">
-        <v>434605828</v>
+        <v>151839983</v>
       </c>
       <c r="F37" t="n">
-        <v>-0.28555</v>
+        <v>-0.79223</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>kas</t>
+          <t>render</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.151407</v>
+        <v>7.38</v>
       </c>
       <c r="D38" t="n">
-        <v>3808608303</v>
+        <v>3817395639</v>
       </c>
       <c r="E38" t="n">
-        <v>152035278</v>
+        <v>434850443</v>
       </c>
       <c r="F38" t="n">
-        <v>-0.54395</v>
+        <v>-0.12395</v>
       </c>
     </row>
     <row r="39">
@@ -1367,16 +1367,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.47192</v>
+        <v>0.472771</v>
       </c>
       <c r="D39" t="n">
-        <v>3760540435</v>
+        <v>3768901866</v>
       </c>
       <c r="E39" t="n">
-        <v>489495021</v>
+        <v>491287376</v>
       </c>
       <c r="F39" t="n">
-        <v>7.29274</v>
+        <v>7.38356</v>
       </c>
     </row>
     <row r="40">
@@ -1391,16 +1391,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>508.17</v>
+        <v>507.56</v>
       </c>
       <c r="D40" t="n">
-        <v>3750000473</v>
+        <v>3757496611</v>
       </c>
       <c r="E40" t="n">
-        <v>286015428</v>
+        <v>284629438</v>
       </c>
       <c r="F40" t="n">
-        <v>3.47623</v>
+        <v>3.05338</v>
       </c>
     </row>
     <row r="41">
@@ -1415,16 +1415,16 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1.003</v>
+        <v>1.002</v>
       </c>
       <c r="D41" t="n">
-        <v>3687728228</v>
+        <v>3687424253</v>
       </c>
       <c r="E41" t="n">
-        <v>223922865</v>
+        <v>224417787</v>
       </c>
       <c r="F41" t="n">
-        <v>0.06525</v>
+        <v>-0.0735</v>
       </c>
     </row>
     <row r="42">
@@ -1439,16 +1439,16 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>24.81</v>
+        <v>24.82</v>
       </c>
       <c r="D42" t="n">
-        <v>3582963813</v>
+        <v>3576586417</v>
       </c>
       <c r="E42" t="n">
-        <v>33496946</v>
+        <v>33415891</v>
       </c>
       <c r="F42" t="n">
-        <v>2.63912</v>
+        <v>2.58434</v>
       </c>
     </row>
     <row r="43">
@@ -1463,16 +1463,16 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1</v>
+        <v>1.001</v>
       </c>
       <c r="D43" t="n">
-        <v>3439078996</v>
+        <v>3443652111</v>
       </c>
       <c r="E43" t="n">
-        <v>154364886</v>
+        <v>154533119</v>
       </c>
       <c r="F43" t="n">
-        <v>-0.00669</v>
+        <v>-0.07159</v>
       </c>
     </row>
     <row r="44">
@@ -1487,16 +1487,16 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>3.4</v>
+        <v>3.38</v>
       </c>
       <c r="D44" t="n">
-        <v>3396851368</v>
+        <v>3386517689</v>
       </c>
       <c r="E44" t="n">
-        <v>1281631615</v>
+        <v>1281177864</v>
       </c>
       <c r="F44" t="n">
-        <v>6.78171</v>
+        <v>6.17607</v>
       </c>
     </row>
     <row r="45">
@@ -1511,16 +1511,16 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3.72</v>
+        <v>3.71</v>
       </c>
       <c r="D45" t="n">
-        <v>3361552390</v>
+        <v>3344314078</v>
       </c>
       <c r="E45" t="n">
-        <v>301693729</v>
+        <v>301495698</v>
       </c>
       <c r="F45" t="n">
-        <v>2.64148</v>
+        <v>2.17889</v>
       </c>
     </row>
     <row r="46">
@@ -1538,13 +1538,13 @@
         <v>1.28</v>
       </c>
       <c r="D46" t="n">
-        <v>3337822225</v>
+        <v>3339864365</v>
       </c>
       <c r="E46" t="n">
-        <v>488298136</v>
+        <v>485294902</v>
       </c>
       <c r="F46" t="n">
-        <v>2.42598</v>
+        <v>2.29024</v>
       </c>
     </row>
     <row r="47">
@@ -1559,16 +1559,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.787967</v>
+        <v>0.78912</v>
       </c>
       <c r="D47" t="n">
-        <v>3226906040</v>
+        <v>3234863626</v>
       </c>
       <c r="E47" t="n">
-        <v>1668181094</v>
+        <v>1667684113</v>
       </c>
       <c r="F47" t="n">
-        <v>12.37254</v>
+        <v>12.79568</v>
       </c>
     </row>
     <row r="48">
@@ -1583,16 +1583,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>160.67</v>
+        <v>161.42</v>
       </c>
       <c r="D48" t="n">
-        <v>2963867990</v>
+        <v>2970687075</v>
       </c>
       <c r="E48" t="n">
-        <v>83352737</v>
+        <v>86854554</v>
       </c>
       <c r="F48" t="n">
-        <v>-1.78004</v>
+        <v>-1.16649</v>
       </c>
     </row>
     <row r="49">
@@ -1607,16 +1607,16 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1.95</v>
+        <v>1.96</v>
       </c>
       <c r="D49" t="n">
-        <v>2933339796</v>
+        <v>2941098154</v>
       </c>
       <c r="E49" t="n">
-        <v>368223956</v>
+        <v>367168437</v>
       </c>
       <c r="F49" t="n">
-        <v>0.21023</v>
+        <v>0.98808</v>
       </c>
     </row>
     <row r="50">
@@ -1631,16 +1631,16 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.846624</v>
+        <v>0.847303</v>
       </c>
       <c r="D50" t="n">
-        <v>2850586086</v>
+        <v>2838053749</v>
       </c>
       <c r="E50" t="n">
-        <v>183686556</v>
+        <v>185133243</v>
       </c>
       <c r="F50" t="n">
-        <v>15.21575</v>
+        <v>15.30567</v>
       </c>
     </row>
     <row r="51">
@@ -1655,16 +1655,16 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>4.71</v>
+        <v>4.7</v>
       </c>
       <c r="D51" t="n">
-        <v>2828845966</v>
+        <v>2819630872</v>
       </c>
       <c r="E51" t="n">
-        <v>583490036</v>
+        <v>581494444</v>
       </c>
       <c r="F51" t="n">
-        <v>7.03179</v>
+        <v>6.70952</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1953772577503</v>
+        <v>1959195618520</v>
       </c>
     </row>
     <row r="3">
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>407043413496</v>
+        <v>408077072603</v>
       </c>
     </row>
     <row r="4">
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>130788831244</v>
+        <v>130946260507</v>
       </c>
     </row>
     <row r="5">
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>124075895781</v>
+        <v>124537701624</v>
       </c>
     </row>
     <row r="6">
@@ -1745,7 +1745,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>92676534988</v>
+        <v>92774471217</v>
       </c>
     </row>
   </sheetData>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$4355.88</t>
+          <t>$4363.16</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>XRP (24.18%)</t>
+          <t>XRP (24.45%)</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bitcoin Cash (-3.06%)</t>
+          <t>Bitcoin Cash (-3.24%)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Excel data - 2024-11-22 05:46:29
</commit_message>
<xml_diff>
--- a/crypto_live_data.xlsx
+++ b/crypto_live_data.xlsx
@@ -479,16 +479,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>99049</v>
+        <v>98973</v>
       </c>
       <c r="D2" t="n">
-        <v>1959195618520</v>
+        <v>1960031497170</v>
       </c>
       <c r="E2" t="n">
-        <v>112637342948</v>
+        <v>112063105617</v>
       </c>
       <c r="F2" t="n">
-        <v>1.23955</v>
+        <v>1.34469</v>
       </c>
     </row>
     <row r="3">
@@ -503,16 +503,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3387.32</v>
+        <v>3391.73</v>
       </c>
       <c r="D3" t="n">
-        <v>408077072603</v>
+        <v>408586496268</v>
       </c>
       <c r="E3" t="n">
-        <v>56006401370</v>
+        <v>57188238984</v>
       </c>
       <c r="F3" t="n">
-        <v>8.157629999999999</v>
+        <v>8.5235</v>
       </c>
     </row>
     <row r="4">
@@ -530,13 +530,13 @@
         <v>1.001</v>
       </c>
       <c r="D4" t="n">
-        <v>130946260507</v>
+        <v>130911146723</v>
       </c>
       <c r="E4" t="n">
-        <v>118643630134</v>
+        <v>161208017217</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.04242</v>
+        <v>-0.06610000000000001</v>
       </c>
     </row>
     <row r="5">
@@ -551,16 +551,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>262.45</v>
+        <v>261.97</v>
       </c>
       <c r="D5" t="n">
-        <v>124537701624</v>
+        <v>124520979419</v>
       </c>
       <c r="E5" t="n">
-        <v>14996288932</v>
+        <v>14956566986</v>
       </c>
       <c r="F5" t="n">
-        <v>8.74217</v>
+        <v>8.4557</v>
       </c>
     </row>
     <row r="6">
@@ -575,16 +575,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>635.4299999999999</v>
+        <v>634.28</v>
       </c>
       <c r="D6" t="n">
-        <v>92774471217</v>
+        <v>92589848319</v>
       </c>
       <c r="E6" t="n">
-        <v>2471223191</v>
+        <v>2461265568</v>
       </c>
       <c r="F6" t="n">
-        <v>3.69055</v>
+        <v>3.64408</v>
       </c>
     </row>
     <row r="7">
@@ -599,16 +599,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.39</v>
+        <v>1.4</v>
       </c>
       <c r="D7" t="n">
-        <v>79043620118</v>
+        <v>79352270388</v>
       </c>
       <c r="E7" t="n">
-        <v>17986070520</v>
+        <v>18051002346</v>
       </c>
       <c r="F7" t="n">
-        <v>24.44778</v>
+        <v>24.9139</v>
       </c>
     </row>
     <row r="8">
@@ -623,16 +623,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.396036</v>
+        <v>0.396461</v>
       </c>
       <c r="D8" t="n">
-        <v>58263803542</v>
+        <v>58243325207</v>
       </c>
       <c r="E8" t="n">
-        <v>9818155855</v>
+        <v>9794203793</v>
       </c>
       <c r="F8" t="n">
-        <v>2.05484</v>
+        <v>2.5468</v>
       </c>
     </row>
     <row r="9">
@@ -650,13 +650,13 @@
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>38333818068</v>
+        <v>38324646891</v>
       </c>
       <c r="E9" t="n">
-        <v>10390110683</v>
+        <v>13566669467</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.05674</v>
+        <v>-0.03895</v>
       </c>
     </row>
     <row r="10">
@@ -671,16 +671,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3386.1</v>
+        <v>3393.11</v>
       </c>
       <c r="D10" t="n">
-        <v>33167306357</v>
+        <v>33237192980</v>
       </c>
       <c r="E10" t="n">
-        <v>148210338</v>
+        <v>147411661</v>
       </c>
       <c r="F10" t="n">
-        <v>8.32367</v>
+        <v>8.583399999999999</v>
       </c>
     </row>
     <row r="11">
@@ -695,16 +695,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.884086</v>
+        <v>0.883182</v>
       </c>
       <c r="D11" t="n">
-        <v>31689028378</v>
+        <v>31606335117</v>
       </c>
       <c r="E11" t="n">
-        <v>3620403635</v>
+        <v>3575419706</v>
       </c>
       <c r="F11" t="n">
-        <v>12.00104</v>
+        <v>11.9422</v>
       </c>
     </row>
     <row r="12">
@@ -719,16 +719,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.20032</v>
+        <v>0.200351</v>
       </c>
       <c r="D12" t="n">
-        <v>17312612565</v>
+        <v>17309848780</v>
       </c>
       <c r="E12" t="n">
-        <v>1068387702</v>
+        <v>1067883664</v>
       </c>
       <c r="F12" t="n">
-        <v>1.32711</v>
+        <v>1.44964</v>
       </c>
     </row>
     <row r="13">
@@ -743,16 +743,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>36.33</v>
+        <v>36.41</v>
       </c>
       <c r="D13" t="n">
-        <v>14861570205</v>
+        <v>14894009679</v>
       </c>
       <c r="E13" t="n">
-        <v>1050610416</v>
+        <v>1051408833</v>
       </c>
       <c r="F13" t="n">
-        <v>6.52267</v>
+        <v>6.92825</v>
       </c>
     </row>
     <row r="14">
@@ -767,16 +767,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.499e-05</v>
+        <v>2.501e-05</v>
       </c>
       <c r="D14" t="n">
-        <v>14719052047</v>
+        <v>14744333428</v>
       </c>
       <c r="E14" t="n">
-        <v>1610749228</v>
+        <v>1608726152</v>
       </c>
       <c r="F14" t="n">
-        <v>2.89691</v>
+        <v>3.15487</v>
       </c>
     </row>
     <row r="15">
@@ -791,16 +791,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>4011.57</v>
+        <v>4008.33</v>
       </c>
       <c r="D15" t="n">
-        <v>14487656085</v>
+        <v>14474546253</v>
       </c>
       <c r="E15" t="n">
-        <v>157676278</v>
+        <v>167732168</v>
       </c>
       <c r="F15" t="n">
-        <v>8.152979999999999</v>
+        <v>8.51431</v>
       </c>
     </row>
     <row r="16">
@@ -815,16 +815,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>99016</v>
+        <v>98469</v>
       </c>
       <c r="D16" t="n">
-        <v>14437890938</v>
+        <v>14383538226</v>
       </c>
       <c r="E16" t="n">
-        <v>854187820</v>
+        <v>845619925</v>
       </c>
       <c r="F16" t="n">
-        <v>1.62661</v>
+        <v>1.4294</v>
       </c>
     </row>
     <row r="17">
@@ -842,13 +842,13 @@
         <v>5.56</v>
       </c>
       <c r="D17" t="n">
-        <v>14174714359</v>
+        <v>14174777304</v>
       </c>
       <c r="E17" t="n">
-        <v>638662056</v>
+        <v>637789593</v>
       </c>
       <c r="F17" t="n">
-        <v>3.18693</v>
+        <v>3.41937</v>
       </c>
     </row>
     <row r="18">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3.62</v>
+        <v>3.61</v>
       </c>
       <c r="D18" t="n">
-        <v>10296343269</v>
+        <v>10273657188</v>
       </c>
       <c r="E18" t="n">
-        <v>2081734581</v>
+        <v>2206148805</v>
       </c>
       <c r="F18" t="n">
-        <v>0.5196</v>
+        <v>0.14521</v>
       </c>
     </row>
     <row r="19">
@@ -887,16 +887,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>497.01</v>
+        <v>497.52</v>
       </c>
       <c r="D19" t="n">
-        <v>9820919497</v>
+        <v>9852940247</v>
       </c>
       <c r="E19" t="n">
-        <v>1936718320</v>
+        <v>1909542516</v>
       </c>
       <c r="F19" t="n">
-        <v>-3.23961</v>
+        <v>-4.17898</v>
       </c>
     </row>
     <row r="20">
@@ -911,16 +911,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3386.67</v>
+        <v>3391.08</v>
       </c>
       <c r="D20" t="n">
-        <v>9647766380</v>
+        <v>9719868552</v>
       </c>
       <c r="E20" t="n">
-        <v>1272082578</v>
+        <v>1466024154</v>
       </c>
       <c r="F20" t="n">
-        <v>8.148099999999999</v>
+        <v>8.617419999999999</v>
       </c>
     </row>
     <row r="21">
@@ -935,64 +935,64 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>15.29</v>
+        <v>15.3</v>
       </c>
       <c r="D21" t="n">
-        <v>9589028913</v>
+        <v>9590618652</v>
       </c>
       <c r="E21" t="n">
-        <v>1250243694</v>
+        <v>1256306565</v>
       </c>
       <c r="F21" t="n">
-        <v>4.19627</v>
+        <v>4.37437</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>dot</t>
+          <t>pepe</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>6.22</v>
+        <v>2.138e-05</v>
       </c>
       <c r="D22" t="n">
-        <v>8950792803</v>
+        <v>8992937206</v>
       </c>
       <c r="E22" t="n">
-        <v>828809348</v>
+        <v>6818526335</v>
       </c>
       <c r="F22" t="n">
-        <v>8.66395</v>
+        <v>9.91516</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>pepe</t>
+          <t>dot</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2.129e-05</v>
+        <v>6.23</v>
       </c>
       <c r="D23" t="n">
-        <v>8947854713</v>
+        <v>8988502483</v>
       </c>
       <c r="E23" t="n">
-        <v>6816364706</v>
+        <v>830212815</v>
       </c>
       <c r="F23" t="n">
-        <v>9.08339</v>
+        <v>9.276669999999999</v>
       </c>
     </row>
     <row r="24">
@@ -1007,16 +1007,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.283467</v>
+        <v>0.283394</v>
       </c>
       <c r="D24" t="n">
-        <v>8476827049</v>
+        <v>8500667311</v>
       </c>
       <c r="E24" t="n">
-        <v>2299577623</v>
+        <v>2299576081</v>
       </c>
       <c r="F24" t="n">
-        <v>18.22379</v>
+        <v>19.34584</v>
       </c>
     </row>
     <row r="25">
@@ -1031,16 +1031,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>8.800000000000001</v>
+        <v>8.789999999999999</v>
       </c>
       <c r="D25" t="n">
-        <v>8141138033</v>
+        <v>8129859866</v>
       </c>
       <c r="E25" t="n">
-        <v>3450901</v>
+        <v>3437669</v>
       </c>
       <c r="F25" t="n">
-        <v>3.34373</v>
+        <v>3.23414</v>
       </c>
     </row>
     <row r="26">
@@ -1055,16 +1055,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>5.8</v>
+        <v>5.81</v>
       </c>
       <c r="D26" t="n">
-        <v>7070338866</v>
+        <v>7079430306</v>
       </c>
       <c r="E26" t="n">
-        <v>1011815621</v>
+        <v>1013157831</v>
       </c>
       <c r="F26" t="n">
-        <v>4.29611</v>
+        <v>4.4035</v>
       </c>
     </row>
     <row r="27">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>90.54000000000001</v>
+        <v>90.98999999999999</v>
       </c>
       <c r="D27" t="n">
-        <v>6809385663</v>
+        <v>6843655404</v>
       </c>
       <c r="E27" t="n">
-        <v>1413117460</v>
+        <v>1421163417</v>
       </c>
       <c r="F27" t="n">
-        <v>4.08485</v>
+        <v>4.39455</v>
       </c>
     </row>
     <row r="28">
@@ -1103,16 +1103,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>12.13</v>
+        <v>12.15</v>
       </c>
       <c r="D28" t="n">
-        <v>6470864453</v>
+        <v>6471704530</v>
       </c>
       <c r="E28" t="n">
-        <v>865197468</v>
+        <v>863170407</v>
       </c>
       <c r="F28" t="n">
-        <v>3.80178</v>
+        <v>3.58351</v>
       </c>
     </row>
     <row r="29">
@@ -1127,16 +1127,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3568.39</v>
+        <v>3572.68</v>
       </c>
       <c r="D29" t="n">
-        <v>6207201257</v>
+        <v>6215050475</v>
       </c>
       <c r="E29" t="n">
-        <v>104283760</v>
+        <v>105919148</v>
       </c>
       <c r="F29" t="n">
-        <v>8.14161</v>
+        <v>8.699859999999999</v>
       </c>
     </row>
     <row r="30">
@@ -1151,16 +1151,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9.41</v>
+        <v>9.449999999999999</v>
       </c>
       <c r="D30" t="n">
-        <v>5652647882</v>
+        <v>5675174761</v>
       </c>
       <c r="E30" t="n">
-        <v>861384256</v>
+        <v>867407640</v>
       </c>
       <c r="F30" t="n">
-        <v>5.93018</v>
+        <v>6.44424</v>
       </c>
     </row>
     <row r="31">
@@ -1175,16 +1175,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.200382</v>
+        <v>0.203407</v>
       </c>
       <c r="D31" t="n">
-        <v>5446042457</v>
+        <v>5518803426</v>
       </c>
       <c r="E31" t="n">
-        <v>126658464</v>
+        <v>130186401</v>
       </c>
       <c r="F31" t="n">
-        <v>14.08539</v>
+        <v>15.95664</v>
       </c>
     </row>
     <row r="32">
@@ -1199,16 +1199,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1.002</v>
+        <v>0.99739</v>
       </c>
       <c r="D32" t="n">
-        <v>5226148199</v>
+        <v>5219437344</v>
       </c>
       <c r="E32" t="n">
-        <v>16537152</v>
+        <v>91138</v>
       </c>
       <c r="F32" t="n">
-        <v>0.00528</v>
+        <v>-0.41544</v>
       </c>
     </row>
     <row r="33">
@@ -1223,16 +1223,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.133661</v>
+        <v>0.132838</v>
       </c>
       <c r="D33" t="n">
-        <v>5102145955</v>
+        <v>5102360242</v>
       </c>
       <c r="E33" t="n">
-        <v>895575078</v>
+        <v>902012626</v>
       </c>
       <c r="F33" t="n">
-        <v>5.98247</v>
+        <v>5.76491</v>
       </c>
     </row>
     <row r="34">
@@ -1247,16 +1247,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9.630000000000001</v>
+        <v>9.65</v>
       </c>
       <c r="D34" t="n">
-        <v>4568754468</v>
+        <v>4574959826</v>
       </c>
       <c r="E34" t="n">
-        <v>274366712</v>
+        <v>274551581</v>
       </c>
       <c r="F34" t="n">
-        <v>5.80122</v>
+        <v>6.2297</v>
       </c>
     </row>
     <row r="35">
@@ -1271,16 +1271,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>27.99</v>
+        <v>28.08</v>
       </c>
       <c r="D35" t="n">
-        <v>4188436495</v>
+        <v>4200949688</v>
       </c>
       <c r="E35" t="n">
-        <v>882892358</v>
+        <v>877961705</v>
       </c>
       <c r="F35" t="n">
-        <v>5.20897</v>
+        <v>5.00049</v>
       </c>
     </row>
     <row r="36">
@@ -1295,64 +1295,64 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>5.195e-05</v>
+        <v>5.21e-05</v>
       </c>
       <c r="D36" t="n">
-        <v>3901989396</v>
+        <v>3909767343</v>
       </c>
       <c r="E36" t="n">
-        <v>1682777811</v>
+        <v>1680780764</v>
       </c>
       <c r="F36" t="n">
-        <v>2.20426</v>
+        <v>2.43461</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>kas</t>
+          <t>render</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.151353</v>
+        <v>7.4</v>
       </c>
       <c r="D37" t="n">
-        <v>3817573608</v>
+        <v>3830524194</v>
       </c>
       <c r="E37" t="n">
-        <v>151839983</v>
+        <v>435811535</v>
       </c>
       <c r="F37" t="n">
-        <v>-0.79223</v>
+        <v>0.63923</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>render</t>
+          <t>kas</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>7.38</v>
+        <v>0.151489</v>
       </c>
       <c r="D38" t="n">
-        <v>3817395639</v>
+        <v>3821068085</v>
       </c>
       <c r="E38" t="n">
-        <v>434850443</v>
+        <v>151494380</v>
       </c>
       <c r="F38" t="n">
-        <v>-0.12395</v>
+        <v>-0.29508</v>
       </c>
     </row>
     <row r="39">
@@ -1367,16 +1367,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.472771</v>
+        <v>0.473954</v>
       </c>
       <c r="D39" t="n">
-        <v>3768901866</v>
+        <v>3779000218</v>
       </c>
       <c r="E39" t="n">
-        <v>491287376</v>
+        <v>492239332</v>
       </c>
       <c r="F39" t="n">
-        <v>7.38356</v>
+        <v>7.932</v>
       </c>
     </row>
     <row r="40">
@@ -1391,16 +1391,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>507.56</v>
+        <v>507.23</v>
       </c>
       <c r="D40" t="n">
-        <v>3757496611</v>
+        <v>3743956169</v>
       </c>
       <c r="E40" t="n">
-        <v>284629438</v>
+        <v>283850524</v>
       </c>
       <c r="F40" t="n">
-        <v>3.05338</v>
+        <v>2.43937</v>
       </c>
     </row>
     <row r="41">
@@ -1418,13 +1418,13 @@
         <v>1.002</v>
       </c>
       <c r="D41" t="n">
-        <v>3687424253</v>
+        <v>3689800135</v>
       </c>
       <c r="E41" t="n">
-        <v>224417787</v>
+        <v>224694439</v>
       </c>
       <c r="F41" t="n">
-        <v>-0.0735</v>
+        <v>-0.05866</v>
       </c>
     </row>
     <row r="42">
@@ -1439,16 +1439,16 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>24.82</v>
+        <v>24.81</v>
       </c>
       <c r="D42" t="n">
-        <v>3576586417</v>
+        <v>3577004631</v>
       </c>
       <c r="E42" t="n">
-        <v>33415891</v>
+        <v>33482480</v>
       </c>
       <c r="F42" t="n">
-        <v>2.58434</v>
+        <v>2.55998</v>
       </c>
     </row>
     <row r="43">
@@ -1463,16 +1463,16 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1.001</v>
+        <v>0.999814</v>
       </c>
       <c r="D43" t="n">
-        <v>3443652111</v>
+        <v>3444066515</v>
       </c>
       <c r="E43" t="n">
-        <v>154533119</v>
+        <v>154806556</v>
       </c>
       <c r="F43" t="n">
-        <v>-0.07159</v>
+        <v>-0.09016</v>
       </c>
     </row>
     <row r="44">
@@ -1487,16 +1487,16 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>3.38</v>
+        <v>3.4</v>
       </c>
       <c r="D44" t="n">
-        <v>3386517689</v>
+        <v>3387805331</v>
       </c>
       <c r="E44" t="n">
-        <v>1281177864</v>
+        <v>1284980672</v>
       </c>
       <c r="F44" t="n">
-        <v>6.17607</v>
+        <v>6.28501</v>
       </c>
     </row>
     <row r="45">
@@ -1511,16 +1511,16 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3.71</v>
+        <v>3.72</v>
       </c>
       <c r="D45" t="n">
-        <v>3344314078</v>
+        <v>3351839645</v>
       </c>
       <c r="E45" t="n">
-        <v>301495698</v>
+        <v>301332116</v>
       </c>
       <c r="F45" t="n">
-        <v>2.17889</v>
+        <v>3.21506</v>
       </c>
     </row>
     <row r="46">
@@ -1538,13 +1538,13 @@
         <v>1.28</v>
       </c>
       <c r="D46" t="n">
-        <v>3339864365</v>
+        <v>3344641105</v>
       </c>
       <c r="E46" t="n">
-        <v>485294902</v>
+        <v>485928047</v>
       </c>
       <c r="F46" t="n">
-        <v>2.29024</v>
+        <v>2.65695</v>
       </c>
     </row>
     <row r="47">
@@ -1559,16 +1559,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.78912</v>
+        <v>0.792956</v>
       </c>
       <c r="D47" t="n">
-        <v>3234863626</v>
+        <v>3248313579</v>
       </c>
       <c r="E47" t="n">
-        <v>1667684113</v>
+        <v>1672915093</v>
       </c>
       <c r="F47" t="n">
-        <v>12.79568</v>
+        <v>13.78308</v>
       </c>
     </row>
     <row r="48">
@@ -1583,16 +1583,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>161.42</v>
+        <v>161.3</v>
       </c>
       <c r="D48" t="n">
-        <v>2970687075</v>
+        <v>2977336240</v>
       </c>
       <c r="E48" t="n">
-        <v>86854554</v>
+        <v>84382065</v>
       </c>
       <c r="F48" t="n">
-        <v>-1.16649</v>
+        <v>-0.91428</v>
       </c>
     </row>
     <row r="49">
@@ -1610,13 +1610,13 @@
         <v>1.96</v>
       </c>
       <c r="D49" t="n">
-        <v>2941098154</v>
+        <v>2948469908</v>
       </c>
       <c r="E49" t="n">
-        <v>367168437</v>
+        <v>364748635</v>
       </c>
       <c r="F49" t="n">
-        <v>0.98808</v>
+        <v>1.20934</v>
       </c>
     </row>
     <row r="50">
@@ -1631,16 +1631,16 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.847303</v>
+        <v>0.847034</v>
       </c>
       <c r="D50" t="n">
-        <v>2838053749</v>
+        <v>2856006968</v>
       </c>
       <c r="E50" t="n">
-        <v>185133243</v>
+        <v>185488113</v>
       </c>
       <c r="F50" t="n">
-        <v>15.30567</v>
+        <v>15.42842</v>
       </c>
     </row>
     <row r="51">
@@ -1655,16 +1655,16 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>4.7</v>
+        <v>4.72</v>
       </c>
       <c r="D51" t="n">
-        <v>2819630872</v>
+        <v>2833166913</v>
       </c>
       <c r="E51" t="n">
-        <v>581494444</v>
+        <v>579787658</v>
       </c>
       <c r="F51" t="n">
-        <v>6.70952</v>
+        <v>7.26919</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1959195618520</v>
+        <v>1960031497170</v>
       </c>
     </row>
     <row r="3">
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>408077072603</v>
+        <v>408586496268</v>
       </c>
     </row>
     <row r="4">
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>130946260507</v>
+        <v>130911146723</v>
       </c>
     </row>
     <row r="5">
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>124537701624</v>
+        <v>124520979419</v>
       </c>
     </row>
     <row r="6">
@@ -1745,7 +1745,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>92774471217</v>
+        <v>92589848319</v>
       </c>
     </row>
   </sheetData>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$4363.16</t>
+          <t>$4351.03</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>XRP (24.45%)</t>
+          <t>XRP (24.91%)</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bitcoin Cash (-3.24%)</t>
+          <t>Bitcoin Cash (-4.18%)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Excel data - 2024-11-22 06:01:32
</commit_message>
<xml_diff>
--- a/crypto_live_data.xlsx
+++ b/crypto_live_data.xlsx
@@ -479,16 +479,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>98973</v>
+        <v>98950</v>
       </c>
       <c r="D2" t="n">
-        <v>1960031497170</v>
+        <v>1957801914152</v>
       </c>
       <c r="E2" t="n">
-        <v>112063105617</v>
+        <v>99838698778</v>
       </c>
       <c r="F2" t="n">
-        <v>1.34469</v>
+        <v>2.0972</v>
       </c>
     </row>
     <row r="3">
@@ -503,16 +503,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3391.73</v>
+        <v>3389.14</v>
       </c>
       <c r="D3" t="n">
-        <v>408586496268</v>
+        <v>408183778081</v>
       </c>
       <c r="E3" t="n">
-        <v>57188238984</v>
+        <v>57101803551</v>
       </c>
       <c r="F3" t="n">
-        <v>8.5235</v>
+        <v>9.253769999999999</v>
       </c>
     </row>
     <row r="4">
@@ -530,13 +530,13 @@
         <v>1.001</v>
       </c>
       <c r="D4" t="n">
-        <v>130911146723</v>
+        <v>130823802841</v>
       </c>
       <c r="E4" t="n">
-        <v>161208017217</v>
+        <v>191268654241</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.06610000000000001</v>
+        <v>0.32316</v>
       </c>
     </row>
     <row r="5">
@@ -551,16 +551,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>261.97</v>
+        <v>261.36</v>
       </c>
       <c r="D5" t="n">
-        <v>124520979419</v>
+        <v>124099389605</v>
       </c>
       <c r="E5" t="n">
-        <v>14956566986</v>
+        <v>14903347184</v>
       </c>
       <c r="F5" t="n">
-        <v>8.4557</v>
+        <v>9.29208</v>
       </c>
     </row>
     <row r="6">
@@ -575,16 +575,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>634.28</v>
+        <v>633.61</v>
       </c>
       <c r="D6" t="n">
-        <v>92589848319</v>
+        <v>92441290124</v>
       </c>
       <c r="E6" t="n">
-        <v>2461265568</v>
+        <v>2462097536</v>
       </c>
       <c r="F6" t="n">
-        <v>3.64408</v>
+        <v>4.16909</v>
       </c>
     </row>
     <row r="7">
@@ -602,13 +602,13 @@
         <v>1.4</v>
       </c>
       <c r="D7" t="n">
-        <v>79352270388</v>
+        <v>79890440378</v>
       </c>
       <c r="E7" t="n">
-        <v>18051002346</v>
+        <v>18216983753</v>
       </c>
       <c r="F7" t="n">
-        <v>24.9139</v>
+        <v>26.85773</v>
       </c>
     </row>
     <row r="8">
@@ -623,16 +623,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.396461</v>
+        <v>0.396715</v>
       </c>
       <c r="D8" t="n">
-        <v>58243325207</v>
+        <v>58265317109</v>
       </c>
       <c r="E8" t="n">
-        <v>9794203793</v>
+        <v>9787067581</v>
       </c>
       <c r="F8" t="n">
-        <v>2.5468</v>
+        <v>3.75439</v>
       </c>
     </row>
     <row r="9">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0.999911</v>
       </c>
       <c r="D9" t="n">
-        <v>38324646891</v>
+        <v>38332070800</v>
       </c>
       <c r="E9" t="n">
-        <v>13566669467</v>
+        <v>8044180063</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.03895</v>
+        <v>0.38615</v>
       </c>
     </row>
     <row r="10">
@@ -671,16 +671,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3393.11</v>
+        <v>3387.07</v>
       </c>
       <c r="D10" t="n">
-        <v>33237192980</v>
+        <v>33211105579</v>
       </c>
       <c r="E10" t="n">
-        <v>147411661</v>
+        <v>145751955</v>
       </c>
       <c r="F10" t="n">
-        <v>8.583399999999999</v>
+        <v>9.066129999999999</v>
       </c>
     </row>
     <row r="11">
@@ -695,16 +695,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.883182</v>
+        <v>0.882131</v>
       </c>
       <c r="D11" t="n">
-        <v>31606335117</v>
+        <v>31574566650</v>
       </c>
       <c r="E11" t="n">
-        <v>3575419706</v>
+        <v>3012421450</v>
       </c>
       <c r="F11" t="n">
-        <v>11.9422</v>
+        <v>12.58447</v>
       </c>
     </row>
     <row r="12">
@@ -719,16 +719,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.200351</v>
+        <v>0.200153</v>
       </c>
       <c r="D12" t="n">
-        <v>17309848780</v>
+        <v>17285755290</v>
       </c>
       <c r="E12" t="n">
-        <v>1067883664</v>
+        <v>1062451930</v>
       </c>
       <c r="F12" t="n">
-        <v>1.44964</v>
+        <v>1.88472</v>
       </c>
     </row>
     <row r="13">
@@ -743,16 +743,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>36.41</v>
+        <v>36.38</v>
       </c>
       <c r="D13" t="n">
-        <v>14894009679</v>
+        <v>14894142924</v>
       </c>
       <c r="E13" t="n">
-        <v>1051408833</v>
+        <v>1049098992</v>
       </c>
       <c r="F13" t="n">
-        <v>6.92825</v>
+        <v>7.78136</v>
       </c>
     </row>
     <row r="14">
@@ -770,13 +770,13 @@
         <v>2.501e-05</v>
       </c>
       <c r="D14" t="n">
-        <v>14744333428</v>
+        <v>14745167792</v>
       </c>
       <c r="E14" t="n">
-        <v>1608726152</v>
+        <v>1599456205</v>
       </c>
       <c r="F14" t="n">
-        <v>3.15487</v>
+        <v>4.18302</v>
       </c>
     </row>
     <row r="15">
@@ -791,16 +791,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>4008.33</v>
+        <v>4011.1</v>
       </c>
       <c r="D15" t="n">
-        <v>14474546253</v>
+        <v>14487010535</v>
       </c>
       <c r="E15" t="n">
-        <v>167732168</v>
+        <v>169572218</v>
       </c>
       <c r="F15" t="n">
-        <v>8.51431</v>
+        <v>9.07639</v>
       </c>
     </row>
     <row r="16">
@@ -815,16 +815,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>98469</v>
+        <v>98859</v>
       </c>
       <c r="D16" t="n">
-        <v>14383538226</v>
+        <v>14444416042</v>
       </c>
       <c r="E16" t="n">
-        <v>845619925</v>
+        <v>847328202</v>
       </c>
       <c r="F16" t="n">
-        <v>1.4294</v>
+        <v>2.29471</v>
       </c>
     </row>
     <row r="17">
@@ -842,13 +842,13 @@
         <v>5.56</v>
       </c>
       <c r="D17" t="n">
-        <v>14174777304</v>
+        <v>14159481773</v>
       </c>
       <c r="E17" t="n">
-        <v>637789593</v>
+        <v>637235491</v>
       </c>
       <c r="F17" t="n">
-        <v>3.41937</v>
+        <v>4.09133</v>
       </c>
     </row>
     <row r="18">
@@ -866,13 +866,13 @@
         <v>3.61</v>
       </c>
       <c r="D18" t="n">
-        <v>10273657188</v>
+        <v>10273589779</v>
       </c>
       <c r="E18" t="n">
-        <v>2206148805</v>
+        <v>2444539501</v>
       </c>
       <c r="F18" t="n">
-        <v>0.14521</v>
+        <v>1.08414</v>
       </c>
     </row>
     <row r="19">
@@ -887,16 +887,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>497.52</v>
+        <v>498.78</v>
       </c>
       <c r="D19" t="n">
-        <v>9852940247</v>
+        <v>9871422041</v>
       </c>
       <c r="E19" t="n">
-        <v>1909542516</v>
+        <v>1867669705</v>
       </c>
       <c r="F19" t="n">
-        <v>-4.17898</v>
+        <v>-2.15394</v>
       </c>
     </row>
     <row r="20">
@@ -911,16 +911,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3391.08</v>
+        <v>3392</v>
       </c>
       <c r="D20" t="n">
-        <v>9719868552</v>
+        <v>9734929278</v>
       </c>
       <c r="E20" t="n">
-        <v>1466024154</v>
+        <v>2223032283</v>
       </c>
       <c r="F20" t="n">
-        <v>8.617419999999999</v>
+        <v>9.49335</v>
       </c>
     </row>
     <row r="21">
@@ -938,13 +938,13 @@
         <v>15.3</v>
       </c>
       <c r="D21" t="n">
-        <v>9590618652</v>
+        <v>9592025550</v>
       </c>
       <c r="E21" t="n">
-        <v>1256306565</v>
+        <v>1257405474</v>
       </c>
       <c r="F21" t="n">
-        <v>4.37437</v>
+        <v>5.48991</v>
       </c>
     </row>
     <row r="22">
@@ -962,13 +962,13 @@
         <v>2.138e-05</v>
       </c>
       <c r="D22" t="n">
-        <v>8992937206</v>
+        <v>8996309587</v>
       </c>
       <c r="E22" t="n">
-        <v>6818526335</v>
+        <v>6804659980</v>
       </c>
       <c r="F22" t="n">
-        <v>9.91516</v>
+        <v>10.57673</v>
       </c>
     </row>
     <row r="23">
@@ -983,16 +983,16 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>6.23</v>
+        <v>6.22</v>
       </c>
       <c r="D23" t="n">
-        <v>8988502483</v>
+        <v>8965227660</v>
       </c>
       <c r="E23" t="n">
-        <v>830212815</v>
+        <v>830110510</v>
       </c>
       <c r="F23" t="n">
-        <v>9.276669999999999</v>
+        <v>10.00362</v>
       </c>
     </row>
     <row r="24">
@@ -1007,16 +1007,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.283394</v>
+        <v>0.285028</v>
       </c>
       <c r="D24" t="n">
-        <v>8500667311</v>
+        <v>8544502079</v>
       </c>
       <c r="E24" t="n">
-        <v>2299576081</v>
+        <v>2312821480</v>
       </c>
       <c r="F24" t="n">
-        <v>19.34584</v>
+        <v>21.06954</v>
       </c>
     </row>
     <row r="25">
@@ -1031,16 +1031,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>8.789999999999999</v>
+        <v>8.81</v>
       </c>
       <c r="D25" t="n">
-        <v>8129859866</v>
+        <v>8122298571</v>
       </c>
       <c r="E25" t="n">
-        <v>3437669</v>
+        <v>3437792</v>
       </c>
       <c r="F25" t="n">
-        <v>3.23414</v>
+        <v>4.04549</v>
       </c>
     </row>
     <row r="26">
@@ -1055,16 +1055,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>5.81</v>
+        <v>5.82</v>
       </c>
       <c r="D26" t="n">
-        <v>7079430306</v>
+        <v>7088167865</v>
       </c>
       <c r="E26" t="n">
-        <v>1013157831</v>
+        <v>1012128839</v>
       </c>
       <c r="F26" t="n">
-        <v>4.4035</v>
+        <v>5.59196</v>
       </c>
     </row>
     <row r="27">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>90.98999999999999</v>
+        <v>90.94</v>
       </c>
       <c r="D27" t="n">
-        <v>6843655404</v>
+        <v>6841601458</v>
       </c>
       <c r="E27" t="n">
-        <v>1421163417</v>
+        <v>1410008469</v>
       </c>
       <c r="F27" t="n">
-        <v>4.39455</v>
+        <v>5.26465</v>
       </c>
     </row>
     <row r="28">
@@ -1103,16 +1103,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>12.15</v>
+        <v>12.14</v>
       </c>
       <c r="D28" t="n">
-        <v>6471704530</v>
+        <v>6471544641</v>
       </c>
       <c r="E28" t="n">
-        <v>863170407</v>
+        <v>859704634</v>
       </c>
       <c r="F28" t="n">
-        <v>3.58351</v>
+        <v>4.33772</v>
       </c>
     </row>
     <row r="29">
@@ -1127,16 +1127,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3572.68</v>
+        <v>3576.2</v>
       </c>
       <c r="D29" t="n">
-        <v>6215050475</v>
+        <v>6220401781</v>
       </c>
       <c r="E29" t="n">
-        <v>105919148</v>
+        <v>106018794</v>
       </c>
       <c r="F29" t="n">
-        <v>8.699859999999999</v>
+        <v>9.409129999999999</v>
       </c>
     </row>
     <row r="30">
@@ -1151,16 +1151,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9.449999999999999</v>
+        <v>9.41</v>
       </c>
       <c r="D30" t="n">
-        <v>5675174761</v>
+        <v>5655338943</v>
       </c>
       <c r="E30" t="n">
-        <v>867407640</v>
+        <v>866236092</v>
       </c>
       <c r="F30" t="n">
-        <v>6.44424</v>
+        <v>6.92099</v>
       </c>
     </row>
     <row r="31">
@@ -1175,16 +1175,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.203407</v>
+        <v>0.203305</v>
       </c>
       <c r="D31" t="n">
-        <v>5518803426</v>
+        <v>5504574071</v>
       </c>
       <c r="E31" t="n">
-        <v>130186401</v>
+        <v>132475693</v>
       </c>
       <c r="F31" t="n">
-        <v>15.95664</v>
+        <v>16.57485</v>
       </c>
     </row>
     <row r="32">
@@ -1199,16 +1199,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.99739</v>
+        <v>0.99746</v>
       </c>
       <c r="D32" t="n">
-        <v>5219437344</v>
+        <v>5229388035</v>
       </c>
       <c r="E32" t="n">
-        <v>91138</v>
+        <v>91130</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.41544</v>
+        <v>0.04723</v>
       </c>
     </row>
     <row r="33">
@@ -1223,16 +1223,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.132838</v>
+        <v>0.133813</v>
       </c>
       <c r="D33" t="n">
-        <v>5102360242</v>
+        <v>5110910421</v>
       </c>
       <c r="E33" t="n">
-        <v>902012626</v>
+        <v>907416623</v>
       </c>
       <c r="F33" t="n">
-        <v>5.76491</v>
+        <v>8.14057</v>
       </c>
     </row>
     <row r="34">
@@ -1247,16 +1247,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9.65</v>
+        <v>9.640000000000001</v>
       </c>
       <c r="D34" t="n">
-        <v>4574959826</v>
+        <v>4572289134</v>
       </c>
       <c r="E34" t="n">
-        <v>274551581</v>
+        <v>274975740</v>
       </c>
       <c r="F34" t="n">
-        <v>6.2297</v>
+        <v>7.32213</v>
       </c>
     </row>
     <row r="35">
@@ -1271,16 +1271,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>28.08</v>
+        <v>28.1</v>
       </c>
       <c r="D35" t="n">
-        <v>4200949688</v>
+        <v>4205261170</v>
       </c>
       <c r="E35" t="n">
-        <v>877961705</v>
+        <v>871015505</v>
       </c>
       <c r="F35" t="n">
-        <v>5.00049</v>
+        <v>6.17713</v>
       </c>
     </row>
     <row r="36">
@@ -1295,64 +1295,64 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>5.21e-05</v>
+        <v>5.213e-05</v>
       </c>
       <c r="D36" t="n">
-        <v>3909767343</v>
+        <v>3915257516</v>
       </c>
       <c r="E36" t="n">
-        <v>1680780764</v>
+        <v>1670661215</v>
       </c>
       <c r="F36" t="n">
-        <v>2.43461</v>
+        <v>2.57426</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Render</t>
+          <t>Kaspa</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>render</t>
+          <t>kas</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>7.4</v>
+        <v>0.152234</v>
       </c>
       <c r="D37" t="n">
-        <v>3830524194</v>
+        <v>3835490531</v>
       </c>
       <c r="E37" t="n">
-        <v>435811535</v>
+        <v>151673221</v>
       </c>
       <c r="F37" t="n">
-        <v>0.63923</v>
+        <v>1.06944</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Kaspa</t>
+          <t>Render</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>kas</t>
+          <t>render</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.151489</v>
+        <v>7.41</v>
       </c>
       <c r="D38" t="n">
-        <v>3821068085</v>
+        <v>3835014471</v>
       </c>
       <c r="E38" t="n">
-        <v>151494380</v>
+        <v>432564798</v>
       </c>
       <c r="F38" t="n">
-        <v>-0.29508</v>
+        <v>1.19444</v>
       </c>
     </row>
     <row r="39">
@@ -1367,16 +1367,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.473954</v>
+        <v>0.473232</v>
       </c>
       <c r="D39" t="n">
-        <v>3779000218</v>
+        <v>3772214715</v>
       </c>
       <c r="E39" t="n">
-        <v>492239332</v>
+        <v>476956609</v>
       </c>
       <c r="F39" t="n">
-        <v>7.932</v>
+        <v>8.94638</v>
       </c>
     </row>
     <row r="40">
@@ -1391,16 +1391,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>507.23</v>
+        <v>504.62</v>
       </c>
       <c r="D40" t="n">
-        <v>3743956169</v>
+        <v>3728030742</v>
       </c>
       <c r="E40" t="n">
-        <v>283850524</v>
+        <v>282237842</v>
       </c>
       <c r="F40" t="n">
-        <v>2.43937</v>
+        <v>2.92676</v>
       </c>
     </row>
     <row r="41">
@@ -1418,13 +1418,13 @@
         <v>1.002</v>
       </c>
       <c r="D41" t="n">
-        <v>3689800135</v>
+        <v>3688538085</v>
       </c>
       <c r="E41" t="n">
-        <v>224694439</v>
+        <v>225145685</v>
       </c>
       <c r="F41" t="n">
-        <v>-0.05866</v>
+        <v>-0.05451</v>
       </c>
     </row>
     <row r="42">
@@ -1442,13 +1442,13 @@
         <v>24.81</v>
       </c>
       <c r="D42" t="n">
-        <v>3577004631</v>
+        <v>3575035917</v>
       </c>
       <c r="E42" t="n">
-        <v>33482480</v>
+        <v>33355617</v>
       </c>
       <c r="F42" t="n">
-        <v>2.55998</v>
+        <v>3.25778</v>
       </c>
     </row>
     <row r="43">
@@ -1463,16 +1463,16 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.999814</v>
+        <v>0.999623</v>
       </c>
       <c r="D43" t="n">
-        <v>3444066515</v>
+        <v>3440873426</v>
       </c>
       <c r="E43" t="n">
-        <v>154806556</v>
+        <v>153373746</v>
       </c>
       <c r="F43" t="n">
-        <v>-0.09016</v>
+        <v>0.32737</v>
       </c>
     </row>
     <row r="44">
@@ -1487,16 +1487,16 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>3.4</v>
+        <v>3.39</v>
       </c>
       <c r="D44" t="n">
-        <v>3387805331</v>
+        <v>3388980858</v>
       </c>
       <c r="E44" t="n">
-        <v>1284980672</v>
+        <v>1282763387</v>
       </c>
       <c r="F44" t="n">
-        <v>6.28501</v>
+        <v>6.66468</v>
       </c>
     </row>
     <row r="45">
@@ -1511,16 +1511,16 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3.72</v>
+        <v>3.73</v>
       </c>
       <c r="D45" t="n">
-        <v>3351839645</v>
+        <v>3363633788</v>
       </c>
       <c r="E45" t="n">
-        <v>301332116</v>
+        <v>301881074</v>
       </c>
       <c r="F45" t="n">
-        <v>3.21506</v>
+        <v>4.29752</v>
       </c>
     </row>
     <row r="46">
@@ -1538,13 +1538,13 @@
         <v>1.28</v>
       </c>
       <c r="D46" t="n">
-        <v>3344641105</v>
+        <v>3347597945</v>
       </c>
       <c r="E46" t="n">
-        <v>485928047</v>
+        <v>485036679</v>
       </c>
       <c r="F46" t="n">
-        <v>2.65695</v>
+        <v>3.18392</v>
       </c>
     </row>
     <row r="47">
@@ -1559,16 +1559,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.792956</v>
+        <v>0.792019</v>
       </c>
       <c r="D47" t="n">
-        <v>3248313579</v>
+        <v>3245886344</v>
       </c>
       <c r="E47" t="n">
-        <v>1672915093</v>
+        <v>1672660052</v>
       </c>
       <c r="F47" t="n">
-        <v>13.78308</v>
+        <v>14.82186</v>
       </c>
     </row>
     <row r="48">
@@ -1583,16 +1583,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>161.3</v>
+        <v>161.12</v>
       </c>
       <c r="D48" t="n">
-        <v>2977336240</v>
+        <v>2972253972</v>
       </c>
       <c r="E48" t="n">
-        <v>84382065</v>
+        <v>86424934</v>
       </c>
       <c r="F48" t="n">
-        <v>-0.91428</v>
+        <v>-0.18419</v>
       </c>
     </row>
     <row r="49">
@@ -1607,16 +1607,16 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1.96</v>
+        <v>1.97</v>
       </c>
       <c r="D49" t="n">
-        <v>2948469908</v>
+        <v>2958504435</v>
       </c>
       <c r="E49" t="n">
-        <v>364748635</v>
+        <v>358440221</v>
       </c>
       <c r="F49" t="n">
-        <v>1.20934</v>
+        <v>3.285</v>
       </c>
     </row>
     <row r="50">
@@ -1631,16 +1631,16 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.847034</v>
+        <v>0.8428</v>
       </c>
       <c r="D50" t="n">
-        <v>2856006968</v>
+        <v>2837535662</v>
       </c>
       <c r="E50" t="n">
-        <v>185488113</v>
+        <v>184150203</v>
       </c>
       <c r="F50" t="n">
-        <v>15.42842</v>
+        <v>16.17144</v>
       </c>
     </row>
     <row r="51">
@@ -1655,16 +1655,16 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>4.72</v>
+        <v>4.71</v>
       </c>
       <c r="D51" t="n">
-        <v>2833166913</v>
+        <v>2830209760</v>
       </c>
       <c r="E51" t="n">
-        <v>579787658</v>
+        <v>578155150</v>
       </c>
       <c r="F51" t="n">
-        <v>7.26919</v>
+        <v>8.21808</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1960031497170</v>
+        <v>1957801914152</v>
       </c>
     </row>
     <row r="3">
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>408586496268</v>
+        <v>408183778081</v>
       </c>
     </row>
     <row r="4">
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>130911146723</v>
+        <v>130823802841</v>
       </c>
     </row>
     <row r="5">
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>124520979419</v>
+        <v>124099389605</v>
       </c>
     </row>
     <row r="6">
@@ -1745,7 +1745,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>92589848319</v>
+        <v>92441290124</v>
       </c>
     </row>
   </sheetData>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$4351.03</t>
+          <t>$4358.28</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>XRP (24.91%)</t>
+          <t>XRP (26.86%)</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bitcoin Cash (-4.18%)</t>
+          <t>Bitcoin Cash (-2.15%)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Excel data - 2024-11-22 06:06:33
</commit_message>
<xml_diff>
--- a/crypto_live_data.xlsx
+++ b/crypto_live_data.xlsx
@@ -479,16 +479,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>98950</v>
+        <v>98949</v>
       </c>
       <c r="D2" t="n">
-        <v>1957801914152</v>
+        <v>1957312348128</v>
       </c>
       <c r="E2" t="n">
-        <v>99838698778</v>
+        <v>105962937556</v>
       </c>
       <c r="F2" t="n">
-        <v>2.0972</v>
+        <v>1.8296</v>
       </c>
     </row>
     <row r="3">
@@ -503,16 +503,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3389.14</v>
+        <v>3385.16</v>
       </c>
       <c r="D3" t="n">
-        <v>408183778081</v>
+        <v>407528946484</v>
       </c>
       <c r="E3" t="n">
-        <v>57101803551</v>
+        <v>57176037571</v>
       </c>
       <c r="F3" t="n">
-        <v>9.253769999999999</v>
+        <v>9.096640000000001</v>
       </c>
     </row>
     <row r="4">
@@ -530,13 +530,13 @@
         <v>1.001</v>
       </c>
       <c r="D4" t="n">
-        <v>130823802841</v>
+        <v>130860870762</v>
       </c>
       <c r="E4" t="n">
-        <v>191268654241</v>
+        <v>126294469787</v>
       </c>
       <c r="F4" t="n">
-        <v>0.32316</v>
+        <v>0.12279</v>
       </c>
     </row>
     <row r="5">
@@ -551,16 +551,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>261.36</v>
+        <v>261.06</v>
       </c>
       <c r="D5" t="n">
-        <v>124099389605</v>
+        <v>123886385324</v>
       </c>
       <c r="E5" t="n">
-        <v>14903347184</v>
+        <v>14815108915</v>
       </c>
       <c r="F5" t="n">
-        <v>9.29208</v>
+        <v>9.37628</v>
       </c>
     </row>
     <row r="6">
@@ -575,16 +575,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>633.61</v>
+        <v>633.28</v>
       </c>
       <c r="D6" t="n">
-        <v>92441290124</v>
+        <v>92366163407</v>
       </c>
       <c r="E6" t="n">
-        <v>2462097536</v>
+        <v>2380817573</v>
       </c>
       <c r="F6" t="n">
-        <v>4.16909</v>
+        <v>4.06307</v>
       </c>
     </row>
     <row r="7">
@@ -602,13 +602,13 @@
         <v>1.4</v>
       </c>
       <c r="D7" t="n">
-        <v>79890440378</v>
+        <v>79935603727</v>
       </c>
       <c r="E7" t="n">
-        <v>18216983753</v>
+        <v>18250929448</v>
       </c>
       <c r="F7" t="n">
-        <v>26.85773</v>
+        <v>26.4852</v>
       </c>
     </row>
     <row r="8">
@@ -623,16 +623,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.396715</v>
+        <v>0.396128</v>
       </c>
       <c r="D8" t="n">
-        <v>58265317109</v>
+        <v>58217902823</v>
       </c>
       <c r="E8" t="n">
-        <v>9787067581</v>
+        <v>9750838152</v>
       </c>
       <c r="F8" t="n">
-        <v>3.75439</v>
+        <v>3.58956</v>
       </c>
     </row>
     <row r="9">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.999911</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>38332070800</v>
+        <v>38321674118</v>
       </c>
       <c r="E9" t="n">
-        <v>8044180063</v>
+        <v>12198920959</v>
       </c>
       <c r="F9" t="n">
-        <v>0.38615</v>
+        <v>0.01437</v>
       </c>
     </row>
     <row r="10">
@@ -671,16 +671,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3387.07</v>
+        <v>3386.24</v>
       </c>
       <c r="D10" t="n">
-        <v>33211105579</v>
+        <v>33159664554</v>
       </c>
       <c r="E10" t="n">
-        <v>145751955</v>
+        <v>143198614</v>
       </c>
       <c r="F10" t="n">
-        <v>9.066129999999999</v>
+        <v>8.99356</v>
       </c>
     </row>
     <row r="11">
@@ -695,16 +695,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.882131</v>
+        <v>0.882772</v>
       </c>
       <c r="D11" t="n">
-        <v>31574566650</v>
+        <v>31541459969</v>
       </c>
       <c r="E11" t="n">
-        <v>3012421450</v>
+        <v>3550138063</v>
       </c>
       <c r="F11" t="n">
-        <v>12.58447</v>
+        <v>12.56423</v>
       </c>
     </row>
     <row r="12">
@@ -719,16 +719,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.200153</v>
+        <v>0.20009</v>
       </c>
       <c r="D12" t="n">
-        <v>17285755290</v>
+        <v>17277520321</v>
       </c>
       <c r="E12" t="n">
-        <v>1062451930</v>
+        <v>1062158397</v>
       </c>
       <c r="F12" t="n">
-        <v>1.88472</v>
+        <v>1.76703</v>
       </c>
     </row>
     <row r="13">
@@ -743,16 +743,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>36.38</v>
+        <v>36.41</v>
       </c>
       <c r="D13" t="n">
-        <v>14894142924</v>
+        <v>14883697914</v>
       </c>
       <c r="E13" t="n">
-        <v>1049098992</v>
+        <v>1047195719</v>
       </c>
       <c r="F13" t="n">
-        <v>7.78136</v>
+        <v>7.4404</v>
       </c>
     </row>
     <row r="14">
@@ -767,16 +767,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.501e-05</v>
+        <v>2.5e-05</v>
       </c>
       <c r="D14" t="n">
-        <v>14745167792</v>
+        <v>14724458250</v>
       </c>
       <c r="E14" t="n">
-        <v>1599456205</v>
+        <v>1598057036</v>
       </c>
       <c r="F14" t="n">
-        <v>4.18302</v>
+        <v>3.9696</v>
       </c>
     </row>
     <row r="15">
@@ -791,16 +791,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>4011.1</v>
+        <v>4005.46</v>
       </c>
       <c r="D15" t="n">
-        <v>14487010535</v>
+        <v>14482650687</v>
       </c>
       <c r="E15" t="n">
-        <v>169572218</v>
+        <v>161361117</v>
       </c>
       <c r="F15" t="n">
-        <v>9.07639</v>
+        <v>8.896800000000001</v>
       </c>
     </row>
     <row r="16">
@@ -815,16 +815,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>98859</v>
+        <v>98714</v>
       </c>
       <c r="D16" t="n">
-        <v>14444416042</v>
+        <v>14414801790</v>
       </c>
       <c r="E16" t="n">
-        <v>847328202</v>
+        <v>837289225</v>
       </c>
       <c r="F16" t="n">
-        <v>2.29471</v>
+        <v>1.93306</v>
       </c>
     </row>
     <row r="17">
@@ -839,16 +839,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5.56</v>
+        <v>5.55</v>
       </c>
       <c r="D17" t="n">
-        <v>14159481773</v>
+        <v>14140621430</v>
       </c>
       <c r="E17" t="n">
-        <v>637235491</v>
+        <v>624413906</v>
       </c>
       <c r="F17" t="n">
-        <v>4.09133</v>
+        <v>3.71466</v>
       </c>
     </row>
     <row r="18">
@@ -866,13 +866,13 @@
         <v>3.61</v>
       </c>
       <c r="D18" t="n">
-        <v>10273589779</v>
+        <v>10262277354</v>
       </c>
       <c r="E18" t="n">
-        <v>2444539501</v>
+        <v>2046611540</v>
       </c>
       <c r="F18" t="n">
-        <v>1.08414</v>
+        <v>0.5314</v>
       </c>
     </row>
     <row r="19">
@@ -887,16 +887,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>498.78</v>
+        <v>498.98</v>
       </c>
       <c r="D19" t="n">
-        <v>9871422041</v>
+        <v>9882578564</v>
       </c>
       <c r="E19" t="n">
-        <v>1867669705</v>
+        <v>1817006727</v>
       </c>
       <c r="F19" t="n">
-        <v>-2.15394</v>
+        <v>-3.37977</v>
       </c>
     </row>
     <row r="20">
@@ -911,16 +911,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3392</v>
+        <v>3383.73</v>
       </c>
       <c r="D20" t="n">
-        <v>9734929278</v>
+        <v>9695241516</v>
       </c>
       <c r="E20" t="n">
-        <v>2223032283</v>
+        <v>2193400238</v>
       </c>
       <c r="F20" t="n">
-        <v>9.49335</v>
+        <v>8.92578</v>
       </c>
     </row>
     <row r="21">
@@ -935,64 +935,64 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>15.3</v>
+        <v>15.32</v>
       </c>
       <c r="D21" t="n">
-        <v>9592025550</v>
+        <v>9597641840</v>
       </c>
       <c r="E21" t="n">
-        <v>1257405474</v>
+        <v>1256233231</v>
       </c>
       <c r="F21" t="n">
-        <v>5.48991</v>
+        <v>5.70752</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>pepe</t>
+          <t>dot</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.138e-05</v>
+        <v>6.24</v>
       </c>
       <c r="D22" t="n">
-        <v>8996309587</v>
+        <v>8977044161</v>
       </c>
       <c r="E22" t="n">
-        <v>6804659980</v>
+        <v>839252580</v>
       </c>
       <c r="F22" t="n">
-        <v>10.57673</v>
+        <v>10.40347</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>dot</t>
+          <t>pepe</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>6.22</v>
+        <v>2.133e-05</v>
       </c>
       <c r="D23" t="n">
-        <v>8965227660</v>
+        <v>8974266732</v>
       </c>
       <c r="E23" t="n">
-        <v>830110510</v>
+        <v>6734296727</v>
       </c>
       <c r="F23" t="n">
-        <v>10.00362</v>
+        <v>10.19788</v>
       </c>
     </row>
     <row r="24">
@@ -1007,16 +1007,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.285028</v>
+        <v>0.284633</v>
       </c>
       <c r="D24" t="n">
-        <v>8544502079</v>
+        <v>8528344379</v>
       </c>
       <c r="E24" t="n">
-        <v>2312821480</v>
+        <v>2313085743</v>
       </c>
       <c r="F24" t="n">
-        <v>21.06954</v>
+        <v>20.34539</v>
       </c>
     </row>
     <row r="25">
@@ -1031,16 +1031,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>8.81</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="D25" t="n">
-        <v>8122298571</v>
+        <v>8138880715</v>
       </c>
       <c r="E25" t="n">
-        <v>3437792</v>
+        <v>3421347</v>
       </c>
       <c r="F25" t="n">
-        <v>4.04549</v>
+        <v>3.3504</v>
       </c>
     </row>
     <row r="26">
@@ -1058,13 +1058,13 @@
         <v>5.82</v>
       </c>
       <c r="D26" t="n">
-        <v>7088167865</v>
+        <v>7080828321</v>
       </c>
       <c r="E26" t="n">
-        <v>1012128839</v>
+        <v>1010209673</v>
       </c>
       <c r="F26" t="n">
-        <v>5.59196</v>
+        <v>5.71874</v>
       </c>
     </row>
     <row r="27">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>90.94</v>
+        <v>91.03</v>
       </c>
       <c r="D27" t="n">
-        <v>6841601458</v>
+        <v>6847455412</v>
       </c>
       <c r="E27" t="n">
-        <v>1410008469</v>
+        <v>1385604498</v>
       </c>
       <c r="F27" t="n">
-        <v>5.26465</v>
+        <v>5.40234</v>
       </c>
     </row>
     <row r="28">
@@ -1106,13 +1106,13 @@
         <v>12.14</v>
       </c>
       <c r="D28" t="n">
-        <v>6471544641</v>
+        <v>6472209222</v>
       </c>
       <c r="E28" t="n">
-        <v>859704634</v>
+        <v>856252554</v>
       </c>
       <c r="F28" t="n">
-        <v>4.33772</v>
+        <v>4.43628</v>
       </c>
     </row>
     <row r="29">
@@ -1127,16 +1127,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3576.2</v>
+        <v>3566.33</v>
       </c>
       <c r="D29" t="n">
-        <v>6220401781</v>
+        <v>6211334766</v>
       </c>
       <c r="E29" t="n">
-        <v>106018794</v>
+        <v>105658696</v>
       </c>
       <c r="F29" t="n">
-        <v>9.409129999999999</v>
+        <v>9.08948</v>
       </c>
     </row>
     <row r="30">
@@ -1151,16 +1151,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9.41</v>
+        <v>9.390000000000001</v>
       </c>
       <c r="D30" t="n">
-        <v>5655338943</v>
+        <v>5640414358</v>
       </c>
       <c r="E30" t="n">
-        <v>866236092</v>
+        <v>870529475</v>
       </c>
       <c r="F30" t="n">
-        <v>6.92099</v>
+        <v>6.54853</v>
       </c>
     </row>
     <row r="31">
@@ -1175,16 +1175,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.203305</v>
+        <v>0.202831</v>
       </c>
       <c r="D31" t="n">
-        <v>5504574071</v>
+        <v>5533748262</v>
       </c>
       <c r="E31" t="n">
-        <v>132475693</v>
+        <v>136788438</v>
       </c>
       <c r="F31" t="n">
-        <v>16.57485</v>
+        <v>16.49178</v>
       </c>
     </row>
     <row r="32">
@@ -1199,16 +1199,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.99746</v>
+        <v>0.999576</v>
       </c>
       <c r="D32" t="n">
-        <v>5229388035</v>
+        <v>5228866032</v>
       </c>
       <c r="E32" t="n">
-        <v>91130</v>
+        <v>16084967</v>
       </c>
       <c r="F32" t="n">
-        <v>0.04723</v>
+        <v>0.13728</v>
       </c>
     </row>
     <row r="33">
@@ -1223,16 +1223,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.133813</v>
+        <v>0.136113</v>
       </c>
       <c r="D33" t="n">
-        <v>5110910421</v>
+        <v>5156068985</v>
       </c>
       <c r="E33" t="n">
-        <v>907416623</v>
+        <v>921621803</v>
       </c>
       <c r="F33" t="n">
-        <v>8.14057</v>
+        <v>10.399</v>
       </c>
     </row>
     <row r="34">
@@ -1247,16 +1247,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9.640000000000001</v>
+        <v>9.68</v>
       </c>
       <c r="D34" t="n">
-        <v>4572289134</v>
+        <v>4584804726</v>
       </c>
       <c r="E34" t="n">
-        <v>274975740</v>
+        <v>275557543</v>
       </c>
       <c r="F34" t="n">
-        <v>7.32213</v>
+        <v>7.56923</v>
       </c>
     </row>
     <row r="35">
@@ -1271,16 +1271,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>28.1</v>
+        <v>28.13</v>
       </c>
       <c r="D35" t="n">
-        <v>4205261170</v>
+        <v>4210412676</v>
       </c>
       <c r="E35" t="n">
-        <v>871015505</v>
+        <v>870064263</v>
       </c>
       <c r="F35" t="n">
-        <v>6.17713</v>
+        <v>6.04145</v>
       </c>
     </row>
     <row r="36">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>5.213e-05</v>
+        <v>5.225e-05</v>
       </c>
       <c r="D36" t="n">
-        <v>3915257516</v>
+        <v>3919437831</v>
       </c>
       <c r="E36" t="n">
-        <v>1670661215</v>
+        <v>1639904482</v>
       </c>
       <c r="F36" t="n">
-        <v>2.57426</v>
+        <v>1.73519</v>
       </c>
     </row>
     <row r="37">
@@ -1319,16 +1319,16 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.152234</v>
+        <v>0.152416</v>
       </c>
       <c r="D37" t="n">
-        <v>3835490531</v>
+        <v>3840028133</v>
       </c>
       <c r="E37" t="n">
-        <v>151673221</v>
+        <v>151628290</v>
       </c>
       <c r="F37" t="n">
-        <v>1.06944</v>
+        <v>1.53692</v>
       </c>
     </row>
     <row r="38">
@@ -1346,13 +1346,13 @@
         <v>7.41</v>
       </c>
       <c r="D38" t="n">
-        <v>3835014471</v>
+        <v>3835215289</v>
       </c>
       <c r="E38" t="n">
-        <v>432564798</v>
+        <v>431243780</v>
       </c>
       <c r="F38" t="n">
-        <v>1.19444</v>
+        <v>1.12561</v>
       </c>
     </row>
     <row r="39">
@@ -1367,16 +1367,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.473232</v>
+        <v>0.469936</v>
       </c>
       <c r="D39" t="n">
-        <v>3772214715</v>
+        <v>3758408261</v>
       </c>
       <c r="E39" t="n">
-        <v>476956609</v>
+        <v>496353927</v>
       </c>
       <c r="F39" t="n">
-        <v>8.94638</v>
+        <v>8.170859999999999</v>
       </c>
     </row>
     <row r="40">
@@ -1391,16 +1391,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>504.62</v>
+        <v>504.32</v>
       </c>
       <c r="D40" t="n">
-        <v>3728030742</v>
+        <v>3722424094</v>
       </c>
       <c r="E40" t="n">
-        <v>282237842</v>
+        <v>281336572</v>
       </c>
       <c r="F40" t="n">
-        <v>2.92676</v>
+        <v>3.64941</v>
       </c>
     </row>
     <row r="41">
@@ -1418,13 +1418,13 @@
         <v>1.002</v>
       </c>
       <c r="D41" t="n">
-        <v>3688538085</v>
+        <v>3689859605</v>
       </c>
       <c r="E41" t="n">
-        <v>225145685</v>
+        <v>224518933</v>
       </c>
       <c r="F41" t="n">
-        <v>-0.05451</v>
+        <v>0.13789</v>
       </c>
     </row>
     <row r="42">
@@ -1439,16 +1439,16 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>24.81</v>
+        <v>24.88</v>
       </c>
       <c r="D42" t="n">
-        <v>3575035917</v>
+        <v>3575145979</v>
       </c>
       <c r="E42" t="n">
-        <v>33355617</v>
+        <v>44086915</v>
       </c>
       <c r="F42" t="n">
-        <v>3.25778</v>
+        <v>2.94399</v>
       </c>
     </row>
     <row r="43">
@@ -1463,16 +1463,16 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.999623</v>
+        <v>1</v>
       </c>
       <c r="D43" t="n">
-        <v>3440873426</v>
+        <v>3441676073</v>
       </c>
       <c r="E43" t="n">
-        <v>153373746</v>
+        <v>156466688</v>
       </c>
       <c r="F43" t="n">
-        <v>0.32737</v>
+        <v>-0.00268</v>
       </c>
     </row>
     <row r="44">
@@ -1490,13 +1490,13 @@
         <v>3.39</v>
       </c>
       <c r="D44" t="n">
-        <v>3388980858</v>
+        <v>3382728022</v>
       </c>
       <c r="E44" t="n">
-        <v>1282763387</v>
+        <v>1286539243</v>
       </c>
       <c r="F44" t="n">
-        <v>6.66468</v>
+        <v>5.68177</v>
       </c>
     </row>
     <row r="45">
@@ -1511,16 +1511,16 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3.73</v>
+        <v>3.78</v>
       </c>
       <c r="D45" t="n">
-        <v>3363633788</v>
+        <v>3381419859</v>
       </c>
       <c r="E45" t="n">
-        <v>301881074</v>
+        <v>302623861</v>
       </c>
       <c r="F45" t="n">
-        <v>4.29752</v>
+        <v>5.24868</v>
       </c>
     </row>
     <row r="46">
@@ -1538,13 +1538,13 @@
         <v>1.28</v>
       </c>
       <c r="D46" t="n">
-        <v>3347597945</v>
+        <v>3344707679</v>
       </c>
       <c r="E46" t="n">
-        <v>485036679</v>
+        <v>484485647</v>
       </c>
       <c r="F46" t="n">
-        <v>3.18392</v>
+        <v>3.49845</v>
       </c>
     </row>
     <row r="47">
@@ -1559,16 +1559,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.792019</v>
+        <v>0.793462</v>
       </c>
       <c r="D47" t="n">
-        <v>3245886344</v>
+        <v>3244693440</v>
       </c>
       <c r="E47" t="n">
-        <v>1672660052</v>
+        <v>1673139119</v>
       </c>
       <c r="F47" t="n">
-        <v>14.82186</v>
+        <v>15.0305</v>
       </c>
     </row>
     <row r="48">
@@ -1583,16 +1583,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>161.12</v>
+        <v>161.26</v>
       </c>
       <c r="D48" t="n">
-        <v>2972253972</v>
+        <v>2974960015</v>
       </c>
       <c r="E48" t="n">
-        <v>86424934</v>
+        <v>86422219</v>
       </c>
       <c r="F48" t="n">
-        <v>-0.18419</v>
+        <v>-0.45054</v>
       </c>
     </row>
     <row r="49">
@@ -1610,13 +1610,13 @@
         <v>1.97</v>
       </c>
       <c r="D49" t="n">
-        <v>2958504435</v>
+        <v>2957274297</v>
       </c>
       <c r="E49" t="n">
-        <v>358440221</v>
+        <v>355653430</v>
       </c>
       <c r="F49" t="n">
-        <v>3.285</v>
+        <v>2.91976</v>
       </c>
     </row>
     <row r="50">
@@ -1631,16 +1631,16 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.8428</v>
+        <v>0.84516</v>
       </c>
       <c r="D50" t="n">
-        <v>2837535662</v>
+        <v>2841679667</v>
       </c>
       <c r="E50" t="n">
-        <v>184150203</v>
+        <v>183193974</v>
       </c>
       <c r="F50" t="n">
-        <v>16.17144</v>
+        <v>16.02787</v>
       </c>
     </row>
     <row r="51">
@@ -1658,13 +1658,13 @@
         <v>4.71</v>
       </c>
       <c r="D51" t="n">
-        <v>2830209760</v>
+        <v>2830947251</v>
       </c>
       <c r="E51" t="n">
-        <v>578155150</v>
+        <v>576676347</v>
       </c>
       <c r="F51" t="n">
-        <v>8.21808</v>
+        <v>8.232100000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1957801914152</v>
+        <v>1957312348128</v>
       </c>
     </row>
     <row r="3">
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>408183778081</v>
+        <v>407528946484</v>
       </c>
     </row>
     <row r="4">
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>130823802841</v>
+        <v>130860870762</v>
       </c>
     </row>
     <row r="5">
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>124099389605</v>
+        <v>123886385324</v>
       </c>
     </row>
     <row r="6">
@@ -1745,7 +1745,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>92441290124</v>
+        <v>92366163407</v>
       </c>
     </row>
   </sheetData>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$4358.28</t>
+          <t>$4354.78</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>XRP (26.86%)</t>
+          <t>XRP (26.49%)</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bitcoin Cash (-2.15%)</t>
+          <t>Bitcoin Cash (-3.38%)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Excel data - 2024-11-22 06:21:36
</commit_message>
<xml_diff>
--- a/crypto_live_data.xlsx
+++ b/crypto_live_data.xlsx
@@ -479,16 +479,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>98949</v>
+        <v>98781</v>
       </c>
       <c r="D2" t="n">
-        <v>1957312348128</v>
+        <v>1954198009844</v>
       </c>
       <c r="E2" t="n">
-        <v>105962937556</v>
+        <v>112390278976</v>
       </c>
       <c r="F2" t="n">
-        <v>1.8296</v>
+        <v>1.60471</v>
       </c>
     </row>
     <row r="3">
@@ -503,16 +503,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3385.16</v>
+        <v>3377.14</v>
       </c>
       <c r="D3" t="n">
-        <v>407528946484</v>
+        <v>406670065516</v>
       </c>
       <c r="E3" t="n">
-        <v>57176037571</v>
+        <v>57054771047</v>
       </c>
       <c r="F3" t="n">
-        <v>9.096640000000001</v>
+        <v>8.469720000000001</v>
       </c>
     </row>
     <row r="4">
@@ -527,16 +527,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.001</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>130860870762</v>
+        <v>130821581010</v>
       </c>
       <c r="E4" t="n">
-        <v>126294469787</v>
+        <v>183012864316</v>
       </c>
       <c r="F4" t="n">
-        <v>0.12279</v>
+        <v>-0.04268</v>
       </c>
     </row>
     <row r="5">
@@ -551,16 +551,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>261.06</v>
+        <v>259.48</v>
       </c>
       <c r="D5" t="n">
-        <v>123886385324</v>
+        <v>123188156523</v>
       </c>
       <c r="E5" t="n">
-        <v>14815108915</v>
+        <v>14777737320</v>
       </c>
       <c r="F5" t="n">
-        <v>9.37628</v>
+        <v>8.589700000000001</v>
       </c>
     </row>
     <row r="6">
@@ -575,16 +575,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>633.28</v>
+        <v>630.97</v>
       </c>
       <c r="D6" t="n">
-        <v>92366163407</v>
+        <v>92052602155</v>
       </c>
       <c r="E6" t="n">
-        <v>2380817573</v>
+        <v>2498055748</v>
       </c>
       <c r="F6" t="n">
-        <v>4.06307</v>
+        <v>3.47283</v>
       </c>
     </row>
     <row r="7">
@@ -599,16 +599,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.4</v>
+        <v>1.41</v>
       </c>
       <c r="D7" t="n">
-        <v>79935603727</v>
+        <v>80370827021</v>
       </c>
       <c r="E7" t="n">
-        <v>18250929448</v>
+        <v>18422362798</v>
       </c>
       <c r="F7" t="n">
-        <v>26.4852</v>
+        <v>26.93999</v>
       </c>
     </row>
     <row r="8">
@@ -623,16 +623,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.396128</v>
+        <v>0.394378</v>
       </c>
       <c r="D8" t="n">
-        <v>58217902823</v>
+        <v>57906961638</v>
       </c>
       <c r="E8" t="n">
-        <v>9750838152</v>
+        <v>9730213490</v>
       </c>
       <c r="F8" t="n">
-        <v>3.58956</v>
+        <v>2.89369</v>
       </c>
     </row>
     <row r="9">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0.999152</v>
       </c>
       <c r="D9" t="n">
-        <v>38321674118</v>
+        <v>38292986605</v>
       </c>
       <c r="E9" t="n">
-        <v>12198920959</v>
+        <v>11690219708</v>
       </c>
       <c r="F9" t="n">
-        <v>0.01437</v>
+        <v>-0.12898</v>
       </c>
     </row>
     <row r="10">
@@ -671,16 +671,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3386.24</v>
+        <v>3378.25</v>
       </c>
       <c r="D10" t="n">
-        <v>33159664554</v>
+        <v>33089387008</v>
       </c>
       <c r="E10" t="n">
-        <v>143198614</v>
+        <v>141546953</v>
       </c>
       <c r="F10" t="n">
-        <v>8.99356</v>
+        <v>8.46048</v>
       </c>
     </row>
     <row r="11">
@@ -695,16 +695,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.882772</v>
+        <v>0.883571</v>
       </c>
       <c r="D11" t="n">
-        <v>31541459969</v>
+        <v>31609255024</v>
       </c>
       <c r="E11" t="n">
-        <v>3550138063</v>
+        <v>3758331072</v>
       </c>
       <c r="F11" t="n">
-        <v>12.56423</v>
+        <v>12.16342</v>
       </c>
     </row>
     <row r="12">
@@ -719,16 +719,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.20009</v>
+        <v>0.199602</v>
       </c>
       <c r="D12" t="n">
-        <v>17277520321</v>
+        <v>17236971977</v>
       </c>
       <c r="E12" t="n">
-        <v>1062158397</v>
+        <v>1070924350</v>
       </c>
       <c r="F12" t="n">
-        <v>1.76703</v>
+        <v>1.23089</v>
       </c>
     </row>
     <row r="13">
@@ -743,16 +743,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>36.41</v>
+        <v>36.28</v>
       </c>
       <c r="D13" t="n">
-        <v>14883697914</v>
+        <v>14844705898</v>
       </c>
       <c r="E13" t="n">
-        <v>1047195719</v>
+        <v>1045261609</v>
       </c>
       <c r="F13" t="n">
-        <v>7.4404</v>
+        <v>7.19604</v>
       </c>
     </row>
     <row r="14">
@@ -767,16 +767,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.5e-05</v>
+        <v>2.494e-05</v>
       </c>
       <c r="D14" t="n">
-        <v>14724458250</v>
+        <v>14693630180</v>
       </c>
       <c r="E14" t="n">
-        <v>1598057036</v>
+        <v>1594894926</v>
       </c>
       <c r="F14" t="n">
-        <v>3.9696</v>
+        <v>3.59182</v>
       </c>
     </row>
     <row r="15">
@@ -791,16 +791,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>4005.46</v>
+        <v>4002.64</v>
       </c>
       <c r="D15" t="n">
-        <v>14482650687</v>
+        <v>14444484957</v>
       </c>
       <c r="E15" t="n">
-        <v>161361117</v>
+        <v>169059682</v>
       </c>
       <c r="F15" t="n">
-        <v>8.896800000000001</v>
+        <v>8.64603</v>
       </c>
     </row>
     <row r="16">
@@ -815,16 +815,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>98714</v>
+        <v>98585</v>
       </c>
       <c r="D16" t="n">
-        <v>14414801790</v>
+        <v>14399440584</v>
       </c>
       <c r="E16" t="n">
-        <v>837289225</v>
+        <v>826645767</v>
       </c>
       <c r="F16" t="n">
-        <v>1.93306</v>
+        <v>1.7654</v>
       </c>
     </row>
     <row r="17">
@@ -839,16 +839,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5.55</v>
+        <v>5.54</v>
       </c>
       <c r="D17" t="n">
-        <v>14140621430</v>
+        <v>14119887111</v>
       </c>
       <c r="E17" t="n">
-        <v>624413906</v>
+        <v>623059661</v>
       </c>
       <c r="F17" t="n">
-        <v>3.71466</v>
+        <v>3.12425</v>
       </c>
     </row>
     <row r="18">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3.61</v>
+        <v>3.6</v>
       </c>
       <c r="D18" t="n">
-        <v>10262277354</v>
+        <v>10232927881</v>
       </c>
       <c r="E18" t="n">
-        <v>2046611540</v>
+        <v>2055446112</v>
       </c>
       <c r="F18" t="n">
-        <v>0.5314</v>
+        <v>0.63511</v>
       </c>
     </row>
     <row r="19">
@@ -887,16 +887,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>498.98</v>
+        <v>495.92</v>
       </c>
       <c r="D19" t="n">
-        <v>9882578564</v>
+        <v>9807988842</v>
       </c>
       <c r="E19" t="n">
-        <v>1817006727</v>
+        <v>1790730676</v>
       </c>
       <c r="F19" t="n">
-        <v>-3.37977</v>
+        <v>-4.17848</v>
       </c>
     </row>
     <row r="20">
@@ -911,16 +911,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3383.73</v>
+        <v>3377</v>
       </c>
       <c r="D20" t="n">
-        <v>9695241516</v>
+        <v>9674931817</v>
       </c>
       <c r="E20" t="n">
-        <v>2193400238</v>
+        <v>2223824701</v>
       </c>
       <c r="F20" t="n">
-        <v>8.92578</v>
+        <v>8.58658</v>
       </c>
     </row>
     <row r="21">
@@ -935,64 +935,64 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>15.32</v>
+        <v>15.31</v>
       </c>
       <c r="D21" t="n">
-        <v>9597641840</v>
+        <v>9596106894</v>
       </c>
       <c r="E21" t="n">
-        <v>1256233231</v>
+        <v>1255002788</v>
       </c>
       <c r="F21" t="n">
-        <v>5.70752</v>
+        <v>5.58711</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Polkadot</t>
+          <t>Pepe</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>dot</t>
+          <t>pepe</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>6.24</v>
+        <v>2.135e-05</v>
       </c>
       <c r="D22" t="n">
-        <v>8977044161</v>
+        <v>8974266732</v>
       </c>
       <c r="E22" t="n">
-        <v>839252580</v>
+        <v>6729179657</v>
       </c>
       <c r="F22" t="n">
-        <v>10.40347</v>
+        <v>10.04046</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Pepe</t>
+          <t>Polkadot</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>pepe</t>
+          <t>dot</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2.133e-05</v>
+        <v>6.22</v>
       </c>
       <c r="D23" t="n">
-        <v>8974266732</v>
+        <v>8969229904</v>
       </c>
       <c r="E23" t="n">
-        <v>6734296727</v>
+        <v>840762108</v>
       </c>
       <c r="F23" t="n">
-        <v>10.19788</v>
+        <v>9.717230000000001</v>
       </c>
     </row>
     <row r="24">
@@ -1007,16 +1007,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.284633</v>
+        <v>0.286093</v>
       </c>
       <c r="D24" t="n">
-        <v>8528344379</v>
+        <v>8579890000</v>
       </c>
       <c r="E24" t="n">
-        <v>2313085743</v>
+        <v>2328650446</v>
       </c>
       <c r="F24" t="n">
-        <v>20.34539</v>
+        <v>19.85431</v>
       </c>
     </row>
     <row r="25">
@@ -1031,16 +1031,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>8.800000000000001</v>
+        <v>8.789999999999999</v>
       </c>
       <c r="D25" t="n">
-        <v>8138880715</v>
+        <v>8127976591</v>
       </c>
       <c r="E25" t="n">
-        <v>3421347</v>
+        <v>3417151</v>
       </c>
       <c r="F25" t="n">
-        <v>3.3504</v>
+        <v>3.64561</v>
       </c>
     </row>
     <row r="26">
@@ -1055,16 +1055,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>5.82</v>
+        <v>5.8</v>
       </c>
       <c r="D26" t="n">
-        <v>7080828321</v>
+        <v>7067686644</v>
       </c>
       <c r="E26" t="n">
-        <v>1010209673</v>
+        <v>1004401919</v>
       </c>
       <c r="F26" t="n">
-        <v>5.71874</v>
+        <v>5.35271</v>
       </c>
     </row>
     <row r="27">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>91.03</v>
+        <v>90.86</v>
       </c>
       <c r="D27" t="n">
-        <v>6847455412</v>
+        <v>6833649109</v>
       </c>
       <c r="E27" t="n">
-        <v>1385604498</v>
+        <v>1335029714</v>
       </c>
       <c r="F27" t="n">
-        <v>5.40234</v>
+        <v>3.91033</v>
       </c>
     </row>
     <row r="28">
@@ -1103,16 +1103,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>12.14</v>
+        <v>12.09</v>
       </c>
       <c r="D28" t="n">
         <v>6472209222</v>
       </c>
       <c r="E28" t="n">
-        <v>856252554</v>
+        <v>851267493</v>
       </c>
       <c r="F28" t="n">
-        <v>4.43628</v>
+        <v>3.9428</v>
       </c>
     </row>
     <row r="29">
@@ -1127,16 +1127,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3566.33</v>
+        <v>3559.51</v>
       </c>
       <c r="D29" t="n">
-        <v>6211334766</v>
+        <v>6194902543</v>
       </c>
       <c r="E29" t="n">
-        <v>105658696</v>
+        <v>105782378</v>
       </c>
       <c r="F29" t="n">
-        <v>9.08948</v>
+        <v>8.69229</v>
       </c>
     </row>
     <row r="30">
@@ -1151,16 +1151,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9.390000000000001</v>
+        <v>9.35</v>
       </c>
       <c r="D30" t="n">
-        <v>5640414358</v>
+        <v>5614203040</v>
       </c>
       <c r="E30" t="n">
-        <v>870529475</v>
+        <v>870750030</v>
       </c>
       <c r="F30" t="n">
-        <v>6.54853</v>
+        <v>5.84469</v>
       </c>
     </row>
     <row r="31">
@@ -1175,64 +1175,64 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.202831</v>
+        <v>0.195065</v>
       </c>
       <c r="D31" t="n">
-        <v>5533748262</v>
+        <v>5341306291</v>
       </c>
       <c r="E31" t="n">
-        <v>136788438</v>
+        <v>141273639</v>
       </c>
       <c r="F31" t="n">
-        <v>16.49178</v>
+        <v>11.78849</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>USDS</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>usds</t>
+          <t>hbar</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.999576</v>
+        <v>0.137038</v>
       </c>
       <c r="D32" t="n">
-        <v>5228866032</v>
+        <v>5238270224</v>
       </c>
       <c r="E32" t="n">
-        <v>16084967</v>
+        <v>934498283</v>
       </c>
       <c r="F32" t="n">
-        <v>0.13728</v>
+        <v>10.09357</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>USDS</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>hbar</t>
+          <t>usds</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.136113</v>
+        <v>0.999299</v>
       </c>
       <c r="D33" t="n">
-        <v>5156068985</v>
+        <v>5230226962</v>
       </c>
       <c r="E33" t="n">
-        <v>921621803</v>
+        <v>16080506</v>
       </c>
       <c r="F33" t="n">
-        <v>10.399</v>
+        <v>-0.32212</v>
       </c>
     </row>
     <row r="34">
@@ -1247,16 +1247,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9.68</v>
+        <v>9.66</v>
       </c>
       <c r="D34" t="n">
-        <v>4584804726</v>
+        <v>4584170683</v>
       </c>
       <c r="E34" t="n">
-        <v>275557543</v>
+        <v>274022971</v>
       </c>
       <c r="F34" t="n">
-        <v>7.56923</v>
+        <v>7.12318</v>
       </c>
     </row>
     <row r="35">
@@ -1271,16 +1271,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>28.13</v>
+        <v>28.06</v>
       </c>
       <c r="D35" t="n">
-        <v>4210412676</v>
+        <v>4199695234</v>
       </c>
       <c r="E35" t="n">
-        <v>870064263</v>
+        <v>866959534</v>
       </c>
       <c r="F35" t="n">
-        <v>6.04145</v>
+        <v>5.17743</v>
       </c>
     </row>
     <row r="36">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>5.225e-05</v>
+        <v>5.233e-05</v>
       </c>
       <c r="D36" t="n">
         <v>3919437831</v>
       </c>
       <c r="E36" t="n">
-        <v>1639904482</v>
+        <v>1630787456</v>
       </c>
       <c r="F36" t="n">
-        <v>1.73519</v>
+        <v>0.41931</v>
       </c>
     </row>
     <row r="37">
@@ -1319,16 +1319,16 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.152416</v>
+        <v>0.152056</v>
       </c>
       <c r="D37" t="n">
-        <v>3840028133</v>
+        <v>3832081221</v>
       </c>
       <c r="E37" t="n">
-        <v>151628290</v>
+        <v>151141330</v>
       </c>
       <c r="F37" t="n">
-        <v>1.53692</v>
+        <v>0.92423</v>
       </c>
     </row>
     <row r="38">
@@ -1343,16 +1343,16 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>7.41</v>
+        <v>7.37</v>
       </c>
       <c r="D38" t="n">
-        <v>3835215289</v>
+        <v>3813426846</v>
       </c>
       <c r="E38" t="n">
-        <v>431243780</v>
+        <v>430485438</v>
       </c>
       <c r="F38" t="n">
-        <v>1.12561</v>
+        <v>0.49782</v>
       </c>
     </row>
     <row r="39">
@@ -1367,16 +1367,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.469936</v>
+        <v>0.467282</v>
       </c>
       <c r="D39" t="n">
-        <v>3758408261</v>
+        <v>3723235499</v>
       </c>
       <c r="E39" t="n">
-        <v>496353927</v>
+        <v>497017761</v>
       </c>
       <c r="F39" t="n">
-        <v>8.170859999999999</v>
+        <v>6.94723</v>
       </c>
     </row>
     <row r="40">
@@ -1391,16 +1391,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>504.32</v>
+        <v>502.34</v>
       </c>
       <c r="D40" t="n">
         <v>3722424094</v>
       </c>
       <c r="E40" t="n">
-        <v>281336572</v>
+        <v>280112348</v>
       </c>
       <c r="F40" t="n">
-        <v>3.64941</v>
+        <v>3.21335</v>
       </c>
     </row>
     <row r="41">
@@ -1415,16 +1415,16 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1.002</v>
+        <v>1.001</v>
       </c>
       <c r="D41" t="n">
-        <v>3689859605</v>
+        <v>3686884674</v>
       </c>
       <c r="E41" t="n">
-        <v>224518933</v>
+        <v>224249364</v>
       </c>
       <c r="F41" t="n">
-        <v>0.13789</v>
+        <v>-0.08049000000000001</v>
       </c>
     </row>
     <row r="42">
@@ -1439,16 +1439,16 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>24.88</v>
+        <v>24.77</v>
       </c>
       <c r="D42" t="n">
         <v>3575145979</v>
       </c>
       <c r="E42" t="n">
-        <v>44086915</v>
+        <v>33131314</v>
       </c>
       <c r="F42" t="n">
-        <v>2.94399</v>
+        <v>2.74346</v>
       </c>
     </row>
     <row r="43">
@@ -1463,64 +1463,64 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1</v>
+        <v>0.999429</v>
       </c>
       <c r="D43" t="n">
-        <v>3441676073</v>
+        <v>3439660368</v>
       </c>
       <c r="E43" t="n">
-        <v>156466688</v>
+        <v>184363126</v>
       </c>
       <c r="F43" t="n">
-        <v>-0.00268</v>
+        <v>0.14324</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>dogwifhat</t>
+          <t>MANTRA</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>wif</t>
+          <t>om</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>3.39</v>
+        <v>3.82</v>
       </c>
       <c r="D44" t="n">
-        <v>3382728022</v>
+        <v>3439598122</v>
       </c>
       <c r="E44" t="n">
-        <v>1286539243</v>
+        <v>304755108</v>
       </c>
       <c r="F44" t="n">
-        <v>5.68177</v>
+        <v>5.80427</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>MANTRA</t>
+          <t>dogwifhat</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>om</t>
+          <t>wif</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3.78</v>
+        <v>3.38</v>
       </c>
       <c r="D45" t="n">
-        <v>3381419859</v>
+        <v>3377151669</v>
       </c>
       <c r="E45" t="n">
-        <v>302623861</v>
+        <v>1281353338</v>
       </c>
       <c r="F45" t="n">
-        <v>5.24868</v>
+        <v>5.16064</v>
       </c>
     </row>
     <row r="46">
@@ -1538,13 +1538,13 @@
         <v>1.28</v>
       </c>
       <c r="D46" t="n">
-        <v>3344707679</v>
+        <v>3350991172</v>
       </c>
       <c r="E46" t="n">
-        <v>484485647</v>
+        <v>481757661</v>
       </c>
       <c r="F46" t="n">
-        <v>3.49845</v>
+        <v>3.13522</v>
       </c>
     </row>
     <row r="47">
@@ -1559,16 +1559,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.793462</v>
+        <v>0.789976</v>
       </c>
       <c r="D47" t="n">
-        <v>3244693440</v>
+        <v>3236809423</v>
       </c>
       <c r="E47" t="n">
-        <v>1673139119</v>
+        <v>1676829198</v>
       </c>
       <c r="F47" t="n">
-        <v>15.0305</v>
+        <v>14.39195</v>
       </c>
     </row>
     <row r="48">
@@ -1583,16 +1583,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>161.26</v>
+        <v>161.18</v>
       </c>
       <c r="D48" t="n">
-        <v>2974960015</v>
+        <v>2972719324</v>
       </c>
       <c r="E48" t="n">
-        <v>86422219</v>
+        <v>83675039</v>
       </c>
       <c r="F48" t="n">
-        <v>-0.45054</v>
+        <v>-0.35097</v>
       </c>
     </row>
     <row r="49">
@@ -1607,16 +1607,16 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1.97</v>
+        <v>1.96</v>
       </c>
       <c r="D49" t="n">
-        <v>2957274297</v>
+        <v>2943890749</v>
       </c>
       <c r="E49" t="n">
-        <v>355653430</v>
+        <v>352719354</v>
       </c>
       <c r="F49" t="n">
-        <v>2.91976</v>
+        <v>2.63933</v>
       </c>
     </row>
     <row r="50">
@@ -1631,16 +1631,16 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.84516</v>
+        <v>0.838499</v>
       </c>
       <c r="D50" t="n">
-        <v>2841679667</v>
+        <v>2824529619</v>
       </c>
       <c r="E50" t="n">
-        <v>183193974</v>
+        <v>185914513</v>
       </c>
       <c r="F50" t="n">
-        <v>16.02787</v>
+        <v>15.13845</v>
       </c>
     </row>
     <row r="51">
@@ -1655,16 +1655,16 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>4.71</v>
+        <v>4.69</v>
       </c>
       <c r="D51" t="n">
-        <v>2830947251</v>
+        <v>2815699050</v>
       </c>
       <c r="E51" t="n">
-        <v>576676347</v>
+        <v>576199430</v>
       </c>
       <c r="F51" t="n">
-        <v>8.232100000000001</v>
+        <v>7.35606</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1957312348128</v>
+        <v>1954198009844</v>
       </c>
     </row>
     <row r="3">
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>407528946484</v>
+        <v>406670065516</v>
       </c>
     </row>
     <row r="4">
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>130860870762</v>
+        <v>130821581010</v>
       </c>
     </row>
     <row r="5">
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>123886385324</v>
+        <v>123188156523</v>
       </c>
     </row>
     <row r="6">
@@ -1745,7 +1745,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>92366163407</v>
+        <v>92052602155</v>
       </c>
     </row>
   </sheetData>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$4354.78</t>
+          <t>$4348.00</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>XRP (26.49%)</t>
+          <t>XRP (26.94%)</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bitcoin Cash (-3.38%)</t>
+          <t>Bitcoin Cash (-4.18%)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Excel data - 2024-11-22 06:26:37
</commit_message>
<xml_diff>
--- a/crypto_live_data.xlsx
+++ b/crypto_live_data.xlsx
@@ -479,16 +479,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>98781</v>
+        <v>98890</v>
       </c>
       <c r="D2" t="n">
-        <v>1954198009844</v>
+        <v>1959698004531</v>
       </c>
       <c r="E2" t="n">
-        <v>112390278976</v>
+        <v>111556511395</v>
       </c>
       <c r="F2" t="n">
-        <v>1.60471</v>
+        <v>1.79611</v>
       </c>
     </row>
     <row r="3">
@@ -503,16 +503,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3377.14</v>
+        <v>3368.92</v>
       </c>
       <c r="D3" t="n">
-        <v>406670065516</v>
+        <v>406338286340</v>
       </c>
       <c r="E3" t="n">
-        <v>57054771047</v>
+        <v>57069836564</v>
       </c>
       <c r="F3" t="n">
-        <v>8.469720000000001</v>
+        <v>8.067830000000001</v>
       </c>
     </row>
     <row r="4">
@@ -527,16 +527,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>1.001</v>
       </c>
       <c r="D4" t="n">
-        <v>130821581010</v>
+        <v>130970143446</v>
       </c>
       <c r="E4" t="n">
-        <v>183012864316</v>
+        <v>182938028684</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.04268</v>
+        <v>0.09354999999999999</v>
       </c>
     </row>
     <row r="5">
@@ -551,16 +551,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>259.48</v>
+        <v>259.58</v>
       </c>
       <c r="D5" t="n">
-        <v>123188156523</v>
+        <v>123494602662</v>
       </c>
       <c r="E5" t="n">
-        <v>14777737320</v>
+        <v>14771296331</v>
       </c>
       <c r="F5" t="n">
-        <v>8.589700000000001</v>
+        <v>8.85698</v>
       </c>
     </row>
     <row r="6">
@@ -575,16 +575,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>630.97</v>
+        <v>630.27</v>
       </c>
       <c r="D6" t="n">
-        <v>92052602155</v>
+        <v>92034027631</v>
       </c>
       <c r="E6" t="n">
-        <v>2498055748</v>
+        <v>2506552932</v>
       </c>
       <c r="F6" t="n">
-        <v>3.47283</v>
+        <v>3.43071</v>
       </c>
     </row>
     <row r="7">
@@ -602,13 +602,13 @@
         <v>1.41</v>
       </c>
       <c r="D7" t="n">
-        <v>80370827021</v>
+        <v>80278940768</v>
       </c>
       <c r="E7" t="n">
-        <v>18422362798</v>
+        <v>18503538652</v>
       </c>
       <c r="F7" t="n">
-        <v>26.93999</v>
+        <v>26.92868</v>
       </c>
     </row>
     <row r="8">
@@ -623,16 +623,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.394378</v>
+        <v>0.393778</v>
       </c>
       <c r="D8" t="n">
-        <v>57906961638</v>
+        <v>58027240960</v>
       </c>
       <c r="E8" t="n">
-        <v>9730213490</v>
+        <v>9748555380</v>
       </c>
       <c r="F8" t="n">
-        <v>2.89369</v>
+        <v>2.59959</v>
       </c>
     </row>
     <row r="9">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.999152</v>
+        <v>0.999411</v>
       </c>
       <c r="D9" t="n">
-        <v>38292986605</v>
+        <v>38359750699</v>
       </c>
       <c r="E9" t="n">
-        <v>11690219708</v>
+        <v>10847807727</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.12898</v>
+        <v>0.02544</v>
       </c>
     </row>
     <row r="10">
@@ -671,16 +671,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3378.25</v>
+        <v>3368.18</v>
       </c>
       <c r="D10" t="n">
-        <v>33089387008</v>
+        <v>33037771601</v>
       </c>
       <c r="E10" t="n">
-        <v>141546953</v>
+        <v>140321815</v>
       </c>
       <c r="F10" t="n">
-        <v>8.46048</v>
+        <v>7.94378</v>
       </c>
     </row>
     <row r="11">
@@ -695,16 +695,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.883571</v>
+        <v>0.884283</v>
       </c>
       <c r="D11" t="n">
-        <v>31609255024</v>
+        <v>31681007165</v>
       </c>
       <c r="E11" t="n">
-        <v>3758331072</v>
+        <v>3764850697</v>
       </c>
       <c r="F11" t="n">
-        <v>12.16342</v>
+        <v>12.03466</v>
       </c>
     </row>
     <row r="12">
@@ -719,16 +719,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.199602</v>
+        <v>0.199391</v>
       </c>
       <c r="D12" t="n">
-        <v>17236971977</v>
+        <v>17228471586</v>
       </c>
       <c r="E12" t="n">
-        <v>1070924350</v>
+        <v>1069521924</v>
       </c>
       <c r="F12" t="n">
-        <v>1.23089</v>
+        <v>0.93377</v>
       </c>
     </row>
     <row r="13">
@@ -743,16 +743,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>36.28</v>
+        <v>36.25</v>
       </c>
       <c r="D13" t="n">
-        <v>14844705898</v>
+        <v>14850836971</v>
       </c>
       <c r="E13" t="n">
-        <v>1045261609</v>
+        <v>1041350077</v>
       </c>
       <c r="F13" t="n">
-        <v>7.19604</v>
+        <v>6.74635</v>
       </c>
     </row>
     <row r="14">
@@ -767,16 +767,16 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.494e-05</v>
+        <v>2.487e-05</v>
       </c>
       <c r="D14" t="n">
-        <v>14693630180</v>
+        <v>14667878935</v>
       </c>
       <c r="E14" t="n">
-        <v>1594894926</v>
+        <v>1592407723</v>
       </c>
       <c r="F14" t="n">
-        <v>3.59182</v>
+        <v>3.34849</v>
       </c>
     </row>
     <row r="15">
@@ -791,16 +791,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>4002.64</v>
+        <v>3994.45</v>
       </c>
       <c r="D15" t="n">
-        <v>14444484957</v>
+        <v>14430087078</v>
       </c>
       <c r="E15" t="n">
-        <v>169059682</v>
+        <v>170220205</v>
       </c>
       <c r="F15" t="n">
-        <v>8.64603</v>
+        <v>7.91847</v>
       </c>
     </row>
     <row r="16">
@@ -815,16 +815,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>98585</v>
+        <v>98404</v>
       </c>
       <c r="D16" t="n">
-        <v>14399440584</v>
+        <v>14398635396</v>
       </c>
       <c r="E16" t="n">
-        <v>826645767</v>
+        <v>820480113</v>
       </c>
       <c r="F16" t="n">
-        <v>1.7654</v>
+        <v>1.45316</v>
       </c>
     </row>
     <row r="17">
@@ -839,16 +839,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5.54</v>
+        <v>5.53</v>
       </c>
       <c r="D17" t="n">
-        <v>14119887111</v>
+        <v>14095403038</v>
       </c>
       <c r="E17" t="n">
-        <v>623059661</v>
+        <v>624264587</v>
       </c>
       <c r="F17" t="n">
-        <v>3.12425</v>
+        <v>2.79731</v>
       </c>
     </row>
     <row r="18">
@@ -866,13 +866,13 @@
         <v>3.6</v>
       </c>
       <c r="D18" t="n">
-        <v>10232927881</v>
+        <v>10245919377</v>
       </c>
       <c r="E18" t="n">
-        <v>2055446112</v>
+        <v>2093423841</v>
       </c>
       <c r="F18" t="n">
-        <v>0.63511</v>
+        <v>0.87947</v>
       </c>
     </row>
     <row r="19">
@@ -887,16 +887,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>495.92</v>
+        <v>495.73</v>
       </c>
       <c r="D19" t="n">
-        <v>9807988842</v>
+        <v>9835172618</v>
       </c>
       <c r="E19" t="n">
-        <v>1790730676</v>
+        <v>1749875615</v>
       </c>
       <c r="F19" t="n">
-        <v>-4.17848</v>
+        <v>-6.09258</v>
       </c>
     </row>
     <row r="20">
@@ -911,16 +911,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3377</v>
+        <v>3363.77</v>
       </c>
       <c r="D20" t="n">
-        <v>9674931817</v>
+        <v>9656540862</v>
       </c>
       <c r="E20" t="n">
-        <v>2223824701</v>
+        <v>2085909929</v>
       </c>
       <c r="F20" t="n">
-        <v>8.58658</v>
+        <v>7.97274</v>
       </c>
     </row>
     <row r="21">
@@ -935,16 +935,16 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>15.31</v>
+        <v>15.26</v>
       </c>
       <c r="D21" t="n">
-        <v>9596106894</v>
+        <v>9606079703</v>
       </c>
       <c r="E21" t="n">
-        <v>1255002788</v>
+        <v>1257251807</v>
       </c>
       <c r="F21" t="n">
-        <v>5.58711</v>
+        <v>4.59659</v>
       </c>
     </row>
     <row r="22">
@@ -959,16 +959,16 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.135e-05</v>
+        <v>2.13e-05</v>
       </c>
       <c r="D22" t="n">
-        <v>8974266732</v>
+        <v>8960436990</v>
       </c>
       <c r="E22" t="n">
-        <v>6729179657</v>
+        <v>6723740508</v>
       </c>
       <c r="F22" t="n">
-        <v>10.04046</v>
+        <v>9.34882</v>
       </c>
     </row>
     <row r="23">
@@ -986,13 +986,13 @@
         <v>6.22</v>
       </c>
       <c r="D23" t="n">
-        <v>8969229904</v>
+        <v>8956646967</v>
       </c>
       <c r="E23" t="n">
-        <v>840762108</v>
+        <v>844240722</v>
       </c>
       <c r="F23" t="n">
-        <v>9.717230000000001</v>
+        <v>9.40147</v>
       </c>
     </row>
     <row r="24">
@@ -1007,16 +1007,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.286093</v>
+        <v>0.287774</v>
       </c>
       <c r="D24" t="n">
-        <v>8579890000</v>
+        <v>8635355878</v>
       </c>
       <c r="E24" t="n">
-        <v>2328650446</v>
+        <v>2343798557</v>
       </c>
       <c r="F24" t="n">
-        <v>19.85431</v>
+        <v>21.1674</v>
       </c>
     </row>
     <row r="25">
@@ -1031,16 +1031,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>8.789999999999999</v>
+        <v>8.81</v>
       </c>
       <c r="D25" t="n">
-        <v>8127976591</v>
+        <v>8139643571</v>
       </c>
       <c r="E25" t="n">
-        <v>3417151</v>
+        <v>3400762</v>
       </c>
       <c r="F25" t="n">
-        <v>3.64561</v>
+        <v>3.85022</v>
       </c>
     </row>
     <row r="26">
@@ -1055,16 +1055,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>5.8</v>
+        <v>5.78</v>
       </c>
       <c r="D26" t="n">
-        <v>7067686644</v>
+        <v>7046717485</v>
       </c>
       <c r="E26" t="n">
-        <v>1004401919</v>
+        <v>1003167791</v>
       </c>
       <c r="F26" t="n">
-        <v>5.35271</v>
+        <v>4.90486</v>
       </c>
     </row>
     <row r="27">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>90.86</v>
+        <v>90.59</v>
       </c>
       <c r="D27" t="n">
-        <v>6833649109</v>
+        <v>6833848492</v>
       </c>
       <c r="E27" t="n">
-        <v>1335029714</v>
+        <v>1334339155</v>
       </c>
       <c r="F27" t="n">
-        <v>3.91033</v>
+        <v>2.55445</v>
       </c>
     </row>
     <row r="28">
@@ -1103,16 +1103,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>12.09</v>
+        <v>12.04</v>
       </c>
       <c r="D28" t="n">
-        <v>6472209222</v>
+        <v>6423652211</v>
       </c>
       <c r="E28" t="n">
-        <v>851267493</v>
+        <v>846792578</v>
       </c>
       <c r="F28" t="n">
-        <v>3.9428</v>
+        <v>3.46879</v>
       </c>
     </row>
     <row r="29">
@@ -1127,16 +1127,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3559.51</v>
+        <v>3548.45</v>
       </c>
       <c r="D29" t="n">
-        <v>6194902543</v>
+        <v>6174101568</v>
       </c>
       <c r="E29" t="n">
-        <v>105782378</v>
+        <v>105211848</v>
       </c>
       <c r="F29" t="n">
-        <v>8.69229</v>
+        <v>8.140940000000001</v>
       </c>
     </row>
     <row r="30">
@@ -1151,88 +1151,88 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9.35</v>
+        <v>9.33</v>
       </c>
       <c r="D30" t="n">
-        <v>5614203040</v>
+        <v>5610657297</v>
       </c>
       <c r="E30" t="n">
-        <v>870750030</v>
+        <v>871047022</v>
       </c>
       <c r="F30" t="n">
-        <v>5.84469</v>
+        <v>5.54208</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>cro</t>
+          <t>hbar</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.195065</v>
+        <v>0.138456</v>
       </c>
       <c r="D31" t="n">
-        <v>5341306291</v>
+        <v>5260297033</v>
       </c>
       <c r="E31" t="n">
-        <v>141273639</v>
+        <v>953925782</v>
       </c>
       <c r="F31" t="n">
-        <v>11.78849</v>
+        <v>10.34519</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>USDS</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>hbar</t>
+          <t>usds</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.137038</v>
+        <v>0.998479</v>
       </c>
       <c r="D32" t="n">
-        <v>5238270224</v>
+        <v>5235359178</v>
       </c>
       <c r="E32" t="n">
-        <v>934498283</v>
+        <v>15996881</v>
       </c>
       <c r="F32" t="n">
-        <v>10.09357</v>
+        <v>-0.59761</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>USDS</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>usds</t>
+          <t>cro</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.999299</v>
+        <v>0.189654</v>
       </c>
       <c r="D33" t="n">
-        <v>5230226962</v>
+        <v>5165132662</v>
       </c>
       <c r="E33" t="n">
-        <v>16080506</v>
+        <v>147234964</v>
       </c>
       <c r="F33" t="n">
-        <v>-0.32212</v>
+        <v>8.17057</v>
       </c>
     </row>
     <row r="34">
@@ -1247,16 +1247,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9.66</v>
+        <v>9.630000000000001</v>
       </c>
       <c r="D34" t="n">
-        <v>4584170683</v>
+        <v>4579534087</v>
       </c>
       <c r="E34" t="n">
-        <v>274022971</v>
+        <v>273635929</v>
       </c>
       <c r="F34" t="n">
-        <v>7.12318</v>
+        <v>6.76845</v>
       </c>
     </row>
     <row r="35">
@@ -1271,16 +1271,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>28.06</v>
+        <v>27.99</v>
       </c>
       <c r="D35" t="n">
-        <v>4199695234</v>
+        <v>4205246650</v>
       </c>
       <c r="E35" t="n">
-        <v>866959534</v>
+        <v>864501403</v>
       </c>
       <c r="F35" t="n">
-        <v>5.17743</v>
+        <v>4.88331</v>
       </c>
     </row>
     <row r="36">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>5.233e-05</v>
+        <v>5.235e-05</v>
       </c>
       <c r="D36" t="n">
-        <v>3919437831</v>
+        <v>3929105870</v>
       </c>
       <c r="E36" t="n">
-        <v>1630787456</v>
+        <v>1612558748</v>
       </c>
       <c r="F36" t="n">
-        <v>0.41931</v>
+        <v>-0.81293</v>
       </c>
     </row>
     <row r="37">
@@ -1319,16 +1319,16 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.152056</v>
+        <v>0.152247</v>
       </c>
       <c r="D37" t="n">
-        <v>3832081221</v>
+        <v>3838980805</v>
       </c>
       <c r="E37" t="n">
-        <v>151141330</v>
+        <v>150112818</v>
       </c>
       <c r="F37" t="n">
-        <v>0.92423</v>
+        <v>0.94309</v>
       </c>
     </row>
     <row r="38">
@@ -1343,16 +1343,16 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>7.37</v>
+        <v>7.35</v>
       </c>
       <c r="D38" t="n">
-        <v>3813426846</v>
+        <v>3813718303</v>
       </c>
       <c r="E38" t="n">
-        <v>430485438</v>
+        <v>430257724</v>
       </c>
       <c r="F38" t="n">
-        <v>0.49782</v>
+        <v>0.43552</v>
       </c>
     </row>
     <row r="39">
@@ -1367,16 +1367,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.467282</v>
+        <v>0.465096</v>
       </c>
       <c r="D39" t="n">
-        <v>3723235499</v>
+        <v>3708833312</v>
       </c>
       <c r="E39" t="n">
-        <v>497017761</v>
+        <v>499273661</v>
       </c>
       <c r="F39" t="n">
-        <v>6.94723</v>
+        <v>6.25999</v>
       </c>
     </row>
     <row r="40">
@@ -1391,16 +1391,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>502.34</v>
+        <v>501.34</v>
       </c>
       <c r="D40" t="n">
-        <v>3722424094</v>
+        <v>3702918639</v>
       </c>
       <c r="E40" t="n">
-        <v>280112348</v>
+        <v>279730680</v>
       </c>
       <c r="F40" t="n">
-        <v>3.21335</v>
+        <v>3.40664</v>
       </c>
     </row>
     <row r="41">
@@ -1418,13 +1418,13 @@
         <v>1.001</v>
       </c>
       <c r="D41" t="n">
-        <v>3686884674</v>
+        <v>3685203575</v>
       </c>
       <c r="E41" t="n">
-        <v>224249364</v>
+        <v>223710665</v>
       </c>
       <c r="F41" t="n">
-        <v>-0.08049000000000001</v>
+        <v>-0.39308</v>
       </c>
     </row>
     <row r="42">
@@ -1439,16 +1439,16 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>24.77</v>
+        <v>24.79</v>
       </c>
       <c r="D42" t="n">
-        <v>3575145979</v>
+        <v>3574017253</v>
       </c>
       <c r="E42" t="n">
-        <v>33131314</v>
+        <v>31550147</v>
       </c>
       <c r="F42" t="n">
-        <v>2.74346</v>
+        <v>2.82256</v>
       </c>
     </row>
     <row r="43">
@@ -1463,16 +1463,16 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.999429</v>
+        <v>0.9993109999999999</v>
       </c>
       <c r="D43" t="n">
-        <v>3439660368</v>
+        <v>3444947266</v>
       </c>
       <c r="E43" t="n">
-        <v>184363126</v>
+        <v>179507355</v>
       </c>
       <c r="F43" t="n">
-        <v>0.14324</v>
+        <v>-0.05053</v>
       </c>
     </row>
     <row r="44">
@@ -1490,13 +1490,13 @@
         <v>3.82</v>
       </c>
       <c r="D44" t="n">
-        <v>3439598122</v>
+        <v>3440542892</v>
       </c>
       <c r="E44" t="n">
-        <v>304755108</v>
+        <v>304974175</v>
       </c>
       <c r="F44" t="n">
-        <v>5.80427</v>
+        <v>5.08724</v>
       </c>
     </row>
     <row r="45">
@@ -1511,16 +1511,16 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3.38</v>
+        <v>3.36</v>
       </c>
       <c r="D45" t="n">
-        <v>3377151669</v>
+        <v>3353709873</v>
       </c>
       <c r="E45" t="n">
-        <v>1281353338</v>
+        <v>1288616085</v>
       </c>
       <c r="F45" t="n">
-        <v>5.16064</v>
+        <v>5.23119</v>
       </c>
     </row>
     <row r="46">
@@ -1538,13 +1538,13 @@
         <v>1.28</v>
       </c>
       <c r="D46" t="n">
-        <v>3350991172</v>
+        <v>3341022642</v>
       </c>
       <c r="E46" t="n">
-        <v>481757661</v>
+        <v>483200976</v>
       </c>
       <c r="F46" t="n">
-        <v>3.13522</v>
+        <v>2.98349</v>
       </c>
     </row>
     <row r="47">
@@ -1559,16 +1559,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.789976</v>
+        <v>0.786529</v>
       </c>
       <c r="D47" t="n">
-        <v>3236809423</v>
+        <v>3225954936</v>
       </c>
       <c r="E47" t="n">
-        <v>1676829198</v>
+        <v>1673163724</v>
       </c>
       <c r="F47" t="n">
-        <v>14.39195</v>
+        <v>13.77642</v>
       </c>
     </row>
     <row r="48">
@@ -1583,16 +1583,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>161.18</v>
+        <v>160.51</v>
       </c>
       <c r="D48" t="n">
-        <v>2972719324</v>
+        <v>2968018563</v>
       </c>
       <c r="E48" t="n">
-        <v>83675039</v>
+        <v>85853749</v>
       </c>
       <c r="F48" t="n">
-        <v>-0.35097</v>
+        <v>-0.55401</v>
       </c>
     </row>
     <row r="49">
@@ -1610,61 +1610,61 @@
         <v>1.96</v>
       </c>
       <c r="D49" t="n">
-        <v>2943890749</v>
+        <v>2944746477</v>
       </c>
       <c r="E49" t="n">
-        <v>352719354</v>
+        <v>350307514</v>
       </c>
       <c r="F49" t="n">
-        <v>2.63933</v>
+        <v>2.22298</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>mnt</t>
+          <t>fil</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.838499</v>
+        <v>4.68</v>
       </c>
       <c r="D50" t="n">
-        <v>2824529619</v>
+        <v>2816547654</v>
       </c>
       <c r="E50" t="n">
-        <v>185914513</v>
+        <v>574134364</v>
       </c>
       <c r="F50" t="n">
-        <v>15.13845</v>
+        <v>6.59424</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>fil</t>
+          <t>mnt</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>4.69</v>
+        <v>0.835849</v>
       </c>
       <c r="D51" t="n">
-        <v>2815699050</v>
+        <v>2813809441</v>
       </c>
       <c r="E51" t="n">
-        <v>576199430</v>
+        <v>186127050</v>
       </c>
       <c r="F51" t="n">
-        <v>7.35606</v>
+        <v>14.36165</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1954198009844</v>
+        <v>1959698004531</v>
       </c>
     </row>
     <row r="3">
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>406670065516</v>
+        <v>406338286340</v>
       </c>
     </row>
     <row r="4">
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>130821581010</v>
+        <v>130970143446</v>
       </c>
     </row>
     <row r="5">
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>123188156523</v>
+        <v>123494602662</v>
       </c>
     </row>
     <row r="6">
@@ -1745,7 +1745,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>92052602155</v>
+        <v>92034027631</v>
       </c>
     </row>
   </sheetData>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$4348.00</t>
+          <t>$4345.48</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>XRP (26.94%)</t>
+          <t>XRP (26.93%)</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bitcoin Cash (-4.18%)</t>
+          <t>Bitcoin Cash (-6.09%)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Excel data - 2024-11-22 06:36:39
</commit_message>
<xml_diff>
--- a/crypto_live_data.xlsx
+++ b/crypto_live_data.xlsx
@@ -479,16 +479,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>98890</v>
+        <v>98821</v>
       </c>
       <c r="D2" t="n">
-        <v>1959698004531</v>
+        <v>1955065374675</v>
       </c>
       <c r="E2" t="n">
-        <v>111556511395</v>
+        <v>107185165245</v>
       </c>
       <c r="F2" t="n">
-        <v>1.79611</v>
+        <v>1.52129</v>
       </c>
     </row>
     <row r="3">
@@ -503,16 +503,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3368.92</v>
+        <v>3367.93</v>
       </c>
       <c r="D3" t="n">
-        <v>406338286340</v>
+        <v>405569114425</v>
       </c>
       <c r="E3" t="n">
-        <v>57069836564</v>
+        <v>56041266202</v>
       </c>
       <c r="F3" t="n">
-        <v>8.067830000000001</v>
+        <v>7.93654</v>
       </c>
     </row>
     <row r="4">
@@ -530,13 +530,13 @@
         <v>1.001</v>
       </c>
       <c r="D4" t="n">
-        <v>130970143446</v>
+        <v>130803059570</v>
       </c>
       <c r="E4" t="n">
-        <v>182938028684</v>
+        <v>112196096160</v>
       </c>
       <c r="F4" t="n">
-        <v>0.09354999999999999</v>
+        <v>0.05625</v>
       </c>
     </row>
     <row r="5">
@@ -551,16 +551,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>259.58</v>
+        <v>259.04</v>
       </c>
       <c r="D5" t="n">
-        <v>123494602662</v>
+        <v>122966673076</v>
       </c>
       <c r="E5" t="n">
-        <v>14771296331</v>
+        <v>14806263273</v>
       </c>
       <c r="F5" t="n">
-        <v>8.85698</v>
+        <v>8.57286</v>
       </c>
     </row>
     <row r="6">
@@ -575,16 +575,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>630.27</v>
+        <v>629.9299999999999</v>
       </c>
       <c r="D6" t="n">
-        <v>92034027631</v>
+        <v>91896601685</v>
       </c>
       <c r="E6" t="n">
-        <v>2506552932</v>
+        <v>2508195564</v>
       </c>
       <c r="F6" t="n">
-        <v>3.43071</v>
+        <v>3.24204</v>
       </c>
     </row>
     <row r="7">
@@ -599,16 +599,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.41</v>
+        <v>1.4</v>
       </c>
       <c r="D7" t="n">
-        <v>80278940768</v>
+        <v>79973167811</v>
       </c>
       <c r="E7" t="n">
-        <v>18503538652</v>
+        <v>18537037700</v>
       </c>
       <c r="F7" t="n">
-        <v>26.92868</v>
+        <v>26.17071</v>
       </c>
     </row>
     <row r="8">
@@ -623,16 +623,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.393778</v>
+        <v>0.394029</v>
       </c>
       <c r="D8" t="n">
-        <v>58027240960</v>
+        <v>57858872160</v>
       </c>
       <c r="E8" t="n">
-        <v>9748555380</v>
+        <v>9755401127</v>
       </c>
       <c r="F8" t="n">
-        <v>2.59959</v>
+        <v>2.45483</v>
       </c>
     </row>
     <row r="9">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.999411</v>
+        <v>0.9998</v>
       </c>
       <c r="D9" t="n">
-        <v>38359750699</v>
+        <v>38307987931</v>
       </c>
       <c r="E9" t="n">
-        <v>10847807727</v>
+        <v>15326576712</v>
       </c>
       <c r="F9" t="n">
-        <v>0.02544</v>
+        <v>-0.04826</v>
       </c>
     </row>
     <row r="10">
@@ -671,16 +671,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3368.18</v>
+        <v>3367.81</v>
       </c>
       <c r="D10" t="n">
-        <v>33037771601</v>
+        <v>33004494921</v>
       </c>
       <c r="E10" t="n">
-        <v>140321815</v>
+        <v>138827377</v>
       </c>
       <c r="F10" t="n">
-        <v>7.94378</v>
+        <v>7.92654</v>
       </c>
     </row>
     <row r="11">
@@ -695,16 +695,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.884283</v>
+        <v>0.880489</v>
       </c>
       <c r="D11" t="n">
-        <v>31681007165</v>
+        <v>31509087095</v>
       </c>
       <c r="E11" t="n">
-        <v>3764850697</v>
+        <v>3762401528</v>
       </c>
       <c r="F11" t="n">
-        <v>12.03466</v>
+        <v>11.75574</v>
       </c>
     </row>
     <row r="12">
@@ -719,16 +719,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.199391</v>
+        <v>0.199221</v>
       </c>
       <c r="D12" t="n">
-        <v>17228471586</v>
+        <v>17202885060</v>
       </c>
       <c r="E12" t="n">
-        <v>1069521924</v>
+        <v>1073391665</v>
       </c>
       <c r="F12" t="n">
-        <v>0.93377</v>
+        <v>0.92219</v>
       </c>
     </row>
     <row r="13">
@@ -743,16 +743,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>36.25</v>
+        <v>36.16</v>
       </c>
       <c r="D13" t="n">
-        <v>14850836971</v>
+        <v>14793159228</v>
       </c>
       <c r="E13" t="n">
-        <v>1041350077</v>
+        <v>1040535609</v>
       </c>
       <c r="F13" t="n">
-        <v>6.74635</v>
+        <v>6.46775</v>
       </c>
     </row>
     <row r="14">
@@ -770,13 +770,13 @@
         <v>2.487e-05</v>
       </c>
       <c r="D14" t="n">
-        <v>14667878935</v>
+        <v>14652797101</v>
       </c>
       <c r="E14" t="n">
-        <v>1592407723</v>
+        <v>1598117103</v>
       </c>
       <c r="F14" t="n">
-        <v>3.34849</v>
+        <v>3.12022</v>
       </c>
     </row>
     <row r="15">
@@ -791,16 +791,16 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>3994.45</v>
+        <v>4000.6</v>
       </c>
       <c r="D15" t="n">
-        <v>14430087078</v>
+        <v>14442456649</v>
       </c>
       <c r="E15" t="n">
-        <v>170220205</v>
+        <v>172086574</v>
       </c>
       <c r="F15" t="n">
-        <v>7.91847</v>
+        <v>8.18927</v>
       </c>
     </row>
     <row r="16">
@@ -815,16 +815,16 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>98404</v>
+        <v>98638</v>
       </c>
       <c r="D16" t="n">
-        <v>14398635396</v>
+        <v>14408704518</v>
       </c>
       <c r="E16" t="n">
-        <v>820480113</v>
+        <v>826177901</v>
       </c>
       <c r="F16" t="n">
-        <v>1.45316</v>
+        <v>1.6381</v>
       </c>
     </row>
     <row r="17">
@@ -839,16 +839,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5.53</v>
+        <v>5.52</v>
       </c>
       <c r="D17" t="n">
-        <v>14095403038</v>
+        <v>14069277184</v>
       </c>
       <c r="E17" t="n">
-        <v>624264587</v>
+        <v>625981057</v>
       </c>
       <c r="F17" t="n">
-        <v>2.79731</v>
+        <v>1.96154</v>
       </c>
     </row>
     <row r="18">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3.6</v>
+        <v>3.59</v>
       </c>
       <c r="D18" t="n">
-        <v>10245919377</v>
+        <v>10230076114</v>
       </c>
       <c r="E18" t="n">
-        <v>2093423841</v>
+        <v>2195757402</v>
       </c>
       <c r="F18" t="n">
-        <v>0.87947</v>
+        <v>0.85599</v>
       </c>
     </row>
     <row r="19">
@@ -887,16 +887,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>495.73</v>
+        <v>493.97</v>
       </c>
       <c r="D19" t="n">
-        <v>9835172618</v>
+        <v>9775691671</v>
       </c>
       <c r="E19" t="n">
-        <v>1749875615</v>
+        <v>1709315082</v>
       </c>
       <c r="F19" t="n">
-        <v>-6.09258</v>
+        <v>-6.39473</v>
       </c>
     </row>
     <row r="20">
@@ -911,16 +911,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3363.77</v>
+        <v>3365.9</v>
       </c>
       <c r="D20" t="n">
-        <v>9656540862</v>
+        <v>9644552154</v>
       </c>
       <c r="E20" t="n">
-        <v>2085909929</v>
+        <v>1442232704</v>
       </c>
       <c r="F20" t="n">
-        <v>7.97274</v>
+        <v>8.026949999999999</v>
       </c>
     </row>
     <row r="21">
@@ -935,16 +935,16 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>15.26</v>
+        <v>15.27</v>
       </c>
       <c r="D21" t="n">
-        <v>9606079703</v>
+        <v>9572585986</v>
       </c>
       <c r="E21" t="n">
-        <v>1257251807</v>
+        <v>1260125079</v>
       </c>
       <c r="F21" t="n">
-        <v>4.59659</v>
+        <v>4.8129</v>
       </c>
     </row>
     <row r="22">
@@ -959,16 +959,16 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.13e-05</v>
+        <v>2.131e-05</v>
       </c>
       <c r="D22" t="n">
-        <v>8960436990</v>
+        <v>8965828127</v>
       </c>
       <c r="E22" t="n">
-        <v>6723740508</v>
+        <v>6726966462</v>
       </c>
       <c r="F22" t="n">
-        <v>9.34882</v>
+        <v>9.410690000000001</v>
       </c>
     </row>
     <row r="23">
@@ -983,16 +983,16 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>6.22</v>
+        <v>6.21</v>
       </c>
       <c r="D23" t="n">
-        <v>8956646967</v>
+        <v>8949858104</v>
       </c>
       <c r="E23" t="n">
-        <v>844240722</v>
+        <v>844734603</v>
       </c>
       <c r="F23" t="n">
-        <v>9.40147</v>
+        <v>9.40584</v>
       </c>
     </row>
     <row r="24">
@@ -1007,16 +1007,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.287774</v>
+        <v>0.286915</v>
       </c>
       <c r="D24" t="n">
-        <v>8635355878</v>
+        <v>8617828912</v>
       </c>
       <c r="E24" t="n">
-        <v>2343798557</v>
+        <v>2346286480</v>
       </c>
       <c r="F24" t="n">
-        <v>21.1674</v>
+        <v>20.77031</v>
       </c>
     </row>
     <row r="25">
@@ -1031,16 +1031,16 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>8.81</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="D25" t="n">
-        <v>8139643571</v>
+        <v>8133488447</v>
       </c>
       <c r="E25" t="n">
-        <v>3400762</v>
+        <v>3391395</v>
       </c>
       <c r="F25" t="n">
-        <v>3.85022</v>
+        <v>3.53993</v>
       </c>
     </row>
     <row r="26">
@@ -1055,16 +1055,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>5.78</v>
+        <v>5.76</v>
       </c>
       <c r="D26" t="n">
-        <v>7046717485</v>
+        <v>7015382282</v>
       </c>
       <c r="E26" t="n">
-        <v>1003167791</v>
+        <v>1003512868</v>
       </c>
       <c r="F26" t="n">
-        <v>4.90486</v>
+        <v>4.87787</v>
       </c>
     </row>
     <row r="27">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>90.59</v>
+        <v>90.18000000000001</v>
       </c>
       <c r="D27" t="n">
-        <v>6833848492</v>
+        <v>6783548458</v>
       </c>
       <c r="E27" t="n">
-        <v>1334339155</v>
+        <v>1315864262</v>
       </c>
       <c r="F27" t="n">
-        <v>2.55445</v>
+        <v>1.30091</v>
       </c>
     </row>
     <row r="28">
@@ -1103,16 +1103,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>12.04</v>
+        <v>12.02</v>
       </c>
       <c r="D28" t="n">
-        <v>6423652211</v>
+        <v>6422121172</v>
       </c>
       <c r="E28" t="n">
-        <v>846792578</v>
+        <v>848170177</v>
       </c>
       <c r="F28" t="n">
-        <v>3.46879</v>
+        <v>3.68462</v>
       </c>
     </row>
     <row r="29">
@@ -1127,16 +1127,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3548.45</v>
+        <v>3546.31</v>
       </c>
       <c r="D29" t="n">
-        <v>6174101568</v>
+        <v>6169611515</v>
       </c>
       <c r="E29" t="n">
-        <v>105211848</v>
+        <v>103651261</v>
       </c>
       <c r="F29" t="n">
-        <v>8.140940000000001</v>
+        <v>8.18763</v>
       </c>
     </row>
     <row r="30">
@@ -1151,16 +1151,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9.33</v>
+        <v>9.32</v>
       </c>
       <c r="D30" t="n">
-        <v>5610657297</v>
+        <v>5595254907</v>
       </c>
       <c r="E30" t="n">
-        <v>871047022</v>
+        <v>872429790</v>
       </c>
       <c r="F30" t="n">
-        <v>5.54208</v>
+        <v>5.52257</v>
       </c>
     </row>
     <row r="31">
@@ -1175,16 +1175,16 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.138456</v>
+        <v>0.138422</v>
       </c>
       <c r="D31" t="n">
-        <v>5260297033</v>
+        <v>5288274559</v>
       </c>
       <c r="E31" t="n">
-        <v>953925782</v>
+        <v>964046702</v>
       </c>
       <c r="F31" t="n">
-        <v>10.34519</v>
+        <v>10.79753</v>
       </c>
     </row>
     <row r="32">
@@ -1199,16 +1199,16 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.998479</v>
+        <v>0.9990520000000001</v>
       </c>
       <c r="D32" t="n">
-        <v>5235359178</v>
+        <v>5226406988</v>
       </c>
       <c r="E32" t="n">
-        <v>15996881</v>
+        <v>16006065</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.59761</v>
+        <v>-0.36705</v>
       </c>
     </row>
     <row r="33">
@@ -1223,16 +1223,16 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.189654</v>
+        <v>0.187995</v>
       </c>
       <c r="D33" t="n">
-        <v>5165132662</v>
+        <v>5141784943</v>
       </c>
       <c r="E33" t="n">
-        <v>147234964</v>
+        <v>150634106</v>
       </c>
       <c r="F33" t="n">
-        <v>8.17057</v>
+        <v>7.82868</v>
       </c>
     </row>
     <row r="34">
@@ -1247,16 +1247,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9.630000000000001</v>
+        <v>9.6</v>
       </c>
       <c r="D34" t="n">
-        <v>4579534087</v>
+        <v>4555261310</v>
       </c>
       <c r="E34" t="n">
-        <v>273635929</v>
+        <v>273488349</v>
       </c>
       <c r="F34" t="n">
-        <v>6.76845</v>
+        <v>6.60921</v>
       </c>
     </row>
     <row r="35">
@@ -1271,16 +1271,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>27.99</v>
+        <v>27.94</v>
       </c>
       <c r="D35" t="n">
-        <v>4205246650</v>
+        <v>4180801808</v>
       </c>
       <c r="E35" t="n">
-        <v>864501403</v>
+        <v>861244532</v>
       </c>
       <c r="F35" t="n">
-        <v>4.88331</v>
+        <v>4.70517</v>
       </c>
     </row>
     <row r="36">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>5.235e-05</v>
+        <v>5.242e-05</v>
       </c>
       <c r="D36" t="n">
-        <v>3929105870</v>
+        <v>3950095141</v>
       </c>
       <c r="E36" t="n">
-        <v>1612558748</v>
+        <v>1601466165</v>
       </c>
       <c r="F36" t="n">
-        <v>-0.81293</v>
+        <v>-0.10235</v>
       </c>
     </row>
     <row r="37">
@@ -1319,16 +1319,16 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.152247</v>
+        <v>0.151879</v>
       </c>
       <c r="D37" t="n">
-        <v>3838980805</v>
+        <v>3832713780</v>
       </c>
       <c r="E37" t="n">
-        <v>150112818</v>
+        <v>150125959</v>
       </c>
       <c r="F37" t="n">
-        <v>0.94309</v>
+        <v>0.45116</v>
       </c>
     </row>
     <row r="38">
@@ -1343,16 +1343,16 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>7.35</v>
+        <v>7.34</v>
       </c>
       <c r="D38" t="n">
-        <v>3813718303</v>
+        <v>3801653465</v>
       </c>
       <c r="E38" t="n">
-        <v>430257724</v>
+        <v>429954829</v>
       </c>
       <c r="F38" t="n">
-        <v>0.43552</v>
+        <v>0.74086</v>
       </c>
     </row>
     <row r="39">
@@ -1367,16 +1367,16 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.465096</v>
+        <v>0.465237</v>
       </c>
       <c r="D39" t="n">
-        <v>3708833312</v>
+        <v>3705435184</v>
       </c>
       <c r="E39" t="n">
-        <v>499273661</v>
+        <v>501118230</v>
       </c>
       <c r="F39" t="n">
-        <v>6.25999</v>
+        <v>6.34705</v>
       </c>
     </row>
     <row r="40">
@@ -1391,16 +1391,16 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>501.34</v>
+        <v>500.21</v>
       </c>
       <c r="D40" t="n">
-        <v>3702918639</v>
+        <v>3696581786</v>
       </c>
       <c r="E40" t="n">
-        <v>279730680</v>
+        <v>280047488</v>
       </c>
       <c r="F40" t="n">
-        <v>3.40664</v>
+        <v>3.58771</v>
       </c>
     </row>
     <row r="41">
@@ -1415,16 +1415,16 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1.001</v>
+        <v>1.002</v>
       </c>
       <c r="D41" t="n">
-        <v>3685203575</v>
+        <v>3688254516</v>
       </c>
       <c r="E41" t="n">
-        <v>223710665</v>
+        <v>222230206</v>
       </c>
       <c r="F41" t="n">
-        <v>-0.39308</v>
+        <v>-0.18498</v>
       </c>
     </row>
     <row r="42">
@@ -1439,16 +1439,16 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>24.79</v>
+        <v>24.78</v>
       </c>
       <c r="D42" t="n">
-        <v>3574017253</v>
+        <v>3570818581</v>
       </c>
       <c r="E42" t="n">
-        <v>31550147</v>
+        <v>32982943</v>
       </c>
       <c r="F42" t="n">
-        <v>2.82256</v>
+        <v>2.58192</v>
       </c>
     </row>
     <row r="43">
@@ -1463,16 +1463,16 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.9993109999999999</v>
+        <v>0.999769</v>
       </c>
       <c r="D43" t="n">
-        <v>3444947266</v>
+        <v>3441159133</v>
       </c>
       <c r="E43" t="n">
-        <v>179507355</v>
+        <v>151317872</v>
       </c>
       <c r="F43" t="n">
-        <v>-0.05053</v>
+        <v>-0.09085</v>
       </c>
     </row>
     <row r="44">
@@ -1490,13 +1490,13 @@
         <v>3.82</v>
       </c>
       <c r="D44" t="n">
-        <v>3440542892</v>
+        <v>3439796552</v>
       </c>
       <c r="E44" t="n">
-        <v>304974175</v>
+        <v>304975628</v>
       </c>
       <c r="F44" t="n">
-        <v>5.08724</v>
+        <v>5.48871</v>
       </c>
     </row>
     <row r="45">
@@ -1511,16 +1511,16 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3.36</v>
+        <v>3.34</v>
       </c>
       <c r="D45" t="n">
-        <v>3353709873</v>
+        <v>3349732168</v>
       </c>
       <c r="E45" t="n">
-        <v>1288616085</v>
+        <v>1291008898</v>
       </c>
       <c r="F45" t="n">
-        <v>5.23119</v>
+        <v>5.12188</v>
       </c>
     </row>
     <row r="46">
@@ -1538,13 +1538,13 @@
         <v>1.28</v>
       </c>
       <c r="D46" t="n">
-        <v>3341022642</v>
+        <v>3329445059</v>
       </c>
       <c r="E46" t="n">
-        <v>483200976</v>
+        <v>482295249</v>
       </c>
       <c r="F46" t="n">
-        <v>2.98349</v>
+        <v>3.22596</v>
       </c>
     </row>
     <row r="47">
@@ -1559,16 +1559,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.786529</v>
+        <v>0.783631</v>
       </c>
       <c r="D47" t="n">
-        <v>3225954936</v>
+        <v>3213465867</v>
       </c>
       <c r="E47" t="n">
-        <v>1673163724</v>
+        <v>1670862527</v>
       </c>
       <c r="F47" t="n">
-        <v>13.77642</v>
+        <v>13.38334</v>
       </c>
     </row>
     <row r="48">
@@ -1583,16 +1583,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>160.51</v>
+        <v>160.73</v>
       </c>
       <c r="D48" t="n">
-        <v>2968018563</v>
+        <v>2965520995</v>
       </c>
       <c r="E48" t="n">
-        <v>85853749</v>
+        <v>85739377</v>
       </c>
       <c r="F48" t="n">
-        <v>-0.55401</v>
+        <v>-0.53269</v>
       </c>
     </row>
     <row r="49">
@@ -1610,13 +1610,13 @@
         <v>1.96</v>
       </c>
       <c r="D49" t="n">
-        <v>2944746477</v>
+        <v>2935957058</v>
       </c>
       <c r="E49" t="n">
-        <v>350307514</v>
+        <v>349512301</v>
       </c>
       <c r="F49" t="n">
-        <v>2.22298</v>
+        <v>1.94279</v>
       </c>
     </row>
     <row r="50">
@@ -1631,16 +1631,16 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>4.68</v>
+        <v>4.67</v>
       </c>
       <c r="D50" t="n">
-        <v>2816547654</v>
+        <v>2807537544</v>
       </c>
       <c r="E50" t="n">
-        <v>574134364</v>
+        <v>567842261</v>
       </c>
       <c r="F50" t="n">
-        <v>6.59424</v>
+        <v>5.23522</v>
       </c>
     </row>
     <row r="51">
@@ -1655,16 +1655,16 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.835849</v>
+        <v>0.832329</v>
       </c>
       <c r="D51" t="n">
-        <v>2813809441</v>
+        <v>2803686073</v>
       </c>
       <c r="E51" t="n">
-        <v>186127050</v>
+        <v>186631406</v>
       </c>
       <c r="F51" t="n">
-        <v>14.36165</v>
+        <v>13.99973</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1959698004531</v>
+        <v>1955065374675</v>
       </c>
     </row>
     <row r="3">
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>406338286340</v>
+        <v>405569114425</v>
       </c>
     </row>
     <row r="4">
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>130970143446</v>
+        <v>130803059570</v>
       </c>
     </row>
     <row r="5">
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>123494602662</v>
+        <v>122966673076</v>
       </c>
     </row>
     <row r="6">
@@ -1745,7 +1745,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>92034027631</v>
+        <v>91896601685</v>
       </c>
     </row>
   </sheetData>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$4345.48</t>
+          <t>$4348.79</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>XRP (26.93%)</t>
+          <t>XRP (26.17%)</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bitcoin Cash (-6.09%)</t>
+          <t>Bitcoin Cash (-6.39%)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Excel data - 2024-11-22 07:27:27
</commit_message>
<xml_diff>
--- a/crypto_live_data.xlsx
+++ b/crypto_live_data.xlsx
@@ -479,16 +479,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>98821</v>
+        <v>99312</v>
       </c>
       <c r="D2" t="n">
-        <v>1955065374675</v>
+        <v>1964885477649</v>
       </c>
       <c r="E2" t="n">
-        <v>107185165245</v>
+        <v>113255252996</v>
       </c>
       <c r="F2" t="n">
-        <v>1.52129</v>
+        <v>2.22498</v>
       </c>
     </row>
     <row r="3">
@@ -503,16 +503,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3367.93</v>
+        <v>3382.34</v>
       </c>
       <c r="D3" t="n">
-        <v>405569114425</v>
+        <v>407330066375</v>
       </c>
       <c r="E3" t="n">
-        <v>56041266202</v>
+        <v>55601389931</v>
       </c>
       <c r="F3" t="n">
-        <v>7.93654</v>
+        <v>8.13508</v>
       </c>
     </row>
     <row r="4">
@@ -527,16 +527,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.001</v>
+        <v>1.002</v>
       </c>
       <c r="D4" t="n">
-        <v>130803059570</v>
+        <v>130971083766</v>
       </c>
       <c r="E4" t="n">
-        <v>112196096160</v>
+        <v>163378253649</v>
       </c>
       <c r="F4" t="n">
-        <v>0.05625</v>
+        <v>0.22326</v>
       </c>
     </row>
     <row r="5">
@@ -551,16 +551,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>259.04</v>
+        <v>260.27</v>
       </c>
       <c r="D5" t="n">
-        <v>122966673076</v>
+        <v>123363846725</v>
       </c>
       <c r="E5" t="n">
-        <v>14806263273</v>
+        <v>14848849268</v>
       </c>
       <c r="F5" t="n">
-        <v>8.57286</v>
+        <v>8.202220000000001</v>
       </c>
     </row>
     <row r="6">
@@ -575,16 +575,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>629.9299999999999</v>
+        <v>630.05</v>
       </c>
       <c r="D6" t="n">
-        <v>91896601685</v>
+        <v>91918590252</v>
       </c>
       <c r="E6" t="n">
-        <v>2508195564</v>
+        <v>2463785495</v>
       </c>
       <c r="F6" t="n">
-        <v>3.24204</v>
+        <v>3.08464</v>
       </c>
     </row>
     <row r="7">
@@ -599,16 +599,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1.4</v>
+        <v>1.38</v>
       </c>
       <c r="D7" t="n">
-        <v>79973167811</v>
+        <v>78351850071</v>
       </c>
       <c r="E7" t="n">
-        <v>18537037700</v>
+        <v>18601406930</v>
       </c>
       <c r="F7" t="n">
-        <v>26.17071</v>
+        <v>24.35371</v>
       </c>
     </row>
     <row r="8">
@@ -623,16 +623,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.394029</v>
+        <v>0.393685</v>
       </c>
       <c r="D8" t="n">
-        <v>57858872160</v>
+        <v>57826630115</v>
       </c>
       <c r="E8" t="n">
-        <v>9755401127</v>
+        <v>9916799832</v>
       </c>
       <c r="F8" t="n">
-        <v>2.45483</v>
+        <v>2.16947</v>
       </c>
     </row>
     <row r="9">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.9998</v>
+        <v>1.001</v>
       </c>
       <c r="D9" t="n">
-        <v>38307987931</v>
+        <v>38353944271</v>
       </c>
       <c r="E9" t="n">
-        <v>15326576712</v>
+        <v>11520333341</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.04826</v>
+        <v>0.14266</v>
       </c>
     </row>
     <row r="10">
@@ -671,16 +671,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3367.81</v>
+        <v>3379.11</v>
       </c>
       <c r="D10" t="n">
-        <v>33004494921</v>
+        <v>33107787454</v>
       </c>
       <c r="E10" t="n">
-        <v>138827377</v>
+        <v>136354656</v>
       </c>
       <c r="F10" t="n">
-        <v>7.92654</v>
+        <v>8.024570000000001</v>
       </c>
     </row>
     <row r="11">
@@ -695,16 +695,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.880489</v>
+        <v>0.872225</v>
       </c>
       <c r="D11" t="n">
-        <v>31509087095</v>
+        <v>31216576721</v>
       </c>
       <c r="E11" t="n">
-        <v>3762401528</v>
+        <v>3791307986</v>
       </c>
       <c r="F11" t="n">
-        <v>11.75574</v>
+        <v>11.45673</v>
       </c>
     </row>
     <row r="12">
@@ -719,16 +719,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.199221</v>
+        <v>0.199188</v>
       </c>
       <c r="D12" t="n">
-        <v>17202885060</v>
+        <v>17201131227</v>
       </c>
       <c r="E12" t="n">
-        <v>1073391665</v>
+        <v>1059695671</v>
       </c>
       <c r="F12" t="n">
-        <v>0.92219</v>
+        <v>0.77823</v>
       </c>
     </row>
     <row r="13">
@@ -743,16 +743,16 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>36.16</v>
+        <v>36.07</v>
       </c>
       <c r="D13" t="n">
-        <v>14793159228</v>
+        <v>14780229554</v>
       </c>
       <c r="E13" t="n">
-        <v>1040535609</v>
+        <v>1043439241</v>
       </c>
       <c r="F13" t="n">
-        <v>6.46775</v>
+        <v>6.33091</v>
       </c>
     </row>
     <row r="14">
@@ -767,64 +767,64 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2.487e-05</v>
+        <v>2.482e-05</v>
       </c>
       <c r="D14" t="n">
-        <v>14652797101</v>
+        <v>14642413929</v>
       </c>
       <c r="E14" t="n">
-        <v>1598117103</v>
+        <v>1621005217</v>
       </c>
       <c r="F14" t="n">
-        <v>3.12022</v>
+        <v>2.97838</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Wrapped stETH</t>
+          <t>Wrapped Bitcoin</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>wsteth</t>
+          <t>wbtc</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>4000.6</v>
+        <v>98838</v>
       </c>
       <c r="D15" t="n">
-        <v>14442456649</v>
+        <v>14444179786</v>
       </c>
       <c r="E15" t="n">
-        <v>172086574</v>
+        <v>805312399</v>
       </c>
       <c r="F15" t="n">
-        <v>8.18927</v>
+        <v>1.89462</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Wrapped Bitcoin</t>
+          <t>Wrapped stETH</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>wbtc</t>
+          <t>wsteth</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>98638</v>
+        <v>4009.34</v>
       </c>
       <c r="D16" t="n">
-        <v>14408704518</v>
+        <v>14436037107</v>
       </c>
       <c r="E16" t="n">
-        <v>826177901</v>
+        <v>168667300</v>
       </c>
       <c r="F16" t="n">
-        <v>1.6381</v>
+        <v>8.228009999999999</v>
       </c>
     </row>
     <row r="17">
@@ -839,16 +839,16 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5.52</v>
+        <v>5.54</v>
       </c>
       <c r="D17" t="n">
-        <v>14069277184</v>
+        <v>14095228925</v>
       </c>
       <c r="E17" t="n">
-        <v>625981057</v>
+        <v>589338135</v>
       </c>
       <c r="F17" t="n">
-        <v>1.96154</v>
+        <v>1.6983</v>
       </c>
     </row>
     <row r="18">
@@ -863,16 +863,16 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3.59</v>
+        <v>3.57</v>
       </c>
       <c r="D18" t="n">
-        <v>10230076114</v>
+        <v>10161865196</v>
       </c>
       <c r="E18" t="n">
-        <v>2195757402</v>
+        <v>2192651552</v>
       </c>
       <c r="F18" t="n">
-        <v>0.85599</v>
+        <v>1.19188</v>
       </c>
     </row>
     <row r="19">
@@ -887,16 +887,16 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>493.97</v>
+        <v>494.43</v>
       </c>
       <c r="D19" t="n">
-        <v>9775691671</v>
+        <v>9785549093</v>
       </c>
       <c r="E19" t="n">
-        <v>1709315082</v>
+        <v>1561011757</v>
       </c>
       <c r="F19" t="n">
-        <v>-6.39473</v>
+        <v>-6.5633</v>
       </c>
     </row>
     <row r="20">
@@ -911,16 +911,16 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3365.9</v>
+        <v>3384.32</v>
       </c>
       <c r="D20" t="n">
-        <v>9644552154</v>
+        <v>9716546060</v>
       </c>
       <c r="E20" t="n">
-        <v>1442232704</v>
+        <v>2170242355</v>
       </c>
       <c r="F20" t="n">
-        <v>8.026949999999999</v>
+        <v>8.236000000000001</v>
       </c>
     </row>
     <row r="21">
@@ -935,16 +935,16 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>15.27</v>
+        <v>15.33</v>
       </c>
       <c r="D21" t="n">
-        <v>9572585986</v>
+        <v>9607367121</v>
       </c>
       <c r="E21" t="n">
-        <v>1260125079</v>
+        <v>1297087105</v>
       </c>
       <c r="F21" t="n">
-        <v>4.8129</v>
+        <v>5.29034</v>
       </c>
     </row>
     <row r="22">
@@ -959,16 +959,16 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.131e-05</v>
+        <v>2.123e-05</v>
       </c>
       <c r="D22" t="n">
-        <v>8965828127</v>
+        <v>8933069598</v>
       </c>
       <c r="E22" t="n">
-        <v>6726966462</v>
+        <v>6736025750</v>
       </c>
       <c r="F22" t="n">
-        <v>9.410690000000001</v>
+        <v>9.71106</v>
       </c>
     </row>
     <row r="23">
@@ -983,16 +983,16 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>6.21</v>
+        <v>6.17</v>
       </c>
       <c r="D23" t="n">
-        <v>8949858104</v>
+        <v>8902126078</v>
       </c>
       <c r="E23" t="n">
-        <v>844734603</v>
+        <v>842741330</v>
       </c>
       <c r="F23" t="n">
-        <v>9.40584</v>
+        <v>8.33896</v>
       </c>
     </row>
     <row r="24">
@@ -1007,16 +1007,16 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.286915</v>
+        <v>0.277936</v>
       </c>
       <c r="D24" t="n">
-        <v>8617828912</v>
+        <v>8336084131</v>
       </c>
       <c r="E24" t="n">
-        <v>2346286480</v>
+        <v>2313903890</v>
       </c>
       <c r="F24" t="n">
-        <v>20.77031</v>
+        <v>17.49732</v>
       </c>
     </row>
     <row r="25">
@@ -1034,13 +1034,13 @@
         <v>8.800000000000001</v>
       </c>
       <c r="D25" t="n">
-        <v>8133488447</v>
+        <v>8123192116</v>
       </c>
       <c r="E25" t="n">
-        <v>3391395</v>
+        <v>3377597</v>
       </c>
       <c r="F25" t="n">
-        <v>3.53993</v>
+        <v>3.44216</v>
       </c>
     </row>
     <row r="26">
@@ -1055,16 +1055,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>5.76</v>
+        <v>5.72</v>
       </c>
       <c r="D26" t="n">
-        <v>7015382282</v>
+        <v>6963745894</v>
       </c>
       <c r="E26" t="n">
-        <v>1003512868</v>
+        <v>1017283186</v>
       </c>
       <c r="F26" t="n">
-        <v>4.87787</v>
+        <v>4.72805</v>
       </c>
     </row>
     <row r="27">
@@ -1079,16 +1079,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>90.18000000000001</v>
+        <v>90.11</v>
       </c>
       <c r="D27" t="n">
-        <v>6783548458</v>
+        <v>6778231611</v>
       </c>
       <c r="E27" t="n">
-        <v>1315864262</v>
+        <v>1218930844</v>
       </c>
       <c r="F27" t="n">
-        <v>1.30091</v>
+        <v>0.01314</v>
       </c>
     </row>
     <row r="28">
@@ -1103,16 +1103,16 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>12.02</v>
+        <v>11.98</v>
       </c>
       <c r="D28" t="n">
-        <v>6422121172</v>
+        <v>6388824576</v>
       </c>
       <c r="E28" t="n">
-        <v>848170177</v>
+        <v>838482957</v>
       </c>
       <c r="F28" t="n">
-        <v>3.68462</v>
+        <v>2.92228</v>
       </c>
     </row>
     <row r="29">
@@ -1127,16 +1127,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3546.31</v>
+        <v>3563.48</v>
       </c>
       <c r="D29" t="n">
-        <v>6169611515</v>
+        <v>6200422543</v>
       </c>
       <c r="E29" t="n">
-        <v>103651261</v>
+        <v>102675119</v>
       </c>
       <c r="F29" t="n">
-        <v>8.18763</v>
+        <v>8.2776</v>
       </c>
     </row>
     <row r="30">
@@ -1151,40 +1151,40 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9.32</v>
+        <v>9.34</v>
       </c>
       <c r="D30" t="n">
-        <v>5595254907</v>
+        <v>5604871536</v>
       </c>
       <c r="E30" t="n">
-        <v>872429790</v>
+        <v>876647483</v>
       </c>
       <c r="F30" t="n">
-        <v>5.52257</v>
+        <v>5.35269</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Hedera</t>
+          <t>Cronos</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>hbar</t>
+          <t>cro</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.138422</v>
+        <v>0.193879</v>
       </c>
       <c r="D31" t="n">
-        <v>5288274559</v>
+        <v>5279008976</v>
       </c>
       <c r="E31" t="n">
-        <v>964046702</v>
+        <v>164256979</v>
       </c>
       <c r="F31" t="n">
-        <v>10.79753</v>
+        <v>10.99994</v>
       </c>
     </row>
     <row r="32">
@@ -1199,40 +1199,40 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.9990520000000001</v>
+        <v>1.002</v>
       </c>
       <c r="D32" t="n">
-        <v>5226406988</v>
+        <v>5239351258</v>
       </c>
       <c r="E32" t="n">
-        <v>16006065</v>
+        <v>15847478</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.36705</v>
+        <v>0.33458</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Cronos</t>
+          <t>Hedera</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>cro</t>
+          <t>hbar</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.187995</v>
+        <v>0.131422</v>
       </c>
       <c r="D33" t="n">
-        <v>5141784943</v>
+        <v>5020172091</v>
       </c>
       <c r="E33" t="n">
-        <v>150634106</v>
+        <v>949771935</v>
       </c>
       <c r="F33" t="n">
-        <v>7.82868</v>
+        <v>4.64373</v>
       </c>
     </row>
     <row r="34">
@@ -1247,16 +1247,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9.6</v>
+        <v>9.59</v>
       </c>
       <c r="D34" t="n">
-        <v>4555261310</v>
+        <v>4550996907</v>
       </c>
       <c r="E34" t="n">
-        <v>273488349</v>
+        <v>273633020</v>
       </c>
       <c r="F34" t="n">
-        <v>6.60921</v>
+        <v>6.46952</v>
       </c>
     </row>
     <row r="35">
@@ -1271,16 +1271,16 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>27.94</v>
+        <v>27.87</v>
       </c>
       <c r="D35" t="n">
-        <v>4180801808</v>
+        <v>4170359427</v>
       </c>
       <c r="E35" t="n">
-        <v>861244532</v>
+        <v>813865857</v>
       </c>
       <c r="F35" t="n">
-        <v>4.70517</v>
+        <v>4.22164</v>
       </c>
     </row>
     <row r="36">
@@ -1295,16 +1295,16 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>5.242e-05</v>
+        <v>5.139e-05</v>
       </c>
       <c r="D36" t="n">
-        <v>3950095141</v>
+        <v>3864186173</v>
       </c>
       <c r="E36" t="n">
-        <v>1601466165</v>
+        <v>1560587657</v>
       </c>
       <c r="F36" t="n">
-        <v>-0.10235</v>
+        <v>-2.60599</v>
       </c>
     </row>
     <row r="37">
@@ -1319,16 +1319,16 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.151879</v>
+        <v>0.151656</v>
       </c>
       <c r="D37" t="n">
-        <v>3832713780</v>
+        <v>3829739860</v>
       </c>
       <c r="E37" t="n">
-        <v>150125959</v>
+        <v>148823784</v>
       </c>
       <c r="F37" t="n">
-        <v>0.45116</v>
+        <v>-0.18715</v>
       </c>
     </row>
     <row r="38">
@@ -1343,40 +1343,40 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>7.34</v>
+        <v>7.36</v>
       </c>
       <c r="D38" t="n">
-        <v>3801653465</v>
+        <v>3813961780</v>
       </c>
       <c r="E38" t="n">
-        <v>429954829</v>
+        <v>415629878</v>
       </c>
       <c r="F38" t="n">
-        <v>0.74086</v>
+        <v>0.47449</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>POL (ex-MATIC)</t>
+          <t>Ethena USDe</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>pol</t>
+          <t>usde</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.465237</v>
+        <v>1.003</v>
       </c>
       <c r="D39" t="n">
-        <v>3705435184</v>
+        <v>3698429840</v>
       </c>
       <c r="E39" t="n">
-        <v>501118230</v>
+        <v>241142883</v>
       </c>
       <c r="F39" t="n">
-        <v>6.34705</v>
+        <v>0.17877</v>
       </c>
     </row>
     <row r="40">
@@ -1391,40 +1391,40 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>500.21</v>
+        <v>500.01</v>
       </c>
       <c r="D40" t="n">
-        <v>3696581786</v>
+        <v>3692800394</v>
       </c>
       <c r="E40" t="n">
-        <v>280047488</v>
+        <v>271819542</v>
       </c>
       <c r="F40" t="n">
-        <v>3.58771</v>
+        <v>3.16576</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Ethena USDe</t>
+          <t>POL (ex-MATIC)</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>usde</t>
+          <t>pol</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1.002</v>
+        <v>0.462898</v>
       </c>
       <c r="D41" t="n">
-        <v>3688254516</v>
+        <v>3692042473</v>
       </c>
       <c r="E41" t="n">
-        <v>222230206</v>
+        <v>499939163</v>
       </c>
       <c r="F41" t="n">
-        <v>-0.18498</v>
+        <v>4.91374</v>
       </c>
     </row>
     <row r="42">
@@ -1439,112 +1439,112 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>24.78</v>
+        <v>24.85</v>
       </c>
       <c r="D42" t="n">
-        <v>3570818581</v>
+        <v>3580492826</v>
       </c>
       <c r="E42" t="n">
-        <v>32982943</v>
+        <v>31973928</v>
       </c>
       <c r="F42" t="n">
-        <v>2.58192</v>
+        <v>3.06658</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Dai</t>
+          <t>MANTRA</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>dai</t>
+          <t>om</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.999769</v>
+        <v>3.84</v>
       </c>
       <c r="D43" t="n">
-        <v>3441159133</v>
+        <v>3472194114</v>
       </c>
       <c r="E43" t="n">
-        <v>151317872</v>
+        <v>312099495</v>
       </c>
       <c r="F43" t="n">
-        <v>-0.09085</v>
+        <v>7.16845</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>MANTRA</t>
+          <t>Dai</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>om</t>
+          <t>dai</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>3.82</v>
+        <v>1.001</v>
       </c>
       <c r="D44" t="n">
-        <v>3439796552</v>
+        <v>3446986754</v>
       </c>
       <c r="E44" t="n">
-        <v>304975628</v>
+        <v>156204789</v>
       </c>
       <c r="F44" t="n">
-        <v>5.48871</v>
+        <v>0.207</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>dogwifhat</t>
+          <t>Artificial Superintelligence Alliance</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>wif</t>
+          <t>fet</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3.34</v>
+        <v>1.27</v>
       </c>
       <c r="D45" t="n">
-        <v>3349732168</v>
+        <v>3325654533</v>
       </c>
       <c r="E45" t="n">
-        <v>1291008898</v>
+        <v>474441754</v>
       </c>
       <c r="F45" t="n">
-        <v>5.12188</v>
+        <v>3.78244</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Artificial Superintelligence Alliance</t>
+          <t>dogwifhat</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>fet</t>
+          <t>wif</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1.28</v>
+        <v>3.3</v>
       </c>
       <c r="D46" t="n">
-        <v>3329445059</v>
+        <v>3301476632</v>
       </c>
       <c r="E46" t="n">
-        <v>482295249</v>
+        <v>1297112574</v>
       </c>
       <c r="F46" t="n">
-        <v>3.22596</v>
+        <v>3.69762</v>
       </c>
     </row>
     <row r="47">
@@ -1559,16 +1559,16 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.783631</v>
+        <v>0.788235</v>
       </c>
       <c r="D47" t="n">
-        <v>3213465867</v>
+        <v>3232107332</v>
       </c>
       <c r="E47" t="n">
-        <v>1670862527</v>
+        <v>1658745968</v>
       </c>
       <c r="F47" t="n">
-        <v>13.38334</v>
+        <v>12.31639</v>
       </c>
     </row>
     <row r="48">
@@ -1583,16 +1583,16 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>160.73</v>
+        <v>161.13</v>
       </c>
       <c r="D48" t="n">
-        <v>2965520995</v>
+        <v>2972306515</v>
       </c>
       <c r="E48" t="n">
-        <v>85739377</v>
+        <v>85859312</v>
       </c>
       <c r="F48" t="n">
-        <v>-0.53269</v>
+        <v>-0.19214</v>
       </c>
     </row>
     <row r="49">
@@ -1607,64 +1607,64 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1.96</v>
+        <v>1.94</v>
       </c>
       <c r="D49" t="n">
-        <v>2935957058</v>
+        <v>2919785176</v>
       </c>
       <c r="E49" t="n">
-        <v>349512301</v>
+        <v>344355492</v>
       </c>
       <c r="F49" t="n">
-        <v>1.94279</v>
+        <v>1.26665</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Filecoin</t>
+          <t>Mantle</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>fil</t>
+          <t>mnt</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>4.67</v>
+        <v>0.8379760000000001</v>
       </c>
       <c r="D50" t="n">
-        <v>2807537544</v>
+        <v>2823626589</v>
       </c>
       <c r="E50" t="n">
-        <v>567842261</v>
+        <v>188849835</v>
       </c>
       <c r="F50" t="n">
-        <v>5.23522</v>
+        <v>14.61509</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Mantle</t>
+          <t>Filecoin</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>mnt</t>
+          <t>fil</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.832329</v>
+        <v>4.67</v>
       </c>
       <c r="D51" t="n">
-        <v>2803686073</v>
+        <v>2807056498</v>
       </c>
       <c r="E51" t="n">
-        <v>186631406</v>
+        <v>532166566</v>
       </c>
       <c r="F51" t="n">
-        <v>13.99973</v>
+        <v>4.09637</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1955065374675</v>
+        <v>1964885477649</v>
       </c>
     </row>
     <row r="3">
@@ -1715,7 +1715,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>405569114425</v>
+        <v>407330066375</v>
       </c>
     </row>
     <row r="4">
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>130803059570</v>
+        <v>130971083766</v>
       </c>
     </row>
     <row r="5">
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>122966673076</v>
+        <v>123363846725</v>
       </c>
     </row>
     <row r="6">
@@ -1745,7 +1745,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>91896601685</v>
+        <v>91918590252</v>
       </c>
     </row>
   </sheetData>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$4348.79</t>
+          <t>$4364.05</t>
         </is>
       </c>
     </row>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>XRP (26.17%)</t>
+          <t>XRP (24.35%)</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bitcoin Cash (-6.39%)</t>
+          <t>Bitcoin Cash (-6.56%)</t>
         </is>
       </c>
     </row>

</xml_diff>